<commit_message>
Braidwood and prairie island
</commit_message>
<xml_diff>
--- a/use_cases/IES_Feb23/run/results.xlsx
+++ b/use_cases/IES_Feb23/run/results.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/IES_Feb23/run/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D459864-98CE-BB49-8990-2486F0556A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAB2220-273D-B543-961D-FF4C8D866B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
+    <workbookView xWindow="15740" yWindow="3240" windowWidth="21000" windowHeight="17440" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Location</t>
   </si>
@@ -63,6 +63,21 @@
   </si>
   <si>
     <t>Cooper</t>
+  </si>
+  <si>
+    <t>Std baseline NPV</t>
+  </si>
+  <si>
+    <t>Std opt NPV</t>
+  </si>
+  <si>
+    <t>Std baseline NPV frac</t>
+  </si>
+  <si>
+    <t>Std opt NPV frac</t>
+  </si>
+  <si>
+    <t>Std delta NPV (%)</t>
   </si>
 </sst>
 </file>
@@ -118,7 +133,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -406,7 +421,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -414,19 +429,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FE355D-8072-1247-9790-841EBA440D66}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.1640625" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -434,35 +453,124 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
       </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
+      <c r="B2">
+        <v>2102483898.8800001</v>
+      </c>
+      <c r="C2">
+        <v>10442175</v>
+      </c>
+      <c r="D2">
+        <f>C2/B2</f>
+        <v>4.9665897586956935E-3</v>
+      </c>
+      <c r="E2">
+        <v>3932705714.9400001</v>
+      </c>
+      <c r="F2">
+        <v>46329.74</v>
+      </c>
+      <c r="G2">
+        <f>F2/E2</f>
+        <v>1.1780627221609139E-5</v>
+      </c>
+      <c r="H2">
+        <f>E2-B2</f>
+        <v>1830221816.0599999</v>
+      </c>
+      <c r="I2">
+        <f>100*SQRT(POWER(G2,2)+POWER(D2,2))</f>
+        <v>0.49666037303532362</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="B3">
+        <v>262560457.34999999</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f>C3/B3</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1534342635.98</v>
+      </c>
+      <c r="F3">
+        <v>21276.57</v>
+      </c>
+      <c r="G3">
+        <f>F3/E3</f>
+        <v>1.3866896155440822E-5</v>
+      </c>
+      <c r="H3">
+        <f>E3-B3</f>
+        <v>1271782178.6300001</v>
+      </c>
+      <c r="I3">
+        <f>100*SQRT(POWER(G3,2)+POWER(D3,2))</f>
+        <v>1.3866896155440823E-3</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
+      <c r="B4">
+        <v>1765764570.5999999</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
+      <c r="B5">
+        <v>2861165724.4899998</v>
+      </c>
+      <c r="C5">
+        <v>75472956.379999995</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
+      </c>
+      <c r="B6">
+        <v>1080996406.4100001</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update graph, add capex costs
</commit_message>
<xml_diff>
--- a/use_cases/IES_Feb23/run/results.xlsx
+++ b/use_cases/IES_Feb23/run/results.xlsx
@@ -8,13 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/IES_Feb23/run/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAEB4EB2-B565-064A-8A2F-1206679CA5AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB81D7A-FA25-3F42-A39D-B87B9C434A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="500" windowWidth="29860" windowHeight="17000" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="cases" sheetId="1" r:id="rId1"/>
+    <sheet name="braidwood_SA" sheetId="2" r:id="rId2"/>
+    <sheet name="covid" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v2.0" hidden="1">cases!$A$3:$A$7</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">cases!$O$2</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">cases!$O$3:$O$7</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">cases!$Q$2</definedName>
+    <definedName name="_xlchart.v2.4" hidden="1">cases!$Q$3:$Q$7</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
   <si>
     <t>Location</t>
   </si>
@@ -105,14 +114,138 @@
   </si>
   <si>
     <t>Houston</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>Mean NPV</t>
+  </si>
+  <si>
+    <t>Std NPV</t>
+  </si>
+  <si>
+    <t>Std NPv (%)</t>
+  </si>
+  <si>
+    <t>Std delta NPV</t>
+  </si>
+  <si>
+    <t>Baseline electricity</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>synfuel low</t>
+  </si>
+  <si>
+    <t>synfuel high</t>
+  </si>
+  <si>
+    <t>capex low</t>
+  </si>
+  <si>
+    <t>capex high</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>no covid baseline</t>
+  </si>
+  <si>
+    <t>no covid</t>
+  </si>
+  <si>
+    <t>CAPEX (M$)</t>
+  </si>
+  <si>
+    <t>co2 med</t>
+  </si>
+  <si>
+    <t>co2 high</t>
+  </si>
+  <si>
+    <t>co2_shipping</t>
+  </si>
+  <si>
+    <t>diesel_sales</t>
+  </si>
+  <si>
+    <t>e_sales</t>
+  </si>
+  <si>
+    <t>elec_cap_market</t>
+  </si>
+  <si>
+    <t>ft_capex</t>
+  </si>
+  <si>
+    <t>ft_fom</t>
+  </si>
+  <si>
+    <t>ft_vom</t>
+  </si>
+  <si>
+    <t>h2_ptc</t>
+  </si>
+  <si>
+    <t>h2_storage_capex</t>
+  </si>
+  <si>
+    <t>htse_capex</t>
+  </si>
+  <si>
+    <t>htse_elec_cap_market</t>
+  </si>
+  <si>
+    <t>htse_fom</t>
+  </si>
+  <si>
+    <t>htse_vom</t>
+  </si>
+  <si>
+    <t>jet_fuel_sales</t>
+  </si>
+  <si>
+    <t>naphtha_sales</t>
+  </si>
+  <si>
+    <t>plant</t>
+  </si>
+  <si>
+    <t>taxes</t>
+  </si>
+  <si>
+    <t>braidwood</t>
+  </si>
+  <si>
+    <t>cooper</t>
+  </si>
+  <si>
+    <t>prairie_island</t>
+  </si>
+  <si>
+    <t>stp</t>
+  </si>
+  <si>
+    <t>davis_besse</t>
+  </si>
+  <si>
+    <t>OM (M$)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -263,11 +396,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -279,6 +413,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -289,9 +424,10 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -332,7 +468,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$2</c:f>
+              <c:f>cases!$O$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -343,14 +479,10 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent6">
-                <a:alpha val="91000"/>
-              </a:schemeClr>
+              <a:schemeClr val="accent6"/>
             </a:solidFill>
             <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
@@ -370,7 +502,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -419,48 +551,48 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$P$3:$P$7</c:f>
+                <c:f>cases!$P$3:$P$7</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>10.442195970338283</c:v>
+                    <c:v>10442195.970338283</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.800790423E-2</c:v>
+                    <c:v>18007.90423</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.4532582657600002E-3</c:v>
+                    <c:v>2453.2582657600001</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5.80901291453E-3</c:v>
+                    <c:v>5809.0129145299998</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>80.58162171734773</c:v>
+                    <c:v>80581621.717347726</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$P$3:$P$7</c:f>
+                <c:f>cases!$P$3:$P$7</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>10.442195970338283</c:v>
+                    <c:v>10442195.970338283</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>1.800790423E-2</c:v>
+                    <c:v>18007.90423</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.4532582657600002E-3</c:v>
+                    <c:v>2453.2582657600001</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5.80901291453E-3</c:v>
+                    <c:v>5809.0129145299998</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>80.58162171734773</c:v>
+                    <c:v>80581621.717347726</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -481,7 +613,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$7</c:f>
+              <c:f>cases!$A$3:$A$7</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -504,31 +636,108 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$3:$O$7</c:f>
+              <c:f>cases!$O$3:$O$7</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1487.1831238399998</c:v>
+                  <c:v>1487183123.8399997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1208.3701209200001</c:v>
+                  <c:v>1208370120.9200001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1356.0625250100002</c:v>
+                  <c:v>1356062525.0100002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1243.05909213</c:v>
+                  <c:v>1243059092.1299999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1750.005306</c:v>
+                  <c:v>1750005306</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EFCB-AF41-82B8-1783BEC85907}"/>
+              <c16:uniqueId val="{00000000-4686-1A4B-B59E-23C2982A3A10}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>cases!$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CAPEX (M$)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>cases!$A$3:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Braidwood</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Prairie Island</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Davis Besse</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Cooper</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>South Texas Project</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>cases!$Q$3:$Q$7</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>320071789.37109995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>178897818.0905</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>262728958.7272</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>247337409.04210001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>204617209.60839999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4686-1A4B-B59E-23C2982A3A10}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -542,11 +751,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="1824573871"/>
-        <c:axId val="1824575519"/>
+        <c:axId val="1218972784"/>
+        <c:axId val="1218974432"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1824573871"/>
+        <c:axId val="1218972784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -574,7 +783,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -589,7 +798,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1824575519"/>
+        <c:crossAx val="1218974432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -597,7 +806,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1824575519"/>
+        <c:axId val="1218974432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -617,9 +826,51 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1218972784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="billions"/>
+          <c:dispUnitsLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
               <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
@@ -636,77 +887,11 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>Δ(NPV) M$(2020)</a:t>
-                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1824573871"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:majorUnit val="500"/>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -716,6 +901,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -754,13 +970,10 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -1300,23 +1513,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>1536700</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>463550</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>787400</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>914400</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4DC97625-FE56-3895-A849-0DA1CCA8A7D2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D9C13AF-5416-55C3-3682-46E9E1BCA5D9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1634,10 +1847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FE355D-8072-1247-9790-841EBA440D66}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:AJ8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AA10" sqref="AA10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1656,18 +1869,22 @@
     <col min="14" max="14" width="12.6640625" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="20.6640625" customWidth="1"/>
     <col min="16" max="16" width="23.33203125" customWidth="1"/>
+    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="14"/>
     </row>
-    <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1716,8 +1933,65 @@
       <c r="P2" t="s">
         <v>19</v>
       </c>
+      <c r="Q2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" t="s">
+        <v>63</v>
+      </c>
+      <c r="T2" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V2" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" t="s">
+        <v>44</v>
+      </c>
+      <c r="X2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
@@ -1768,15 +2042,74 @@
         <v>10442195.970338283</v>
       </c>
       <c r="O3" s="1">
-        <f>L3/1000000</f>
-        <v>1487.1831238399998</v>
+        <f>L3</f>
+        <v>1487183123.8399997</v>
       </c>
       <c r="P3" s="1">
-        <f>N3/1000000</f>
-        <v>10.442195970338283</v>
+        <f>N3</f>
+        <v>10442195.970338283</v>
+      </c>
+      <c r="Q3" s="1">
+        <f>ABS(X3+AC3+AB3)</f>
+        <v>320071789.37109995</v>
+      </c>
+      <c r="R3" s="1">
+        <f>ABS(T3+Y3+Z3+AE3+AF3)</f>
+        <v>1374267486.8539767</v>
+      </c>
+      <c r="T3">
+        <v>-1.1539766655999999</v>
+      </c>
+      <c r="U3">
+        <v>784993059.20999897</v>
+      </c>
+      <c r="V3">
+        <v>12996245.300499899</v>
+      </c>
+      <c r="W3">
+        <v>-5860214.3420000002</v>
+      </c>
+      <c r="X3">
+        <v>-299795112.39999998</v>
+      </c>
+      <c r="Y3">
+        <v>-305989671.60000002</v>
+      </c>
+      <c r="Z3">
+        <v>-107571298.56</v>
+      </c>
+      <c r="AA3">
+        <v>5462903274.6999998</v>
+      </c>
+      <c r="AB3">
+        <v>-19576500</v>
+      </c>
+      <c r="AC3">
+        <v>-700176.97109999997</v>
+      </c>
+      <c r="AD3">
+        <v>-462130996.799999</v>
+      </c>
+      <c r="AE3">
+        <v>-501614080</v>
+      </c>
+      <c r="AF3">
+        <v>-459092435.54000002</v>
+      </c>
+      <c r="AG3">
+        <v>1737621649.3599999</v>
+      </c>
+      <c r="AH3">
+        <v>676618806.59999895</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ3">
+        <v>-2923135525.0834198</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
@@ -1827,15 +2160,74 @@
         <v>18007.90423</v>
       </c>
       <c r="O4" s="1">
-        <f t="shared" ref="O4:O8" si="5">L4/1000000</f>
-        <v>1208.3701209200001</v>
+        <f t="shared" ref="O4:O8" si="5">L4</f>
+        <v>1208370120.9200001</v>
       </c>
       <c r="P4" s="1">
-        <f t="shared" ref="P4:P8" si="6">N4/1000000</f>
-        <v>1.800790423E-2</v>
+        <f t="shared" ref="P4:P8" si="6">N4</f>
+        <v>18007.90423</v>
+      </c>
+      <c r="Q4" s="1">
+        <f t="shared" ref="Q4:Q8" si="7">ABS(X4+AC4+AB4)</f>
+        <v>178897818.0905</v>
+      </c>
+      <c r="R4" s="1">
+        <f t="shared" ref="R4:R8" si="8">ABS(T4+Y4+Z4+AE4+AF4)</f>
+        <v>836787255.16524041</v>
+      </c>
+      <c r="T4">
+        <v>-1.4202404037999901</v>
+      </c>
+      <c r="U4">
+        <v>394833167.79000002</v>
+      </c>
+      <c r="V4">
+        <v>7578786.5296510002</v>
+      </c>
+      <c r="W4">
+        <v>-5931802.1880000001</v>
+      </c>
+      <c r="X4">
+        <v>-175484359.5</v>
+      </c>
+      <c r="Y4">
+        <v>-309727613.60000002</v>
+      </c>
+      <c r="Z4">
+        <v>-108885379.76000001</v>
+      </c>
+      <c r="AA4">
+        <v>2385392346.99999</v>
+      </c>
+      <c r="AB4">
+        <v>-2689000</v>
+      </c>
+      <c r="AC4">
+        <v>-724458.59050000005</v>
+      </c>
+      <c r="AD4">
+        <v>-201840517.40000001</v>
+      </c>
+      <c r="AE4">
+        <v>-219085164.40000001</v>
+      </c>
+      <c r="AF4">
+        <v>-199089095.98500001</v>
+      </c>
+      <c r="AG4">
+        <v>720097787.05999899</v>
+      </c>
+      <c r="AH4">
+        <v>387046227.23000002</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ4">
+        <v>-1200560344.4958999</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>6</v>
       </c>
@@ -1887,14 +2279,73 @@
       </c>
       <c r="O5" s="1">
         <f t="shared" si="5"/>
-        <v>1356.0625250100002</v>
+        <v>1356062525.0100002</v>
       </c>
       <c r="P5" s="1">
         <f t="shared" si="6"/>
-        <v>2.4532582657600002E-3</v>
+        <v>2453.2582657600001</v>
+      </c>
+      <c r="Q5" s="1">
+        <f t="shared" si="7"/>
+        <v>262728958.7272</v>
+      </c>
+      <c r="R5" s="1">
+        <f t="shared" si="8"/>
+        <v>1270553097.7362475</v>
+      </c>
+      <c r="T5">
+        <v>-1.5862495952</v>
+      </c>
+      <c r="U5">
+        <v>764161074.72999895</v>
+      </c>
+      <c r="V5">
+        <v>1128230.1472700001</v>
+      </c>
+      <c r="W5">
+        <v>-6576092.7999999896</v>
+      </c>
+      <c r="X5">
+        <v>-249984024</v>
+      </c>
+      <c r="Y5">
+        <v>-343369091.799999</v>
+      </c>
+      <c r="Z5">
+        <v>-120712110.59999999</v>
+      </c>
+      <c r="AA5">
+        <v>4585937499.5</v>
+      </c>
+      <c r="AB5">
+        <v>-12037500</v>
+      </c>
+      <c r="AC5">
+        <v>-707434.72719999996</v>
+      </c>
+      <c r="AD5">
+        <v>-387945340.19999897</v>
+      </c>
+      <c r="AE5">
+        <v>-421090223.99999899</v>
+      </c>
+      <c r="AF5">
+        <v>-385381669.75</v>
+      </c>
+      <c r="AG5">
+        <v>1484027150.75</v>
+      </c>
+      <c r="AH5">
+        <v>806284329.05999994</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ5">
+        <v>-2591907699.1138201</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
@@ -1946,14 +2397,73 @@
       </c>
       <c r="O6" s="1">
         <f t="shared" si="5"/>
-        <v>1243.05909213</v>
+        <v>1243059092.1299999</v>
       </c>
       <c r="P6" s="1">
         <f t="shared" si="6"/>
-        <v>5.80901291453E-3</v>
+        <v>5809.0129145299998</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" si="7"/>
+        <v>247337409.04210001</v>
+      </c>
+      <c r="R6" s="1">
+        <f t="shared" si="8"/>
+        <v>1065590666.9014182</v>
+      </c>
+      <c r="T6">
+        <v>-1.3314181646000001</v>
+      </c>
+      <c r="U6">
+        <v>622093023.10000002</v>
+      </c>
+      <c r="V6">
+        <v>829231.42429</v>
+      </c>
+      <c r="W6">
+        <v>-6062491.6279999902</v>
+      </c>
+      <c r="X6">
+        <v>-227097690.40000001</v>
+      </c>
+      <c r="Y6">
+        <v>-316551531</v>
+      </c>
+      <c r="Z6">
+        <v>-111284341.95999999</v>
+      </c>
+      <c r="AA6">
+        <v>3626579180.9000001</v>
+      </c>
+      <c r="AB6">
+        <v>-19528000.02</v>
+      </c>
+      <c r="AC6">
+        <v>-711718.62210000004</v>
+      </c>
+      <c r="AD6">
+        <v>-306786488.99999899</v>
+      </c>
+      <c r="AE6">
+        <v>-332997404.39999998</v>
+      </c>
+      <c r="AF6">
+        <v>-304757388.20999998</v>
+      </c>
+      <c r="AG6">
+        <v>1197993900.8099999</v>
+      </c>
+      <c r="AH6">
+        <v>408440961.57999998</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ6">
+        <v>-1906103742.70277</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>17</v>
       </c>
@@ -2005,14 +2515,73 @@
       </c>
       <c r="O7" s="1">
         <f t="shared" si="5"/>
-        <v>1750.005306</v>
+        <v>1750005306</v>
       </c>
       <c r="P7" s="1">
         <f t="shared" si="6"/>
-        <v>80.58162171734773</v>
+        <v>80581621.717347726</v>
+      </c>
+      <c r="Q7" s="1">
+        <f t="shared" si="7"/>
+        <v>204617209.60839999</v>
+      </c>
+      <c r="R7" s="1">
+        <f t="shared" si="8"/>
+        <v>1436174702.5125432</v>
+      </c>
+      <c r="T7">
+        <v>-2.326544218</v>
+      </c>
+      <c r="U7">
+        <v>391253658.669999</v>
+      </c>
+      <c r="V7">
+        <v>3834753586.0289998</v>
+      </c>
+      <c r="W7">
+        <v>-6576092.7999999896</v>
+      </c>
+      <c r="X7">
+        <v>-153587835</v>
+      </c>
+      <c r="Y7">
+        <v>-343369091.799999</v>
+      </c>
+      <c r="Z7">
+        <v>-120712110.59999999</v>
+      </c>
+      <c r="AA7">
+        <v>6507684200.6000004</v>
+      </c>
+      <c r="AB7">
+        <v>-50330880.950000003</v>
+      </c>
+      <c r="AC7">
+        <v>-698493.65839999996</v>
+      </c>
+      <c r="AD7">
+        <v>-558305865.19999897</v>
+      </c>
+      <c r="AE7">
+        <v>-606005840</v>
+      </c>
+      <c r="AF7">
+        <v>-366087657.78600001</v>
+      </c>
+      <c r="AG7">
+        <v>720583663.12</v>
+      </c>
+      <c r="AH7">
+        <v>223872134.73199999</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ7">
+        <v>-5001440731.5800505</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>22</v>
       </c>
@@ -2062,11 +2631,19 @@
       </c>
       <c r="O8" s="1">
         <f t="shared" si="5"/>
-        <v>1739.5652711100006</v>
+        <v>1739565271.1100006</v>
       </c>
       <c r="P8" s="1">
         <f t="shared" si="6"/>
-        <v>75.532251481066012</v>
+        <v>75532251.481066018</v>
+      </c>
+      <c r="Q8" s="1">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="R8" s="1">
+        <f t="shared" si="8"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2076,4 +2653,364 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBA1661-1357-8E4D-8878-EEFCBAD9628D}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>2102483898.8800001</v>
+      </c>
+      <c r="C2">
+        <v>10442175.4814</v>
+      </c>
+      <c r="D2" s="11">
+        <f>C2/B2</f>
+        <v>4.966589987662964E-3</v>
+      </c>
+      <c r="E2">
+        <f>B2-$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>SQRT(POWER($C$2,2)+POWER(C2,2))</f>
+        <v>14767466.186475683</v>
+      </c>
+      <c r="G2" s="11" t="e">
+        <f>F2/E2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
+        <v>3589667022.7199998</v>
+      </c>
+      <c r="C3">
+        <v>20927.310484099999</v>
+      </c>
+      <c r="D3" s="11">
+        <f t="shared" ref="D3:D7" si="0">C3/B3</f>
+        <v>5.8298751253654551E-6</v>
+      </c>
+      <c r="E3">
+        <f>B3-$B$2</f>
+        <v>1487183123.8399997</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F7" si="1">SQRT(POWER($C$2,2)+POWER(C3,2))</f>
+        <v>10442196.451737316</v>
+      </c>
+      <c r="G3" s="11">
+        <f>F3/E3</f>
+        <v>7.0214597545828206E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>3274713277.4400001</v>
+      </c>
+      <c r="C4">
+        <v>1511245.9402099999</v>
+      </c>
+      <c r="D4" s="11">
+        <f t="shared" si="0"/>
+        <v>4.6148954493854593E-4</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E7" si="2">B4-$B$2</f>
+        <v>1172229378.5599999</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="1"/>
+        <v>10550966.452233298</v>
+      </c>
+      <c r="G4" s="11">
+        <f t="shared" ref="G4:G7" si="3">F4/E4</f>
+        <v>9.0007695125286884E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5">
+        <v>3922539711.2800002</v>
+      </c>
+      <c r="C5">
+        <v>20794.873572600001</v>
+      </c>
+      <c r="D5" s="11">
+        <f t="shared" si="0"/>
+        <v>5.3013799994938064E-6</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>1820055812.4000001</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="1"/>
+        <v>10442196.187159013</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="3"/>
+        <v>5.7372944917494072E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <v>3619836618.1599998</v>
+      </c>
+      <c r="C6">
+        <v>560204.140839</v>
+      </c>
+      <c r="D6" s="11">
+        <f t="shared" si="0"/>
+        <v>1.5475950987085089E-4</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>1517352719.2799997</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="1"/>
+        <v>10457191.662380703</v>
+      </c>
+      <c r="G6" s="11">
+        <f t="shared" si="3"/>
+        <v>6.8917342220487492E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="11" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>-2102483898.8800001</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="1"/>
+        <v>10442175.4814</v>
+      </c>
+      <c r="G7" s="11">
+        <f t="shared" si="3"/>
+        <v>-4.966589987662964E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BBBBF4E-63B1-3B49-81EC-48E68EDAAD9B}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2">
+        <v>2102483898.8800001</v>
+      </c>
+      <c r="C2">
+        <v>10442175.4814</v>
+      </c>
+      <c r="D2" s="11">
+        <f>C2/B2</f>
+        <v>4.966589987662964E-3</v>
+      </c>
+      <c r="E2">
+        <f>B2-$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <f>SQRT(POWER(C2,2)+POWER($C$2,2))</f>
+        <v>14767466.186475683</v>
+      </c>
+      <c r="G2" s="11" t="e">
+        <f>F2/E2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3">
+        <v>3589667022.7199998</v>
+      </c>
+      <c r="C3">
+        <v>20927.310484099999</v>
+      </c>
+      <c r="D3" s="11">
+        <f t="shared" ref="D3:D5" si="0">C3/B3</f>
+        <v>5.8298751253654551E-6</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E5" si="1">B3-$B$2</f>
+        <v>1487183123.8399997</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F5" si="2">SQRT(POWER(C3,2)+POWER($C$2,2))</f>
+        <v>10442196.451737316</v>
+      </c>
+      <c r="G3" s="11">
+        <f t="shared" ref="G3:G5" si="3">F3/E3</f>
+        <v>7.0214597545828206E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4">
+        <v>2162947058</v>
+      </c>
+      <c r="C4">
+        <v>15334997.619999999</v>
+      </c>
+      <c r="D4" s="11">
+        <f t="shared" si="0"/>
+        <v>7.0898626775357711E-3</v>
+      </c>
+      <c r="E4">
+        <f>B4-$B$2</f>
+        <v>60463159.119999886</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>18552659.668892678</v>
+      </c>
+      <c r="G4" s="11">
+        <f t="shared" si="3"/>
+        <v>0.30684238036705341</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5">
+        <v>3311505178.27</v>
+      </c>
+      <c r="C5">
+        <v>4118428.9192300001</v>
+      </c>
+      <c r="D5" s="11">
+        <f t="shared" si="0"/>
+        <v>1.2436728005908039E-3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>1209021279.3899999</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="2"/>
+        <v>11224993.788287871</v>
+      </c>
+      <c r="G5" s="11">
+        <f t="shared" si="3"/>
+        <v>9.2843641213257496E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update results after co2 shipping costs update
</commit_message>
<xml_diff>
--- a/use_cases/IES_Feb23/run/results.xlsx
+++ b/use_cases/IES_Feb23/run/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/IES_Feb23/run/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB81D7A-FA25-3F42-A39D-B87B9C434A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3E188F-9F4B-EA40-8045-6F54FB5C7273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
   </bookViews>
@@ -17,13 +17,9 @@
     <sheet name="braidwood_SA" sheetId="2" r:id="rId2"/>
     <sheet name="covid" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v2.0" hidden="1">cases!$A$3:$A$7</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">cases!$O$2</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">cases!$O$3:$O$7</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">cases!$Q$2</definedName>
-    <definedName name="_xlchart.v2.4" hidden="1">cases!$Q$3:$Q$7</definedName>
-  </definedNames>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -45,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
   <si>
     <t>Location</t>
   </si>
@@ -237,17 +233,39 @@
   </si>
   <si>
     <t>OM (M$)</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Std low</t>
+  </si>
+  <si>
+    <t>Std high</t>
+  </si>
+  <si>
+    <t>Synfuel Price</t>
+  </si>
+  <si>
+    <t>CAPEX</t>
+  </si>
+  <si>
+    <t>CO2 Cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -258,6 +276,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -401,7 +426,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -423,6 +448,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -556,19 +583,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>10442195.970338283</c:v>
+                    <c:v>10791773.621722151</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>18007.90423</c:v>
+                    <c:v>112426.783738</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2453.2582657600001</c:v>
+                    <c:v>1136859.4810800001</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5809.0129145299998</c:v>
+                    <c:v>2014357.9649499999</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>80581621.717347726</c:v>
+                    <c:v>81217687.647704601</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -580,19 +607,19 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>10442195.970338283</c:v>
+                    <c:v>10791773.621722151</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>18007.90423</c:v>
+                    <c:v>112426.783738</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2453.2582657600001</c:v>
+                    <c:v>1136859.4810800001</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>5809.0129145299998</c:v>
+                    <c:v>2014357.9649499999</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>80581621.717347726</c:v>
+                    <c:v>81217687.647704601</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -641,19 +668,19 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1487183123.8399997</c:v>
+                  <c:v>988706502.11999989</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1208370120.9200001</c:v>
+                  <c:v>797305235.92999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1356062525.0100002</c:v>
+                  <c:v>748584278.82999992</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1243059092.1299999</c:v>
+                  <c:v>800336972.89999986</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1750005306</c:v>
+                  <c:v>886522516.21000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -969,6 +996,890 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13656364383023548"/>
+          <c:y val="0.20686157962845172"/>
+          <c:w val="0.73386719517203203"/>
+          <c:h val="0.71235847608185465"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>braidwood_SA!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Synfuel Price</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>[1]New_fin_param!$D$14:$D$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>13044061.337726347</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>14584955.770416418</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>14477794.612199999</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>[1]New_fin_param!$D$14:$D$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>13044061.337726347</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>14584955.770416418</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>14477794.612199999</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>braidwood_SA!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CO2 Cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>braidwood_SA!$B$12:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1172229378.5599999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1820055812.4000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3789-624C-893F-DC9282CA661B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>braidwood_SA!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CAPEX</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>[1]New_fin_param!$E$14:$E$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>14749672.60467495</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>14477794.612199999</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>[1]New_fin_param!$E$14:$E$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>14749672.60467495</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>14477794.612199999</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>braidwood_SA!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CO2 Cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>braidwood_SA!$B$13:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1517352719.2799997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1429864232.73</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3789-624C-893F-DC9282CA661B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>braidwood_SA!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CO2 Cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>braidwood_SA!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CO2 Cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>braidwood_SA!$B$14:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1175413563.48</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1066926071.1199999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3789-624C-893F-DC9282CA661B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="300"/>
+        <c:overlap val="100"/>
+        <c:axId val="1079498976"/>
+        <c:axId val="1079459696"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1079498976"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="22225" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1079459696"/>
+        <c:crossesAt val="1476746599.9999998"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1079459696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;?_);_(@_)" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1079498976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="billions"/>
+          <c:dispUnitsLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11876018574601252"/>
+          <c:y val="0.13282057494292504"/>
+          <c:w val="0.79406840298808801"/>
+          <c:h val="0.79854037180263715"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Low</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="wdDnDiag">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln w="31750">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>braidwood_SA!$A$12:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Synfuel Price</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CAPEX</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CO2 Cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>braidwood_SA!$B$12:$B$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1172229378.5599999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1517352719.2799997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1175413563.48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1F26-DF46-825B-52CEF0CBC6B4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>braidwood_SA!$C$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>High</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="28575">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>braidwood_SA!$A$12:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Synfuel Price</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>CAPEX</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>CO2 Cost</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>braidwood_SA!$C$12:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1820055812.4000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1429864232.73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1066926071.1199999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1F26-DF46-825B-52CEF0CBC6B4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:overlap val="100"/>
+        <c:axId val="414221104"/>
+        <c:axId val="1796024143"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="414221104"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1796024143"/>
+        <c:crossesAt val="1487183124.0000002"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1796024143"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="t"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="414221104"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="250000000"/>
+        <c:minorUnit val="100000000"/>
+        <c:dispUnits>
+          <c:builtInUnit val="billions"/>
+          <c:dispUnitsLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
@@ -1006,6 +1917,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1477,6 +2468,1016 @@
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1519,10 +3520,10 @@
       <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>914400</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1548,6 +3549,952 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A188611D-D3FF-6646-8ED0-8E1D8DE54A57}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B0287DE-5719-7713-E572-18F3E1BCA967}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.12018</cdr:x>
+      <cdr:y>0.05547</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.27543</cdr:x>
+      <cdr:y>0.1229</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26AA5548-A60A-D05C-0D51-011C1B561077}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1384300" y="266284"/>
+          <a:ext cx="1788310" cy="323704"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>[23, LMP, 65] $/MWe </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.11344</cdr:x>
+      <cdr:y>0.06514</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26AA5548-A60A-D05C-0D51-011C1B561077}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="0"/>
+          <a:ext cx="1354246" cy="343322"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>[x0.8, x1, x1.2] </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.30703</cdr:x>
+      <cdr:y>0.03574</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.46228</cdr:x>
+      <cdr:y>0.10317</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="6" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1077D5F8-C748-21F0-1680-A2B87A7E2AB9}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3536625" y="171595"/>
+          <a:ext cx="1788308" cy="323705"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1400"/>
+            <a:t>[1, Supply, 75] $/ton </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.53209</cdr:x>
+      <cdr:y>0.04324</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.82171</cdr:x>
+      <cdr:y>0.12434</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CB80F9F-6919-B9CE-5CCD-98C3DD19EDE7}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="6129114" y="207576"/>
+          <a:ext cx="3336104" cy="389324"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Reference case Δ(NPV)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> = $1,430,198,349</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.00486</cdr:x>
+      <cdr:y>0.85414</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.09444</cdr:x>
+      <cdr:y>0.92583</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FCFB347-86E3-68C2-1ACD-C064B58A522B}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="57150" y="4387850"/>
+          <a:ext cx="1054100" cy="368300"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.02785</cdr:x>
+      <cdr:y>0.82027</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.11204</cdr:x>
+      <cdr:y>0.89443</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{882866D9-D847-D3F5-3422-E895513A3DB1}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="344860" y="4401351"/>
+          <a:ext cx="1042456" cy="397954"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="r"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>[</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>30</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>60</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>]</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0"/>
+            <a:t> $/ton</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.54675</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.11487</cdr:x>
+      <cdr:y>0.62604</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="4" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAE259CA-9266-FB6F-5812-9B6CCD141894}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="2933700"/>
+          <a:ext cx="1422400" cy="425450"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="r"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>[</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>x0.75</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>x1.25</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>]</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0"/>
+            <a:t> (FT+HTSE+H2 sto.)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.02872</cdr:x>
+      <cdr:y>0.28166</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.11291</cdr:x>
+      <cdr:y>0.35582</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="5" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAE259CA-9266-FB6F-5812-9B6CCD141894}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="355600" y="1511300"/>
+          <a:ext cx="1042456" cy="397954"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="r"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>[</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>x0.75</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>x1.25</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>]</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.58359</cdr:x>
+      <cdr:y>0.01775</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.82667</cdr:x>
+      <cdr:y>0.09349</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73A233EE-B2CE-5ED7-10F4-960E333D34BB}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="7226300" y="95250"/>
+          <a:ext cx="3009900" cy="406400"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Braidwood</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="C00000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> Ref. Δ(NPV) = $bn 1.487</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" b="1">
+            <a:solidFill>
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+          </a:endParaRPr>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="New_fin_param"/>
+      <sheetName val="Old_fin_param"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="13">
+          <cell r="B13" t="str">
+            <v>Low</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="D14">
+            <v>13044061.337726347</v>
+          </cell>
+          <cell r="E14">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="D15">
+            <v>14584955.770416418</v>
+          </cell>
+          <cell r="E15">
+            <v>14749672.60467495</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="D16">
+            <v>14477794.612199999</v>
+          </cell>
+          <cell r="E16">
+            <v>14477794.612199999</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1850,7 +4797,7 @@
   <dimension ref="A1:AJ8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+      <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1858,15 +4805,15 @@
     <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="11.83203125" customWidth="1"/>
     <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="19" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="15.83203125" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.6640625" customWidth="1"/>
     <col min="16" max="16" width="23.33203125" customWidth="1"/>
     <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
@@ -2002,12 +4949,10 @@
         <v>1175</v>
       </c>
       <c r="D3">
-        <f>29528/1000</f>
-        <v>29.527999999999999</v>
+        <v>10.1</v>
       </c>
       <c r="E3" s="3">
-        <f>39153/1000</f>
-        <v>39.152999999999999</v>
+        <v>51.2</v>
       </c>
       <c r="F3">
         <v>2102483898.8800001</v>
@@ -2019,35 +4964,35 @@
         <f>G3/F3</f>
         <v>4.9665897586956935E-3</v>
       </c>
-      <c r="I3">
-        <v>3589667022.7199998</v>
-      </c>
-      <c r="J3">
-        <v>20927.310484099999</v>
+      <c r="I3" s="15">
+        <v>3091190401</v>
+      </c>
+      <c r="J3" s="15">
+        <v>2724584.22</v>
       </c>
       <c r="K3">
         <f>J3/I3</f>
-        <v>5.8298751253654551E-6</v>
+        <v>8.8140291168043133E-4</v>
       </c>
       <c r="L3">
         <f>I3-F3</f>
-        <v>1487183123.8399997</v>
+        <v>988706502.11999989</v>
       </c>
       <c r="M3">
         <f>100*SQRT(POWER(K3,2)+POWER(H3,2))</f>
-        <v>0.49665931803022612</v>
+        <v>0.50441931885981217</v>
       </c>
       <c r="N3">
         <f>SQRT(POWER(J3,2)+POWER(G3,2))</f>
-        <v>10442195.970338283</v>
+        <v>10791773.621722151</v>
       </c>
       <c r="O3" s="1">
         <f>L3</f>
-        <v>1487183123.8399997</v>
+        <v>988706502.11999989</v>
       </c>
       <c r="P3" s="1">
         <f>N3</f>
-        <v>10442195.970338283</v>
+        <v>10791773.621722151</v>
       </c>
       <c r="Q3" s="1">
         <f>ABS(X3+AC3+AB3)</f>
@@ -2120,12 +5065,10 @@
         <v>507</v>
       </c>
       <c r="D4">
-        <f>12551/1000</f>
-        <v>12.551</v>
+        <v>10.1</v>
       </c>
       <c r="E4" s="3">
-        <f>5378/1000</f>
-        <v>5.3780000000000001</v>
+        <v>5.4</v>
       </c>
       <c r="F4">
         <v>262560457.34999999</v>
@@ -2138,34 +5081,34 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>1470930578.27</v>
+        <v>1059865693.28</v>
       </c>
       <c r="J4">
-        <v>18007.90423</v>
+        <v>112426.783738</v>
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K8" si="1">J4/I4</f>
-        <v>1.2242524899563627E-5</v>
+        <v>1.0607644388419561E-4</v>
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L8" si="2">I4-F4</f>
-        <v>1208370120.9200001</v>
+        <v>797305235.92999995</v>
       </c>
       <c r="M4">
         <f t="shared" ref="M4:M8" si="3">100*SQRT(POWER(K4,2)+POWER(H4,2))</f>
-        <v>1.2242524899563627E-3</v>
+        <v>1.0607644388419562E-2</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N8" si="4">SQRT(POWER(J4,2)+POWER(G4,2))</f>
-        <v>18007.90423</v>
+        <v>112426.783738</v>
       </c>
       <c r="O4" s="1">
         <f t="shared" ref="O4:O8" si="5">L4</f>
-        <v>1208370120.9200001</v>
+        <v>797305235.92999995</v>
       </c>
       <c r="P4" s="1">
         <f t="shared" ref="P4:P8" si="6">N4</f>
-        <v>18007.90423</v>
+        <v>112426.783738</v>
       </c>
       <c r="Q4" s="1">
         <f t="shared" ref="Q4:Q8" si="7">ABS(X4+AC4+AB4)</f>
@@ -2238,12 +5181,10 @@
         <v>879</v>
       </c>
       <c r="D5">
-        <f>22089/1000</f>
-        <v>22.088999999999999</v>
-      </c>
-      <c r="E5" s="3">
-        <f>24075/1000</f>
-        <v>24.074999999999999</v>
+        <v>10.1</v>
+      </c>
+      <c r="E5" s="16">
+        <v>30</v>
       </c>
       <c r="F5">
         <v>1765764570.5999999</v>
@@ -2256,34 +5197,34 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>3121827095.6100001</v>
+        <v>2514348849.4299998</v>
       </c>
       <c r="J5">
-        <v>2453.2582657600001</v>
+        <v>1136859.4810800001</v>
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
-        <v>7.8584053204286677E-7</v>
+        <v>4.5214866717389868E-4</v>
       </c>
       <c r="L5">
         <f t="shared" si="2"/>
-        <v>1356062525.0100002</v>
+        <v>748584278.82999992</v>
       </c>
       <c r="M5">
         <f t="shared" si="3"/>
-        <v>7.8584053204286671E-5</v>
+        <v>4.5214866717389869E-2</v>
       </c>
       <c r="N5">
         <f t="shared" si="4"/>
-        <v>2453.2582657600001</v>
+        <v>1136859.4810800001</v>
       </c>
       <c r="O5" s="1">
         <f t="shared" si="5"/>
-        <v>1356062525.0100002</v>
+        <v>748584278.82999992</v>
       </c>
       <c r="P5" s="1">
         <f t="shared" si="6"/>
-        <v>2453.2582657600001</v>
+        <v>1136859.4810800001</v>
       </c>
       <c r="Q5" s="1">
         <f t="shared" si="7"/>
@@ -2356,12 +5297,10 @@
         <v>754</v>
       </c>
       <c r="D6">
-        <f>18948/1000</f>
-        <v>18.948</v>
+        <v>10.1</v>
       </c>
       <c r="E6" s="3">
-        <f>39056/1000</f>
-        <v>39.055999999999997</v>
+        <v>17.8</v>
       </c>
       <c r="F6">
         <v>1080996406.4100001</v>
@@ -2374,34 +5313,34 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>2324055498.54</v>
+        <v>1881333379.3099999</v>
       </c>
       <c r="J6">
-        <v>5809.0129145299998</v>
+        <v>2014357.9649499999</v>
       </c>
       <c r="K6">
         <f t="shared" si="1"/>
-        <v>2.4995155744685497E-6</v>
+        <v>1.0707076093492735E-3</v>
       </c>
       <c r="L6">
         <f t="shared" si="2"/>
-        <v>1243059092.1299999</v>
+        <v>800336972.89999986</v>
       </c>
       <c r="M6">
         <f t="shared" si="3"/>
-        <v>2.49951557446855E-4</v>
+        <v>0.10707076093492734</v>
       </c>
       <c r="N6">
         <f t="shared" si="4"/>
-        <v>5809.0129145299998</v>
+        <v>2014357.9649499999</v>
       </c>
       <c r="O6" s="1">
         <f t="shared" si="5"/>
-        <v>1243059092.1299999</v>
+        <v>800336972.89999986</v>
       </c>
       <c r="P6" s="1">
         <f t="shared" si="6"/>
-        <v>5809.0129145299998</v>
+        <v>2014357.9649499999</v>
       </c>
       <c r="Q6" s="1">
         <f t="shared" si="7"/>
@@ -2471,15 +5410,13 @@
         <v>1280</v>
       </c>
       <c r="C7" s="4">
-        <v>1265</v>
+        <v>1042</v>
       </c>
       <c r="D7" s="4">
-        <f>10144/1000</f>
-        <v>10.144</v>
+        <v>10.1</v>
       </c>
       <c r="E7" s="5">
-        <f>100661/1000</f>
-        <v>100.661</v>
+        <v>76.400000000000006</v>
       </c>
       <c r="F7">
         <v>2721027335.4499998</v>
@@ -2492,34 +5429,34 @@
         <v>2.7969213517920744E-2</v>
       </c>
       <c r="I7">
-        <v>4471032641.4499998</v>
+        <v>3607549851.6599998</v>
       </c>
       <c r="J7">
-        <v>26484477.825399999</v>
+        <v>28360934.292199999</v>
       </c>
       <c r="K7">
         <f t="shared" si="1"/>
-        <v>5.9235706713182982E-3</v>
+        <v>7.8615502095278952E-3</v>
       </c>
       <c r="L7">
         <f t="shared" si="2"/>
-        <v>1750005306</v>
+        <v>886522516.21000004</v>
       </c>
       <c r="M7">
         <f t="shared" si="3"/>
-        <v>2.8589606403536632</v>
+        <v>2.90530700014296</v>
       </c>
       <c r="N7">
         <f t="shared" si="4"/>
-        <v>80581621.717347726</v>
+        <v>81217687.647704601</v>
       </c>
       <c r="O7" s="1">
         <f t="shared" si="5"/>
-        <v>1750005306</v>
+        <v>886522516.21000004</v>
       </c>
       <c r="P7" s="1">
         <f t="shared" si="6"/>
-        <v>80581621.717347726</v>
+        <v>81217687.647704601</v>
       </c>
       <c r="Q7" s="1">
         <f t="shared" si="7"/>
@@ -2657,15 +5594,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBA1661-1357-8E4D-8878-EEFCBAD9628D}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="T17" sqref="T17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -2731,7 +5669,7 @@
         <v>20927.310484099999</v>
       </c>
       <c r="D3" s="11">
-        <f t="shared" ref="D3:D7" si="0">C3/B3</f>
+        <f t="shared" ref="D3:D9" si="0">C3/B3</f>
         <v>5.8298751253654551E-6</v>
       </c>
       <c r="E3">
@@ -2739,7 +5677,7 @@
         <v>1487183123.8399997</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F7" si="1">SQRT(POWER($C$2,2)+POWER(C3,2))</f>
+        <f t="shared" ref="F3:F9" si="1">SQRT(POWER($C$2,2)+POWER(C3,2))</f>
         <v>10442196.451737316</v>
       </c>
       <c r="G3" s="11">
@@ -2762,7 +5700,7 @@
         <v>4.6148954493854593E-4</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E7" si="2">B4-$B$2</f>
+        <f t="shared" ref="E4:E9" si="2">B4-$B$2</f>
         <v>1172229378.5599999</v>
       </c>
       <c r="F4">
@@ -2770,7 +5708,7 @@
         <v>10550966.452233298</v>
       </c>
       <c r="G4" s="11">
-        <f t="shared" ref="G4:G7" si="3">F4/E4</f>
+        <f t="shared" ref="G4:G9" si="3">F4/E4</f>
         <v>9.0007695125286884E-3</v>
       </c>
     </row>
@@ -2832,35 +5770,166 @@
       <c r="A7" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="11" t="e">
+      <c r="B7">
+        <v>3532348131.6100001</v>
+      </c>
+      <c r="C7">
+        <v>18113.533749900002</v>
+      </c>
+      <c r="D7" s="11">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>5.1279016322901559E-6</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
-        <v>-2102483898.8800001</v>
+        <v>1429864232.73</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>10442175.4814</v>
+        <v>10442191.191721028</v>
       </c>
       <c r="G7" s="11">
         <f t="shared" si="3"/>
-        <v>-4.966589987662964E-3</v>
+        <v>7.3029249579759353E-3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>39</v>
       </c>
+      <c r="B8">
+        <v>3277897462.3600001</v>
+      </c>
+      <c r="C8">
+        <v>3378696.8678199998</v>
+      </c>
+      <c r="D8" s="11">
+        <f t="shared" si="0"/>
+        <v>1.0307512381389217E-3</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>1175413563.48</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="1"/>
+        <v>10975182.062679781</v>
+      </c>
+      <c r="G8" s="11">
+        <f t="shared" si="3"/>
+        <v>9.3372940415848166E-3</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>40</v>
       </c>
+      <c r="B9">
+        <v>3169409970</v>
+      </c>
+      <c r="C9">
+        <v>4256561.38</v>
+      </c>
+      <c r="D9" s="11">
+        <f t="shared" si="0"/>
+        <v>1.3430138165432728E-3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>1066926071.1199999</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>11276406.500568291</v>
+      </c>
+      <c r="G9" s="11">
+        <f t="shared" si="3"/>
+        <v>1.0569060786686882E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" t="s">
+        <v>65</v>
+      </c>
+      <c r="D11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12">
+        <f>E4</f>
+        <v>1172229378.5599999</v>
+      </c>
+      <c r="C12">
+        <f>E5</f>
+        <v>1820055812.4000001</v>
+      </c>
+      <c r="D12">
+        <f>F4</f>
+        <v>10550966.452233298</v>
+      </c>
+      <c r="E12">
+        <f>F5</f>
+        <v>10442196.187159013</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13">
+        <f>E6</f>
+        <v>1517352719.2799997</v>
+      </c>
+      <c r="C13">
+        <f>E7</f>
+        <v>1429864232.73</v>
+      </c>
+      <c r="D13">
+        <f>F6</f>
+        <v>10457191.662380703</v>
+      </c>
+      <c r="E13">
+        <f>F7</f>
+        <v>10442191.191721028</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14">
+        <f>E8</f>
+        <v>1175413563.48</v>
+      </c>
+      <c r="C14">
+        <f>E9</f>
+        <v>1066926071.1199999</v>
+      </c>
+      <c r="D14">
+        <f>F8</f>
+        <v>10975182.062679781</v>
+      </c>
+      <c r="E14">
+        <f>F9</f>
+        <v>11276406.500568291</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add intermediate results for OM SA
</commit_message>
<xml_diff>
--- a/use_cases/IES_Feb23/run/results.xlsx
+++ b/use_cases/IES_Feb23/run/results.xlsx
@@ -8,18 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/IES_Feb23/run/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3E188F-9F4B-EA40-8045-6F54FB5C7273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBA52CF-5AC1-BD47-8C84-838090CC9645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
+    <workbookView xWindow="30720" yWindow="-940" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
     <sheet name="braidwood_SA" sheetId="2" r:id="rId2"/>
     <sheet name="covid" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="74">
   <si>
     <t>Location</t>
   </si>
@@ -254,6 +251,15 @@
   </si>
   <si>
     <t>CO2 Cost</t>
+  </si>
+  <si>
+    <t>om low</t>
+  </si>
+  <si>
+    <t>om high</t>
+  </si>
+  <si>
+    <t>OM Costs</t>
   </si>
 </sst>
 </file>
@@ -263,7 +269,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -439,6 +445,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -448,8 +456,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1017,526 +1023,6 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13656364383023548"/>
-          <c:y val="0.20686157962845172"/>
-          <c:w val="0.73386719517203203"/>
-          <c:h val="0.71235847608185465"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>braidwood_SA!$A$12</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Synfuel Price</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>[1]New_fin_param!$D$14:$D$16</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
-                  <c:pt idx="0">
-                    <c:v>13044061.337726347</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>14584955.770416418</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>14477794.612199999</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>[1]New_fin_param!$D$14:$D$16</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
-                  <c:pt idx="0">
-                    <c:v>13044061.337726347</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>14584955.770416418</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>14477794.612199999</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:cat>
-            <c:strRef>
-              <c:f>braidwood_SA!$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>CO2 Cost</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>braidwood_SA!$B$12:$C$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1172229378.5599999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1820055812.4000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3789-624C-893F-DC9282CA661B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>braidwood_SA!$A$13</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>CAPEX</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>[1]New_fin_param!$E$14:$E$16</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
-                  <c:pt idx="0">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>14749672.60467495</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>14477794.612199999</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>[1]New_fin_param!$E$14:$E$16</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="3"/>
-                  <c:pt idx="0">
-                    <c:v>0</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>14749672.60467495</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>14477794.612199999</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:cat>
-            <c:strRef>
-              <c:f>braidwood_SA!$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>CO2 Cost</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>braidwood_SA!$B$13:$C$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1517352719.2799997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1429864232.73</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-3789-624C-893F-DC9282CA661B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>braidwood_SA!$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>CO2 Cost</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>braidwood_SA!$A$14</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>CO2 Cost</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>braidwood_SA!$B$14:$C$14</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>1175413563.48</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1066926071.1199999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-3789-624C-893F-DC9282CA661B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="300"/>
-        <c:overlap val="100"/>
-        <c:axId val="1079498976"/>
-        <c:axId val="1079459696"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1079498976"/>
-        <c:scaling>
-          <c:orientation val="maxMin"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="low"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="22225" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:srgbClr val="C00000"/>
-            </a:solidFill>
-            <a:prstDash val="dash"/>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1079459696"/>
-        <c:crossesAt val="1476746599.9999998"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1079459696"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="t"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:numFmt formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;?_);_(@_)" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1079498976"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:dispUnits>
-          <c:builtInUnit val="billions"/>
-          <c:dispUnitsLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-          </c:dispUnitsLbl>
-        </c:dispUnits>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-  <c:userShapes r:id="rId3"/>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
           <c:x val="0.11876018574601252"/>
           <c:y val="0.13282057494292504"/>
           <c:w val="0.79406840298808801"/>
@@ -1572,9 +1058,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>braidwood_SA!$A$12:$A$14</c:f>
+              <c:f>braidwood_SA!$A$14:$A$17</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Synfuel Price</c:v>
                 </c:pt>
@@ -1584,23 +1070,29 @@
                 <c:pt idx="2">
                   <c:v>CO2 Cost</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>OM Costs</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>braidwood_SA!$B$12:$B$14</c:f>
+              <c:f>braidwood_SA!$B$14:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1172229378.5599999</c:v>
+                  <c:v>880381001.11999989</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1517352719.2799997</c:v>
+                  <c:v>1011661667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1175413563.48</c:v>
+                  <c:v>893309063.67000008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1125774210.8099999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1616,7 +1108,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>braidwood_SA!$C$11</c:f>
+              <c:f>braidwood_SA!$C$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1637,9 +1129,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>braidwood_SA!$A$12:$A$14</c:f>
+              <c:f>braidwood_SA!$A$14:$A$17</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>Synfuel Price</c:v>
                 </c:pt>
@@ -1649,23 +1141,29 @@
                 <c:pt idx="2">
                   <c:v>CO2 Cost</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>OM Costs</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>braidwood_SA!$C$12:$C$14</c:f>
+              <c:f>braidwood_SA!$C$14:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1820055812.4000001</c:v>
+                  <c:v>1099884513.1199999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1429864232.73</c:v>
+                  <c:v>970655949.33999968</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1066926071.1199999</c:v>
+                  <c:v>796970247.11999989</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>852118150.08999968</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1731,7 +1229,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1796024143"/>
-        <c:crossesAt val="1487183124.0000002"/>
+        <c:crossesAt val="988706500"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1741,6 +1239,7 @@
         <c:axId val="1796024143"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="750000000.00000012"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -1792,10 +1291,10 @@
         <c:crossAx val="414221104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="250000000"/>
-        <c:minorUnit val="100000000"/>
+        <c:majorUnit val="50000000"/>
+        <c:minorUnit val="50000000"/>
         <c:dispUnits>
-          <c:builtInUnit val="billions"/>
+          <c:builtInUnit val="millions"/>
           <c:dispUnitsLbl>
             <c:spPr>
               <a:noFill/>
@@ -1957,46 +1456,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2501,511 +1960,6 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3555,53 +2509,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>698500</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A188611D-D3FF-6646-8ED0-8E1D8DE54A57}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>774700</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3621,7 +2537,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3631,385 +2547,6 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.12018</cdr:x>
-      <cdr:y>0.05547</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.27543</cdr:x>
-      <cdr:y>0.1229</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="4" name="TextBox 1">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26AA5548-A60A-D05C-0D51-011C1B561077}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1384300" y="266284"/>
-          <a:ext cx="1788310" cy="323704"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:lvl1pPr marL="0" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>[23, LMP, 65] $/MWe </a:t>
-          </a:r>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0</cdr:x>
-      <cdr:y>0</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.11344</cdr:x>
-      <cdr:y>0.06514</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="5" name="TextBox 1">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26AA5548-A60A-D05C-0D51-011C1B561077}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="0" y="0"/>
-          <a:ext cx="1354246" cy="343322"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:lvl1pPr marL="0" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>[x0.8, x1, x1.2] </a:t>
-          </a:r>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.30703</cdr:x>
-      <cdr:y>0.03574</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.46228</cdr:x>
-      <cdr:y>0.10317</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="6" name="TextBox 1">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1077D5F8-C748-21F0-1680-A2B87A7E2AB9}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="3536625" y="171595"/>
-          <a:ext cx="1788308" cy="323705"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:lvl1pPr marL="0" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl1pPr>
-          <a:lvl2pPr marL="457200" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl2pPr>
-          <a:lvl3pPr marL="914400" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl3pPr>
-          <a:lvl4pPr marL="1371600" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl4pPr>
-          <a:lvl5pPr marL="1828800" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl5pPr>
-          <a:lvl6pPr marL="2286000" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl6pPr>
-          <a:lvl7pPr marL="2743200" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl7pPr>
-          <a:lvl8pPr marL="3200400" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl8pPr>
-          <a:lvl9pPr marL="3657600" indent="0">
-            <a:defRPr sz="1100">
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:lvl9pPr>
-        </a:lstStyle>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:r>
-            <a:rPr lang="en-US" sz="1400"/>
-            <a:t>[1, Supply, 75] $/ton </a:t>
-          </a:r>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
-    <cdr:from>
-      <cdr:x>0.53209</cdr:x>
-      <cdr:y>0.04324</cdr:y>
-    </cdr:from>
-    <cdr:to>
-      <cdr:x>0.82171</cdr:x>
-      <cdr:y>0.12434</cdr:y>
-    </cdr:to>
-    <cdr:sp macro="" textlink="">
-      <cdr:nvSpPr>
-        <cdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0CB80F9F-6919-B9CE-5CCD-98C3DD19EDE7}"/>
-            </a:ext>
-          </a:extLst>
-        </cdr:cNvPr>
-        <cdr:cNvSpPr txBox="1"/>
-      </cdr:nvSpPr>
-      <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="6129114" y="207576"/>
-          <a:ext cx="3336104" cy="389324"/>
-        </a:xfrm>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </cdr:spPr>
-      <cdr:txBody>
-        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
-        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1">
-              <a:solidFill>
-                <a:srgbClr val="C00000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Reference case Δ(NPV)</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1400" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="C00000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> = $1,430,198,349</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1400" b="1">
-            <a:solidFill>
-              <a:srgbClr val="C00000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </cdr:txBody>
-    </cdr:sp>
-  </cdr:relSizeAnchor>
-</c:userShapes>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -4052,11 +2589,11 @@
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
       <cdr:x>0.02785</cdr:x>
-      <cdr:y>0.82027</cdr:y>
+      <cdr:y>0.64512</cdr:y>
     </cdr:from>
     <cdr:to>
       <cdr:x>0.11204</cdr:x>
-      <cdr:y>0.89443</cdr:y>
+      <cdr:y>0.71928</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4071,8 +2608,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="344860" y="4401351"/>
-          <a:ext cx="1042456" cy="397954"/>
+          <a:off x="344853" y="3461564"/>
+          <a:ext cx="1042482" cy="397924"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4123,11 +2660,11 @@
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
       <cdr:x>0</cdr:x>
-      <cdr:y>0.54675</cdr:y>
+      <cdr:y>0.44497</cdr:y>
     </cdr:from>
     <cdr:to>
       <cdr:x>0.11487</cdr:x>
-      <cdr:y>0.62604</cdr:y>
+      <cdr:y>0.52426</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4142,8 +2679,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="0" y="2933700"/>
-          <a:ext cx="1422400" cy="425450"/>
+          <a:off x="0" y="2387624"/>
+          <a:ext cx="1422378" cy="425450"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4257,12 +2794,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.02872</cdr:x>
-      <cdr:y>0.28166</cdr:y>
+      <cdr:x>0.02769</cdr:x>
+      <cdr:y>0.24616</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.11291</cdr:x>
-      <cdr:y>0.35582</cdr:y>
+      <cdr:x>0.11188</cdr:x>
+      <cdr:y>0.32032</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4277,8 +2814,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="355600" y="1511300"/>
-          <a:ext cx="1042456" cy="397954"/>
+          <a:off x="342925" y="1320817"/>
+          <a:ext cx="1042483" cy="397924"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4392,12 +2929,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.58359</cdr:x>
-      <cdr:y>0.01775</cdr:y>
+      <cdr:x>0.46769</cdr:x>
+      <cdr:y>0.01538</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.82667</cdr:x>
-      <cdr:y>0.09349</cdr:y>
+      <cdr:x>0.71077</cdr:x>
+      <cdr:y>0.09112</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -4412,8 +2949,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="7226300" y="95250"/>
-          <a:ext cx="3009900" cy="406400"/>
+          <a:off x="5791203" y="82542"/>
+          <a:ext cx="3009938" cy="406402"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -4438,7 +2975,7 @@
                 <a:srgbClr val="C00000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> Ref. Δ(NPV) = $bn 1.487</a:t>
+            <a:t> Ref. Δ(NPV) = $M 988,71</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1400" b="1">
             <a:solidFill>
@@ -4449,52 +2986,142 @@
       </cdr:txBody>
     </cdr:sp>
   </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0</cdr:x>
+      <cdr:y>0.84024</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.11487</cdr:x>
+      <cdr:y>0.91953</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="8" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BB6F14E-B88B-D129-C5D6-6CC3C9D66D90}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="0" y="4508500"/>
+          <a:ext cx="1422378" cy="425450"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="r"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>[</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>x0.75</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>x1.25</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>]</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0"/>
+            <a:t> (FT+HTSE+H2 sto.)</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
 </c:userShapes>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="New_fin_param"/>
-      <sheetName val="Old_fin_param"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="13">
-          <cell r="B13" t="str">
-            <v>Low</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="D14">
-            <v>13044061.337726347</v>
-          </cell>
-          <cell r="E14">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="D15">
-            <v>14584955.770416418</v>
-          </cell>
-          <cell r="E15">
-            <v>14749672.60467495</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="D16">
-            <v>14477794.612199999</v>
-          </cell>
-          <cell r="E16">
-            <v>14477794.612199999</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4796,7 +3423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FE355D-8072-1247-9790-841EBA440D66}">
   <dimension ref="A1:AJ8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E7"/>
     </sheetView>
   </sheetViews>
@@ -4824,12 +3451,12 @@
   <sheetData>
     <row r="1" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="14"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -4964,10 +3591,10 @@
         <f>G3/F3</f>
         <v>4.9665897586956935E-3</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="12">
         <v>3091190401</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J3" s="12">
         <v>2724584.22</v>
       </c>
       <c r="K3">
@@ -5183,7 +3810,7 @@
       <c r="D5">
         <v>10.1</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="13">
         <v>30</v>
       </c>
       <c r="F5">
@@ -5594,10 +4221,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBA1661-1357-8E4D-8878-EEFCBAD9628D}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5663,26 +4290,26 @@
         <v>29</v>
       </c>
       <c r="B3">
-        <v>3589667022.7199998</v>
+        <v>3091190401</v>
       </c>
       <c r="C3">
-        <v>20927.310484099999</v>
+        <v>2724584.22</v>
       </c>
       <c r="D3" s="11">
-        <f t="shared" ref="D3:D9" si="0">C3/B3</f>
-        <v>5.8298751253654551E-6</v>
+        <f t="shared" ref="D3:D11" si="0">C3/B3</f>
+        <v>8.8140291168043133E-4</v>
       </c>
       <c r="E3">
         <f>B3-$B$2</f>
-        <v>1487183123.8399997</v>
+        <v>988706502.11999989</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F9" si="1">SQRT(POWER($C$2,2)+POWER(C3,2))</f>
-        <v>10442196.451737316</v>
+        <f t="shared" ref="F3:F11" si="1">SQRT(POWER($C$2,2)+POWER(C3,2))</f>
+        <v>10791774.087527238</v>
       </c>
       <c r="G3" s="11">
         <f>F3/E3</f>
-        <v>7.0214597545828206E-3</v>
+        <v>1.0915043103678744E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -5690,26 +4317,26 @@
         <v>30</v>
       </c>
       <c r="B4">
-        <v>3274713277.4400001</v>
+        <v>2982864900</v>
       </c>
       <c r="C4">
-        <v>1511245.9402099999</v>
+        <v>4436364.47</v>
       </c>
       <c r="D4" s="11">
         <f t="shared" si="0"/>
-        <v>4.6148954493854593E-4</v>
+        <v>1.4872830713854991E-3</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E9" si="2">B4-$B$2</f>
-        <v>1172229378.5599999</v>
+        <f t="shared" ref="E4:E11" si="2">B4-$B$2</f>
+        <v>880381001.11999989</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>10550966.452233298</v>
+        <v>11345499.481954494</v>
       </c>
       <c r="G4" s="11">
-        <f t="shared" ref="G4:G9" si="3">F4/E4</f>
-        <v>9.0007695125286884E-3</v>
+        <f t="shared" ref="G4:G11" si="3">F4/E4</f>
+        <v>1.2887033531528983E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -5717,26 +4344,26 @@
         <v>31</v>
       </c>
       <c r="B5">
-        <v>3922539711.2800002</v>
+        <v>3202368412</v>
       </c>
       <c r="C5">
-        <v>20794.873572600001</v>
+        <v>2472844.06</v>
       </c>
       <c r="D5" s="11">
         <f t="shared" si="0"/>
-        <v>5.3013799994938064E-6</v>
+        <v>7.7219224706741828E-4</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
-        <v>1820055812.4000001</v>
+        <v>1099884513.1199999</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>10442196.187159013</v>
+        <v>10730982.551911479</v>
       </c>
       <c r="G5" s="11">
         <f t="shared" si="3"/>
-        <v>5.7372944917494072E-3</v>
+        <v>9.7564629958024549E-3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -5744,26 +4371,26 @@
         <v>32</v>
       </c>
       <c r="B6">
-        <v>3619836618.1599998</v>
+        <v>3114145565.8800001</v>
       </c>
       <c r="C6">
-        <v>560204.140839</v>
+        <v>4555498.9392900001</v>
       </c>
       <c r="D6" s="11">
         <f t="shared" si="0"/>
-        <v>1.5475950987085089E-4</v>
+        <v>1.4628407192014802E-3</v>
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
-        <v>1517352719.2799997</v>
+        <v>1011661667</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>10457191.662380703</v>
+        <v>11392611.61324407</v>
       </c>
       <c r="G6" s="11">
         <f t="shared" si="3"/>
-        <v>6.8917342220487492E-3</v>
+        <v>1.1261286243085524E-2</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -5771,26 +4398,26 @@
         <v>33</v>
       </c>
       <c r="B7">
-        <v>3532348131.6100001</v>
+        <v>3073139848.2199998</v>
       </c>
       <c r="C7">
-        <v>18113.533749900002</v>
+        <v>3087947.7798199998</v>
       </c>
       <c r="D7" s="11">
         <f t="shared" si="0"/>
-        <v>5.1279016322901559E-6</v>
+        <v>1.0048185023563366E-3</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
-        <v>1429864232.73</v>
+        <v>970655949.33999968</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>10442191.191721028</v>
+        <v>10889189.605992109</v>
       </c>
       <c r="G7" s="11">
         <f t="shared" si="3"/>
-        <v>7.3029249579759353E-3</v>
+        <v>1.1218382387081895E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -5798,26 +4425,26 @@
         <v>39</v>
       </c>
       <c r="B8">
-        <v>3277897462.3600001</v>
+        <v>2995792962.5500002</v>
       </c>
       <c r="C8">
-        <v>3378696.8678199998</v>
+        <v>5906834.7022700002</v>
       </c>
       <c r="D8" s="11">
         <f t="shared" si="0"/>
-        <v>1.0307512381389217E-3</v>
+        <v>1.9717099199145389E-3</v>
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
-        <v>1175413563.48</v>
+        <v>893309063.67000008</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>10975182.062679781</v>
+        <v>11997071.517011659</v>
       </c>
       <c r="G8" s="11">
         <f t="shared" si="3"/>
-        <v>9.3372940415848166E-3</v>
+        <v>1.3429922526167867E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -5825,106 +4452,181 @@
         <v>40</v>
       </c>
       <c r="B9">
-        <v>3169409970</v>
+        <v>2899454146</v>
       </c>
       <c r="C9">
-        <v>4256561.38</v>
+        <v>1244304.42</v>
       </c>
       <c r="D9" s="11">
         <f t="shared" si="0"/>
-        <v>1.3430138165432728E-3</v>
+        <v>4.291512668743546E-4</v>
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
-        <v>1066926071.1199999</v>
+        <v>796970247.11999989</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>11276406.500568291</v>
+        <v>10516050.697575722</v>
       </c>
       <c r="G9" s="11">
         <f t="shared" si="3"/>
-        <v>1.0569060786686882E-2</v>
+        <v>1.3195035492952749E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B10">
+        <v>3228258109.6900001</v>
+      </c>
+      <c r="C10">
+        <v>3394463.3216200001</v>
+      </c>
+      <c r="D10" s="11">
+        <f t="shared" si="0"/>
+        <v>1.0514844867673733E-3</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>1125774210.8099999</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>10980045.993809626</v>
+      </c>
+      <c r="G10" s="11">
+        <f t="shared" si="3"/>
+        <v>9.7533287655518688E-3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12">
-        <f>E4</f>
-        <v>1172229378.5599999</v>
-      </c>
-      <c r="C12">
-        <f>E5</f>
-        <v>1820055812.4000001</v>
-      </c>
-      <c r="D12">
-        <f>F4</f>
-        <v>10550966.452233298</v>
-      </c>
-      <c r="E12">
-        <f>F5</f>
-        <v>10442196.187159013</v>
+        <v>72</v>
+      </c>
+      <c r="B11">
+        <v>2954602048.9699998</v>
+      </c>
+      <c r="C11">
+        <v>5465429.1587100001</v>
+      </c>
+      <c r="D11" s="11">
+        <f t="shared" si="0"/>
+        <v>1.8498021283831765E-3</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>852118150.08999968</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>11786006.307194512</v>
+      </c>
+      <c r="G11" s="11">
+        <f t="shared" si="3"/>
+        <v>1.3831422680000056E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>69</v>
-      </c>
-      <c r="B13">
-        <f>E6</f>
-        <v>1517352719.2799997</v>
-      </c>
-      <c r="C13">
-        <f>E7</f>
-        <v>1429864232.73</v>
-      </c>
-      <c r="D13">
-        <f>F6</f>
-        <v>10457191.662380703</v>
-      </c>
-      <c r="E13">
-        <f>F7</f>
-        <v>10442191.191721028</v>
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14">
+        <f>E4</f>
+        <v>880381001.11999989</v>
+      </c>
+      <c r="C14">
+        <f>E5</f>
+        <v>1099884513.1199999</v>
+      </c>
+      <c r="D14">
+        <f>F4</f>
+        <v>11345499.481954494</v>
+      </c>
+      <c r="E14">
+        <f>F5</f>
+        <v>10730982.551911479</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15">
+        <f>E6</f>
+        <v>1011661667</v>
+      </c>
+      <c r="C15">
+        <f>E7</f>
+        <v>970655949.33999968</v>
+      </c>
+      <c r="D15">
+        <f>F6</f>
+        <v>11392611.61324407</v>
+      </c>
+      <c r="E15">
+        <f>F7</f>
+        <v>10889189.605992109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
         <v>70</v>
       </c>
-      <c r="B14">
+      <c r="B16">
         <f>E8</f>
-        <v>1175413563.48</v>
-      </c>
-      <c r="C14">
+        <v>893309063.67000008</v>
+      </c>
+      <c r="C16">
         <f>E9</f>
-        <v>1066926071.1199999</v>
-      </c>
-      <c r="D14">
+        <v>796970247.11999989</v>
+      </c>
+      <c r="D16">
         <f>F8</f>
-        <v>10975182.062679781</v>
-      </c>
-      <c r="E14">
+        <v>11997071.517011659</v>
+      </c>
+      <c r="E16">
         <f>F9</f>
-        <v>11276406.500568291</v>
+        <v>10516050.697575722</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17">
+        <f>E10</f>
+        <v>1125774210.8099999</v>
+      </c>
+      <c r="C17">
+        <f>E11</f>
+        <v>852118150.08999968</v>
+      </c>
+      <c r="D17">
+        <f>F10</f>
+        <v>10980045.993809626</v>
+      </c>
+      <c r="E17">
+        <f>F11</f>
+        <v>11786006.307194512</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update results after htse capex fix
</commit_message>
<xml_diff>
--- a/use_cases/IES_Feb23/run/results.xlsx
+++ b/use_cases/IES_Feb23/run/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/IES_Feb23/run/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEBA52CF-5AC1-BD47-8C84-838090CC9645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{872C7089-B355-FD46-A250-0F7656D1202C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30720" yWindow="-940" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
+    <workbookView xWindow="15320" yWindow="500" windowWidth="20520" windowHeight="20200" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
@@ -154,9 +154,6 @@
     <t>no covid</t>
   </si>
   <si>
-    <t>CAPEX (M$)</t>
-  </si>
-  <si>
     <t>co2 med</t>
   </si>
   <si>
@@ -260,6 +257,9 @@
   </si>
   <si>
     <t>OM Costs</t>
+  </si>
+  <si>
+    <t>Synfuel CAPEX (M$)</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -456,6 +456,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -521,6 +522,209 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:numFmt formatCode="&quot;$&quot;#,##0" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="0">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr">
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>cases!$P$3:$P$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>10764062.343691755</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>47346.100903300001</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2778013.9205800002</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3125292.0733699999</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>80038945.415160388</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>cases!$P$3:$P$7</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>10764062.343691755</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>47346.100903300001</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2778013.9205800002</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3125292.0733699999</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>80038945.415160388</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>cases!$A$3:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Braidwood</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Prairie Island</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Davis Besse</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Cooper</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>South Texas Project</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>cases!$O$3:$O$7</c:f>
+              <c:numCache>
+                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>280889891.63999987</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>448235076.44599998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>238515675.85000014</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>363592802.25999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>699881946.74000025</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4686-1A4B-B59E-23C2982A3A10}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>cases!$Q$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Synfuel CAPEX (M$)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="&quot;$&quot;#,##0" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -578,149 +782,6 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:errBars>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>cases!$P$3:$P$7</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>10791773.621722151</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>112426.783738</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>1136859.4810800001</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>2014357.9649499999</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>81217687.647704601</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>cases!$P$3:$P$7</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
-                  <c:pt idx="0">
-                    <c:v>10791773.621722151</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>112426.783738</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>1136859.4810800001</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>2014357.9649499999</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>81217687.647704601</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:cat>
-            <c:strRef>
-              <c:f>cases!$A$3:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Braidwood</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Prairie Island</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Davis Besse</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Cooper</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>South Texas Project</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>cases!$O$3:$O$7</c:f>
-              <c:numCache>
-                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>988706502.11999989</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>797305235.92999995</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>748584278.82999992</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>800336972.89999986</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>886522516.21000004</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4686-1A4B-B59E-23C2982A3A10}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>cases!$Q$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>CAPEX (M$)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>cases!$A$3:$A$7</c:f>
@@ -751,19 +812,19 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>320071789.37109995</c:v>
+                  <c:v>839161044.90999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>178897818.0905</c:v>
+                  <c:v>572914401.57000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>262728958.7272</c:v>
+                  <c:v>398285924.56999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>247337409.04210001</c:v>
+                  <c:v>905276044.97000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>204617209.60839999</c:v>
+                  <c:v>650849884.57000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -894,7 +955,7 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:dispUnits>
-          <c:builtInUnit val="billions"/>
+          <c:builtInUnit val="millions"/>
           <c:dispUnitsLbl>
             <c:spPr>
               <a:noFill/>
@@ -3423,8 +3484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FE355D-8072-1247-9790-841EBA440D66}">
   <dimension ref="A1:AJ8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E7"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3508,61 +3569,61 @@
         <v>19</v>
       </c>
       <c r="Q2" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="R2" t="s">
-        <v>63</v>
-      </c>
-      <c r="T2" t="s">
+        <v>62</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" s="12" t="s">
         <v>56</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.2">
@@ -3576,10 +3637,10 @@
         <v>1175</v>
       </c>
       <c r="D3">
-        <v>10.1</v>
+        <v>2.5</v>
       </c>
       <c r="E3" s="3">
-        <v>51.2</v>
+        <v>12.7</v>
       </c>
       <c r="F3">
         <v>2102483898.8800001</v>
@@ -3591,94 +3652,94 @@
         <f>G3/F3</f>
         <v>4.9665897586956935E-3</v>
       </c>
-      <c r="I3" s="12">
-        <v>3091190401</v>
-      </c>
-      <c r="J3" s="12">
-        <v>2724584.22</v>
+      <c r="I3">
+        <v>2383373790.52</v>
+      </c>
+      <c r="J3">
+        <v>2612665.1925300001</v>
       </c>
       <c r="K3">
         <f>J3/I3</f>
-        <v>8.8140291168043133E-4</v>
+        <v>1.0962045495851382E-3</v>
       </c>
       <c r="L3">
         <f>I3-F3</f>
-        <v>988706502.11999989</v>
+        <v>280889891.63999987</v>
       </c>
       <c r="M3">
         <f>100*SQRT(POWER(K3,2)+POWER(H3,2))</f>
-        <v>0.50441931885981217</v>
+        <v>0.50861260548389964</v>
       </c>
       <c r="N3">
         <f>SQRT(POWER(J3,2)+POWER(G3,2))</f>
-        <v>10791773.621722151</v>
+        <v>10764062.343691755</v>
       </c>
       <c r="O3" s="1">
         <f>L3</f>
-        <v>988706502.11999989</v>
+        <v>280889891.63999987</v>
       </c>
       <c r="P3" s="1">
         <f>N3</f>
-        <v>10791773.621722151</v>
+        <v>10764062.343691755</v>
       </c>
       <c r="Q3" s="1">
         <f>ABS(X3+AC3+AB3)</f>
-        <v>320071789.37109995</v>
+        <v>839161044.90999997</v>
       </c>
       <c r="R3" s="1">
         <f>ABS(T3+Y3+Z3+AE3+AF3)</f>
-        <v>1374267486.8539767</v>
-      </c>
-      <c r="T3">
-        <v>-1.1539766655999999</v>
-      </c>
-      <c r="U3">
-        <v>784993059.20999897</v>
-      </c>
-      <c r="V3">
-        <v>12996245.300499899</v>
-      </c>
-      <c r="W3">
+        <v>1318857619</v>
+      </c>
+      <c r="T3" s="12">
+        <v>-159556675.40000001</v>
+      </c>
+      <c r="U3" s="12">
+        <v>67596719.530000001</v>
+      </c>
+      <c r="V3" s="12">
+        <v>2460801431</v>
+      </c>
+      <c r="W3" s="12">
         <v>-5860214.3420000002</v>
       </c>
-      <c r="X3">
-        <v>-299795112.39999998</v>
-      </c>
-      <c r="Y3">
+      <c r="X3" s="12">
+        <v>-64590994.810000002</v>
+      </c>
+      <c r="Y3" s="12">
         <v>-305989671.60000002</v>
       </c>
-      <c r="Z3">
-        <v>-107571298.56</v>
-      </c>
-      <c r="AA3">
-        <v>5462903274.6999998</v>
-      </c>
-      <c r="AB3">
-        <v>-19576500</v>
-      </c>
-      <c r="AC3">
-        <v>-700176.97109999997</v>
-      </c>
-      <c r="AD3">
-        <v>-462130996.799999</v>
-      </c>
-      <c r="AE3">
+      <c r="Z3" s="12">
+        <v>-107571299</v>
+      </c>
+      <c r="AA3" s="12">
+        <v>5320219258</v>
+      </c>
+      <c r="AB3" s="12">
+        <v>-6349175.0999999996</v>
+      </c>
+      <c r="AC3" s="12">
+        <v>-768220875</v>
+      </c>
+      <c r="AD3" s="12">
+        <v>-462130997</v>
+      </c>
+      <c r="AE3" s="12">
         <v>-501614080</v>
       </c>
-      <c r="AF3">
-        <v>-459092435.54000002</v>
-      </c>
-      <c r="AG3">
-        <v>1737621649.3599999</v>
-      </c>
-      <c r="AH3">
-        <v>676618806.59999895</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AJ3">
-        <v>-2923135525.0834198</v>
+      <c r="AF3" s="12">
+        <v>-244125893</v>
+      </c>
+      <c r="AG3" s="12">
+        <v>149628733</v>
+      </c>
+      <c r="AH3" s="12">
+        <v>58264473.700000003</v>
+      </c>
+      <c r="AI3" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ3" s="17">
+        <v>-3047000000</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.2">
@@ -3692,7 +3753,7 @@
         <v>507</v>
       </c>
       <c r="D4">
-        <v>10.1</v>
+        <v>2.5</v>
       </c>
       <c r="E4" s="3">
         <v>5.4</v>
@@ -3708,93 +3769,93 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>1059865693.28</v>
+        <v>710795533.796</v>
       </c>
       <c r="J4">
-        <v>112426.783738</v>
+        <v>47346.100903300001</v>
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K8" si="1">J4/I4</f>
-        <v>1.0607644388419561E-4</v>
+        <v>6.6610014627481383E-5</v>
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L8" si="2">I4-F4</f>
-        <v>797305235.92999995</v>
+        <v>448235076.44599998</v>
       </c>
       <c r="M4">
         <f t="shared" ref="M4:M8" si="3">100*SQRT(POWER(K4,2)+POWER(H4,2))</f>
-        <v>1.0607644388419562E-2</v>
+        <v>6.6610014627481381E-3</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N8" si="4">SQRT(POWER(J4,2)+POWER(G4,2))</f>
-        <v>112426.783738</v>
+        <v>47346.100903300001</v>
       </c>
       <c r="O4" s="1">
         <f t="shared" ref="O4:O8" si="5">L4</f>
-        <v>797305235.92999995</v>
+        <v>448235076.44599998</v>
       </c>
       <c r="P4" s="1">
         <f t="shared" ref="P4:P8" si="6">N4</f>
-        <v>112426.783738</v>
+        <v>47346.100903300001</v>
       </c>
       <c r="Q4" s="1">
         <f t="shared" ref="Q4:Q8" si="7">ABS(X4+AC4+AB4)</f>
-        <v>178897818.0905</v>
+        <v>572914401.57000005</v>
       </c>
       <c r="R4" s="1">
         <f t="shared" ref="R4:R8" si="8">ABS(T4+Y4+Z4+AE4+AF4)</f>
-        <v>836787255.16524041</v>
-      </c>
-      <c r="T4">
-        <v>-1.4202404037999901</v>
-      </c>
-      <c r="U4">
-        <v>394833167.79000002</v>
-      </c>
-      <c r="V4">
-        <v>7578786.5296510002</v>
-      </c>
-      <c r="W4">
-        <v>-5931802.1880000001</v>
-      </c>
-      <c r="X4">
-        <v>-175484359.5</v>
-      </c>
-      <c r="Y4">
-        <v>-309727613.60000002</v>
-      </c>
-      <c r="Z4">
-        <v>-108885379.76000001</v>
-      </c>
-      <c r="AA4">
-        <v>2385392346.99999</v>
-      </c>
-      <c r="AB4">
-        <v>-2689000</v>
-      </c>
-      <c r="AC4">
-        <v>-724458.59050000005</v>
-      </c>
-      <c r="AD4">
-        <v>-201840517.40000001</v>
-      </c>
-      <c r="AE4">
-        <v>-219085164.40000001</v>
-      </c>
-      <c r="AF4">
-        <v>-199089095.98500001</v>
-      </c>
-      <c r="AG4">
-        <v>720097787.05999899</v>
-      </c>
-      <c r="AH4">
-        <v>387046227.23000002</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ4">
-        <v>-1200560344.4958999</v>
+        <v>1116501293.3</v>
+      </c>
+      <c r="T4" s="12">
+        <v>-181941219.30000001</v>
+      </c>
+      <c r="U4" s="12">
+        <v>82505791.370000005</v>
+      </c>
+      <c r="V4" s="12">
+        <v>1317080775</v>
+      </c>
+      <c r="W4" s="12">
+        <v>-6062491.6279999996</v>
+      </c>
+      <c r="X4" s="12">
+        <v>-64117789.57</v>
+      </c>
+      <c r="Y4" s="12">
+        <v>-316551531</v>
+      </c>
+      <c r="Z4" s="12">
+        <v>-111284342</v>
+      </c>
+      <c r="AA4" s="12">
+        <v>3612255836</v>
+      </c>
+      <c r="AB4" s="12">
+        <v>-15827642</v>
+      </c>
+      <c r="AC4" s="12">
+        <v>-492968970</v>
+      </c>
+      <c r="AD4" s="12">
+        <v>-306786489</v>
+      </c>
+      <c r="AE4" s="12">
+        <v>-332997404</v>
+      </c>
+      <c r="AF4" s="12">
+        <v>-173726797</v>
+      </c>
+      <c r="AG4" s="12">
+        <v>158885300</v>
+      </c>
+      <c r="AH4" s="12">
+        <v>54169944.700000003</v>
+      </c>
+      <c r="AI4" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="AJ4" s="17">
+        <v>-1778000000</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.2">
@@ -3808,10 +3869,10 @@
         <v>879</v>
       </c>
       <c r="D5">
-        <v>10.1</v>
+        <v>2.5</v>
       </c>
       <c r="E5" s="13">
-        <v>30</v>
+        <v>24.1</v>
       </c>
       <c r="F5">
         <v>1765764570.5999999</v>
@@ -3824,93 +3885,93 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>2514348849.4299998</v>
+        <v>2004280246.45</v>
       </c>
       <c r="J5">
-        <v>1136859.4810800001</v>
+        <v>2778013.9205800002</v>
       </c>
       <c r="K5">
         <f t="shared" si="1"/>
-        <v>4.5214866717389868E-4</v>
+        <v>1.3860406624774378E-3</v>
       </c>
       <c r="L5">
         <f t="shared" si="2"/>
-        <v>748584278.82999992</v>
+        <v>238515675.85000014</v>
       </c>
       <c r="M5">
         <f t="shared" si="3"/>
-        <v>4.5214866717389869E-2</v>
+        <v>0.13860406624774377</v>
       </c>
       <c r="N5">
         <f t="shared" si="4"/>
-        <v>1136859.4810800001</v>
+        <v>2778013.9205800002</v>
       </c>
       <c r="O5" s="1">
         <f t="shared" si="5"/>
-        <v>748584278.82999992</v>
+        <v>238515675.85000014</v>
       </c>
       <c r="P5" s="1">
         <f t="shared" si="6"/>
-        <v>1136859.4810800001</v>
+        <v>2778013.9205800002</v>
       </c>
       <c r="Q5" s="1">
         <f t="shared" si="7"/>
-        <v>262728958.7272</v>
+        <v>398285924.56999999</v>
       </c>
       <c r="R5" s="1">
         <f t="shared" si="8"/>
-        <v>1270553097.7362475</v>
-      </c>
-      <c r="T5">
-        <v>-1.5862495952</v>
-      </c>
-      <c r="U5">
-        <v>764161074.72999895</v>
-      </c>
-      <c r="V5">
-        <v>1128230.1472700001</v>
-      </c>
-      <c r="W5">
-        <v>-6576092.7999999896</v>
-      </c>
-      <c r="X5">
-        <v>-249984024</v>
-      </c>
-      <c r="Y5">
-        <v>-343369091.799999</v>
-      </c>
-      <c r="Z5">
-        <v>-120712110.59999999</v>
-      </c>
-      <c r="AA5">
-        <v>4585937499.5</v>
-      </c>
-      <c r="AB5">
-        <v>-12037500</v>
-      </c>
-      <c r="AC5">
-        <v>-707434.72719999996</v>
-      </c>
-      <c r="AD5">
-        <v>-387945340.19999897</v>
-      </c>
-      <c r="AE5">
-        <v>-421090223.99999899</v>
-      </c>
-      <c r="AF5">
-        <v>-385381669.75</v>
-      </c>
-      <c r="AG5">
-        <v>1484027150.75</v>
-      </c>
-      <c r="AH5">
-        <v>806284329.05999994</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AJ5">
-        <v>-2591907699.1138201</v>
+        <v>954964898.20000005</v>
+      </c>
+      <c r="T5" s="12">
+        <v>-194078973.59999999</v>
+      </c>
+      <c r="U5" s="12">
+        <v>79052465.370000005</v>
+      </c>
+      <c r="V5" s="12">
+        <v>268199947.5</v>
+      </c>
+      <c r="W5" s="12">
+        <v>-5931802.1880000001</v>
+      </c>
+      <c r="X5" s="12">
+        <v>-64117789.57</v>
+      </c>
+      <c r="Y5" s="12">
+        <v>-309727613.60000002</v>
+      </c>
+      <c r="Z5" s="12">
+        <v>-108885380</v>
+      </c>
+      <c r="AA5" s="12">
+        <v>2381820594</v>
+      </c>
+      <c r="AB5" s="12">
+        <v>-2689000</v>
+      </c>
+      <c r="AC5" s="12">
+        <v>-331479135</v>
+      </c>
+      <c r="AD5" s="12">
+        <v>-201840517</v>
+      </c>
+      <c r="AE5" s="12">
+        <v>-219085164</v>
+      </c>
+      <c r="AF5" s="12">
+        <v>-123187767</v>
+      </c>
+      <c r="AG5" s="12">
+        <v>144176100</v>
+      </c>
+      <c r="AH5" s="12">
+        <v>77493385.799999997</v>
+      </c>
+      <c r="AI5" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ5" s="12">
+        <v>-678923816</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.2">
@@ -3924,10 +3985,10 @@
         <v>754</v>
       </c>
       <c r="D6">
-        <v>10.1</v>
+        <v>2.5</v>
       </c>
       <c r="E6" s="3">
-        <v>17.8</v>
+        <v>31.7</v>
       </c>
       <c r="F6">
         <v>1080996406.4100001</v>
@@ -3940,93 +4001,93 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>1881333379.3099999</v>
+        <v>1444589208.6700001</v>
       </c>
       <c r="J6">
-        <v>2014357.9649499999</v>
+        <v>3125292.0733699999</v>
       </c>
       <c r="K6">
         <f t="shared" si="1"/>
-        <v>1.0707076093492735E-3</v>
+        <v>2.1634469194515057E-3</v>
       </c>
       <c r="L6">
         <f t="shared" si="2"/>
-        <v>800336972.89999986</v>
+        <v>363592802.25999999</v>
       </c>
       <c r="M6">
         <f t="shared" si="3"/>
-        <v>0.10707076093492734</v>
+        <v>0.21634469194515057</v>
       </c>
       <c r="N6">
         <f t="shared" si="4"/>
-        <v>2014357.9649499999</v>
+        <v>3125292.0733699999</v>
       </c>
       <c r="O6" s="1">
         <f t="shared" si="5"/>
-        <v>800336972.89999986</v>
+        <v>363592802.25999999</v>
       </c>
       <c r="P6" s="1">
         <f t="shared" si="6"/>
-        <v>2014357.9649499999</v>
+        <v>3125292.0733699999</v>
       </c>
       <c r="Q6" s="1">
         <f t="shared" si="7"/>
-        <v>247337409.04210001</v>
+        <v>905276044.97000003</v>
       </c>
       <c r="R6" s="1">
         <f t="shared" si="8"/>
-        <v>1065590666.9014182</v>
-      </c>
-      <c r="T6">
-        <v>-1.3314181646000001</v>
-      </c>
-      <c r="U6">
-        <v>622093023.10000002</v>
-      </c>
-      <c r="V6">
-        <v>829231.42429</v>
-      </c>
-      <c r="W6">
-        <v>-6062491.6279999902</v>
-      </c>
-      <c r="X6">
-        <v>-227097690.40000001</v>
-      </c>
-      <c r="Y6">
-        <v>-316551531</v>
-      </c>
-      <c r="Z6">
-        <v>-111284341.95999999</v>
-      </c>
-      <c r="AA6">
-        <v>3626579180.9000001</v>
-      </c>
-      <c r="AB6">
-        <v>-19528000.02</v>
-      </c>
-      <c r="AC6">
-        <v>-711718.62210000004</v>
-      </c>
-      <c r="AD6">
-        <v>-306786488.99999899</v>
-      </c>
-      <c r="AE6">
-        <v>-332997404.39999998</v>
-      </c>
-      <c r="AF6">
-        <v>-304757388.20999998</v>
-      </c>
-      <c r="AG6">
-        <v>1197993900.8099999</v>
-      </c>
-      <c r="AH6">
-        <v>408440961.57999998</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ6">
-        <v>-1906103742.70277</v>
+        <v>1676410541</v>
+      </c>
+      <c r="T6" s="12">
+        <v>-318375700.19999999</v>
+      </c>
+      <c r="U6" s="12">
+        <v>97058773.25</v>
+      </c>
+      <c r="V6" s="12">
+        <v>4822640884</v>
+      </c>
+      <c r="W6" s="12">
+        <v>-6576092.7999999998</v>
+      </c>
+      <c r="X6" s="12">
+        <v>-64174373.969999999</v>
+      </c>
+      <c r="Y6" s="12">
+        <v>-343369091.80000001</v>
+      </c>
+      <c r="Z6" s="12">
+        <v>-120712111</v>
+      </c>
+      <c r="AA6" s="12">
+        <v>6430992992</v>
+      </c>
+      <c r="AB6" s="12">
+        <v>-21915670</v>
+      </c>
+      <c r="AC6" s="12">
+        <v>-819186001</v>
+      </c>
+      <c r="AD6" s="12">
+        <v>-552988308</v>
+      </c>
+      <c r="AE6" s="12">
+        <v>-600233967</v>
+      </c>
+      <c r="AF6" s="12">
+        <v>-293719671</v>
+      </c>
+      <c r="AG6" s="12">
+        <v>178756070</v>
+      </c>
+      <c r="AH6" s="12">
+        <v>55536235.799999997</v>
+      </c>
+      <c r="AI6" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ6" s="17">
+        <v>-5023000000</v>
       </c>
     </row>
     <row r="7" spans="1:36" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4037,13 +4098,13 @@
         <v>1280</v>
       </c>
       <c r="C7" s="4">
-        <v>1042</v>
+        <v>1252</v>
       </c>
       <c r="D7" s="4">
-        <v>10.1</v>
+        <v>2.5</v>
       </c>
       <c r="E7" s="5">
-        <v>76.400000000000006</v>
+        <v>43.8</v>
       </c>
       <c r="F7">
         <v>2721027335.4499998</v>
@@ -4056,93 +4117,93 @@
         <v>2.7969213517920744E-2</v>
       </c>
       <c r="I7">
-        <v>3607549851.6599998</v>
+        <v>3420909282.1900001</v>
       </c>
       <c r="J7">
-        <v>28360934.292199999</v>
+        <v>24784321.460499998</v>
       </c>
       <c r="K7">
         <f t="shared" si="1"/>
-        <v>7.8615502095278952E-3</v>
+        <v>7.2449513904190863E-3</v>
       </c>
       <c r="L7">
         <f t="shared" si="2"/>
-        <v>886522516.21000004</v>
+        <v>699881946.74000025</v>
       </c>
       <c r="M7">
         <f t="shared" si="3"/>
-        <v>2.90530700014296</v>
+        <v>2.8892321219669697</v>
       </c>
       <c r="N7">
         <f t="shared" si="4"/>
-        <v>81217687.647704601</v>
+        <v>80038945.415160388</v>
       </c>
       <c r="O7" s="1">
         <f t="shared" si="5"/>
-        <v>886522516.21000004</v>
+        <v>699881946.74000025</v>
       </c>
       <c r="P7" s="1">
         <f t="shared" si="6"/>
-        <v>81217687.647704601</v>
+        <v>80038945.415160388</v>
       </c>
       <c r="Q7" s="1">
         <f t="shared" si="7"/>
-        <v>204617209.60839999</v>
+        <v>650849884.57000005</v>
       </c>
       <c r="R7" s="1">
         <f t="shared" si="8"/>
-        <v>1436174702.5125432</v>
-      </c>
-      <c r="T7">
-        <v>-2.326544218</v>
-      </c>
-      <c r="U7">
-        <v>391253658.669999</v>
-      </c>
-      <c r="V7">
-        <v>3834753586.0289998</v>
-      </c>
-      <c r="W7">
-        <v>-6576092.7999999896</v>
-      </c>
-      <c r="X7">
-        <v>-153587835</v>
-      </c>
-      <c r="Y7">
-        <v>-343369091.799999</v>
-      </c>
-      <c r="Z7">
-        <v>-120712110.59999999</v>
-      </c>
-      <c r="AA7">
-        <v>6507684200.6000004</v>
-      </c>
-      <c r="AB7">
-        <v>-50330880.950000003</v>
-      </c>
-      <c r="AC7">
-        <v>-698493.65839999996</v>
-      </c>
-      <c r="AD7">
-        <v>-558305865.19999897</v>
-      </c>
-      <c r="AE7">
-        <v>-606005840</v>
-      </c>
-      <c r="AF7">
-        <v>-366087657.78600001</v>
-      </c>
-      <c r="AG7">
-        <v>720583663.12</v>
-      </c>
-      <c r="AH7">
-        <v>223872134.73199999</v>
-      </c>
-      <c r="AI7" t="s">
+        <v>1312805569.4000001</v>
+      </c>
+      <c r="T7" s="12">
+        <v>-216764494.59999999</v>
+      </c>
+      <c r="U7" s="12">
+        <v>86936338.530000001</v>
+      </c>
+      <c r="V7" s="12">
+        <v>2025170723</v>
+      </c>
+      <c r="W7" s="12">
+        <v>-6576092.7999999998</v>
+      </c>
+      <c r="X7" s="12">
+        <v>-64117789.57</v>
+      </c>
+      <c r="Y7" s="12">
+        <v>-343369091.80000001</v>
+      </c>
+      <c r="Z7" s="12">
+        <v>-120712111</v>
+      </c>
+      <c r="AA7" s="12">
+        <v>4468067921</v>
+      </c>
+      <c r="AB7" s="12">
+        <v>-12037500</v>
+      </c>
+      <c r="AC7" s="12">
+        <v>-574694595</v>
+      </c>
+      <c r="AD7" s="12">
+        <v>-387945340</v>
+      </c>
+      <c r="AE7" s="12">
+        <v>-421090224</v>
+      </c>
+      <c r="AF7" s="12">
+        <v>-210869648</v>
+      </c>
+      <c r="AG7" s="12">
+        <v>168833369</v>
+      </c>
+      <c r="AH7" s="12">
+        <v>91728575.099999994</v>
+      </c>
+      <c r="AI7" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="AJ7">
-        <v>-5001440731.5800505</v>
+      <c r="AJ7" s="17">
+        <v>-2478000000</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.2">
@@ -4223,7 +4284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBA1661-1357-8E4D-8878-EEFCBAD9628D}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
@@ -4422,7 +4483,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8">
         <v>2995792962.5500002</v>
@@ -4449,7 +4510,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B9">
         <v>2899454146</v>
@@ -4476,7 +4537,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10">
         <v>3228258109.6900001</v>
@@ -4503,7 +4564,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B11">
         <v>2954602048.9699998</v>
@@ -4533,21 +4594,21 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" t="s">
         <v>64</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>65</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>66</v>
-      </c>
-      <c r="E13" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14">
         <f>E4</f>
@@ -4568,7 +4629,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B15">
         <f>E6</f>
@@ -4589,7 +4650,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16">
         <f>E8</f>
@@ -4610,7 +4671,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B17">
         <f>E10</f>

</xml_diff>

<commit_message>
Latest results locations + braidwood SA
</commit_message>
<xml_diff>
--- a/use_cases/IES_Feb23/run/results.xlsx
+++ b/use_cases/IES_Feb23/run/results.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/IES_Feb23/run/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2FAD37-E4CB-B046-B8AB-7613C0540301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB11A45-FBFA-F249-B550-04FD1B0849CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20200" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
+    <workbookView xWindow="36140" yWindow="2000" windowWidth="35840" windowHeight="20200" activeTab="2" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
-    <sheet name="braidwood_SA" sheetId="2" r:id="rId2"/>
-    <sheet name="covid" sheetId="3" r:id="rId3"/>
+    <sheet name="data" sheetId="4" r:id="rId2"/>
+    <sheet name="braidwood_SA" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="95">
   <si>
     <t>Location</t>
   </si>
@@ -52,18 +52,6 @@
     <t>Delta NPV</t>
   </si>
   <si>
-    <t>Braidwood</t>
-  </si>
-  <si>
-    <t>Prairie Island</t>
-  </si>
-  <si>
-    <t>Davis Besse</t>
-  </si>
-  <si>
-    <t>Cooper</t>
-  </si>
-  <si>
     <t>Std baseline NPV</t>
   </si>
   <si>
@@ -85,15 +73,9 @@
     <t>HTSE (MWe)</t>
   </si>
   <si>
-    <t>FT (ton-H2)</t>
-  </si>
-  <si>
     <t>H2 storage (ton-H2)</t>
   </si>
   <si>
-    <t>South Texas Project</t>
-  </si>
-  <si>
     <t>Delta NPV (M$)</t>
   </si>
   <si>
@@ -103,12 +85,6 @@
     <t>Std Delta NPV</t>
   </si>
   <si>
-    <t>Components</t>
-  </si>
-  <si>
-    <t>Houston</t>
-  </si>
-  <si>
     <t>Case</t>
   </si>
   <si>
@@ -127,87 +103,6 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>synfuel low</t>
-  </si>
-  <si>
-    <t>synfuel high</t>
-  </si>
-  <si>
-    <t>capex low</t>
-  </si>
-  <si>
-    <t>capex high</t>
-  </si>
-  <si>
-    <t>baseline</t>
-  </si>
-  <si>
-    <t>reference</t>
-  </si>
-  <si>
-    <t>no covid baseline</t>
-  </si>
-  <si>
-    <t>no covid</t>
-  </si>
-  <si>
-    <t>co2 med</t>
-  </si>
-  <si>
-    <t>co2 high</t>
-  </si>
-  <si>
-    <t>co2_shipping</t>
-  </si>
-  <si>
-    <t>diesel_sales</t>
-  </si>
-  <si>
-    <t>e_sales</t>
-  </si>
-  <si>
-    <t>elec_cap_market</t>
-  </si>
-  <si>
-    <t>ft_capex</t>
-  </si>
-  <si>
-    <t>ft_fom</t>
-  </si>
-  <si>
-    <t>ft_vom</t>
-  </si>
-  <si>
-    <t>h2_ptc</t>
-  </si>
-  <si>
-    <t>h2_storage_capex</t>
-  </si>
-  <si>
-    <t>htse_capex</t>
-  </si>
-  <si>
-    <t>htse_elec_cap_market</t>
-  </si>
-  <si>
-    <t>htse_fom</t>
-  </si>
-  <si>
-    <t>htse_vom</t>
-  </si>
-  <si>
-    <t>jet_fuel_sales</t>
-  </si>
-  <si>
-    <t>naphtha_sales</t>
-  </si>
-  <si>
-    <t>plant</t>
-  </si>
-  <si>
-    <t>taxes</t>
-  </si>
-  <si>
     <t>braidwood</t>
   </si>
   <si>
@@ -223,9 +118,6 @@
     <t>davis_besse</t>
   </si>
   <si>
-    <t>OM (M$)</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -247,25 +139,190 @@
     <t>CO2 Cost</t>
   </si>
   <si>
-    <t>om low</t>
-  </si>
-  <si>
-    <t>om high</t>
-  </si>
-  <si>
-    <t>OM Costs</t>
-  </si>
-  <si>
-    <t>Synfuel CAPEX (M$)</t>
-  </si>
-  <si>
-    <t>ROI</t>
-  </si>
-  <si>
-    <t>ROI II</t>
-  </si>
-  <si>
     <t>BAU</t>
+  </si>
+  <si>
+    <t>HTSE</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>kWh/kg-H2</t>
+  </si>
+  <si>
+    <t>Outputs</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>kg-H2/kWh</t>
+  </si>
+  <si>
+    <t>kg-H2/MWh</t>
+  </si>
+  <si>
+    <t>ton-h2/MWh</t>
+  </si>
+  <si>
+    <t>FT (ton-H2/h)</t>
+  </si>
+  <si>
+    <t>HTSE (ton-H2/h)</t>
+  </si>
+  <si>
+    <t>Components Capacities</t>
+  </si>
+  <si>
+    <t>npp_capacity</t>
+  </si>
+  <si>
+    <t>htse_capacity</t>
+  </si>
+  <si>
+    <t>ft_capacity</t>
+  </si>
+  <si>
+    <t>ft_elec_consumption_capacity</t>
+  </si>
+  <si>
+    <t>electricity_market_capacity</t>
+  </si>
+  <si>
+    <t>naphtha_market_capacity</t>
+  </si>
+  <si>
+    <t>jet_fuel_market_capacity</t>
+  </si>
+  <si>
+    <t>diesel_market_capacity</t>
+  </si>
+  <si>
+    <t>h2_storage_capacity</t>
+  </si>
+  <si>
+    <t>scenario_label</t>
+  </si>
+  <si>
+    <t>location_label</t>
+  </si>
+  <si>
+    <t>fuel_region_label</t>
+  </si>
+  <si>
+    <t>elec_data_label</t>
+  </si>
+  <si>
+    <t>mean_NPV</t>
+  </si>
+  <si>
+    <t>std_NPV</t>
+  </si>
+  <si>
+    <t>med_NPV</t>
+  </si>
+  <si>
+    <t>max_NPV</t>
+  </si>
+  <si>
+    <t>min_NPV</t>
+  </si>
+  <si>
+    <t>perc_5_NPV</t>
+  </si>
+  <si>
+    <t>perc_95_NPV</t>
+  </si>
+  <si>
+    <t>samp_NPV</t>
+  </si>
+  <si>
+    <t>var_NPV</t>
+  </si>
+  <si>
+    <t>prefix</t>
+  </si>
+  <si>
+    <t>ProbabilityWeight-ft_capacity</t>
+  </si>
+  <si>
+    <t>ProbabilityWeight</t>
+  </si>
+  <si>
+    <t>ProbabilityWeight-h2_storage_capacity</t>
+  </si>
+  <si>
+    <t>ProbabilityWeight-htse_capacity</t>
+  </si>
+  <si>
+    <t>PointProbability</t>
+  </si>
+  <si>
+    <t>ref</t>
+  </si>
+  <si>
+    <t>illinois</t>
+  </si>
+  <si>
+    <t>covid</t>
+  </si>
+  <si>
+    <t>nebraska</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>davis-besse</t>
+  </si>
+  <si>
+    <t>ohio</t>
+  </si>
+  <si>
+    <t>prairie-island</t>
+  </si>
+  <si>
+    <t>minnesota</t>
+  </si>
+  <si>
+    <t>south_texas_project</t>
+  </si>
+  <si>
+    <t>west_south_central</t>
+  </si>
+  <si>
+    <t>Storage/HTSE(day) ratio</t>
+  </si>
+  <si>
+    <t>synfuel 0.75</t>
+  </si>
+  <si>
+    <t>synfuel 1.25</t>
+  </si>
+  <si>
+    <t>capex 0.75</t>
+  </si>
+  <si>
+    <t>capex 1.25</t>
+  </si>
+  <si>
+    <t>co2 cost med</t>
+  </si>
+  <si>
+    <t>co2 cost high</t>
+  </si>
+  <si>
+    <t>co2 tax med</t>
+  </si>
+  <si>
+    <t>co2 tax high</t>
+  </si>
+  <si>
+    <t>CO2 Tax</t>
   </si>
 </sst>
 </file>
@@ -308,128 +365,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -438,32 +379,24 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -497,11 +430,41 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="col"/>
+        <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -509,7 +472,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>cases!$O$2</c:f>
+              <c:f>cases!$Q$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -538,13 +501,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="0">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
-                <a:pPr algn="ctr">
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -593,48 +556,48 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>cases!$P$3:$P$7</c:f>
+                <c:f>cases!$R$3:$R$8</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
+                  <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>10764062.343691755</c:v>
+                    <c:v>10442175.071948605</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>47346.100903300001</c:v>
+                    <c:v>6952.2878666099996</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2778013.9205800002</c:v>
+                    <c:v>1077.46392866</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3125292.0733699999</c:v>
+                    <c:v>45333.174797</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>80038945.415160388</c:v>
+                    <c:v>78308930.708383322</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>cases!$P$3:$P$7</c:f>
+                <c:f>cases!$R$3:$R$8</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="5"/>
+                  <c:ptCount val="6"/>
                   <c:pt idx="0">
-                    <c:v>10764062.343691755</c:v>
+                    <c:v>10442175.071948605</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>47346.100903300001</c:v>
+                    <c:v>6952.2878666099996</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2778013.9205800002</c:v>
+                    <c:v>1077.46392866</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>3125292.0733699999</c:v>
+                    <c:v>45333.174797</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>80038945.415160388</c:v>
+                    <c:v>78308930.708383322</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -659,155 +622,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Braidwood</c:v>
+                  <c:v>BRAIDWOOD</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Prairie Island</c:v>
+                  <c:v>COOPER</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Davis Besse</c:v>
+                  <c:v>DAVIS-BESSE</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Cooper</c:v>
+                  <c:v>PRAIRIE-ISLAND</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>South Texas Project</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>cases!$O$3:$O$7</c:f>
-              <c:numCache>
-                <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>280889891.63999987</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>448235076.44599998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>238515675.85000014</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>363592802.25999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>699881946.74000025</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4686-1A4B-B59E-23C2982A3A10}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>cases!$Q$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Synfuel CAPEX (M$)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:numFmt formatCode="&quot;$&quot;#,##0" sourceLinked="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="outEnd"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>cases!$A$3:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>Braidwood</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Prairie Island</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Davis Besse</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Cooper</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>South Texas Project</c:v>
+                  <c:v>STP</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -819,49 +646,49 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>839161044.90999997</c:v>
+                  <c:v>1305897263.1300001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>572914401.57000005</c:v>
+                  <c:v>1678864838.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>398285924.56999999</c:v>
+                  <c:v>591488449.03000021</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>905276044.97000003</c:v>
+                  <c:v>96082313.309999943</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>650849884.57000005</c:v>
+                  <c:v>159634546.57000017</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4686-1A4B-B59E-23C2982A3A10}"/>
+              <c16:uniqueId val="{00000000-F3B8-794E-A7DC-932C02F6F780}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1218972784"/>
-        <c:axId val="1218974432"/>
+        <c:gapWidth val="182"/>
+        <c:axId val="2124376752"/>
+        <c:axId val="2124379024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1218972784"/>
+        <c:axId val="2124376752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -884,7 +711,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -899,7 +726,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1218974432"/>
+        <c:crossAx val="2124379024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -907,12 +734,13 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1218974432"/>
+        <c:axId val="2124379024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2000000000"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -943,7 +771,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -958,9 +786,10 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1218972784"/>
+        <c:crossAx val="2124376752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="250000000"/>
         <c:dispUnits>
           <c:builtInUnit val="millions"/>
           <c:dispUnitsLbl>
@@ -972,11 +801,11 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1002,37 +831,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1139,7 +937,7 @@
                   <c:v>CO2 Cost</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>OM Costs</c:v>
+                  <c:v>CO2 Tax</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1151,16 +949,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>292440602.25999975</c:v>
+                  <c:v>972150087.25999975</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>496834954.11999989</c:v>
+                  <c:v>1535805647.1199999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>259304090.15999985</c:v>
+                  <c:v>895252871.1500001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>413681907.0999999</c:v>
+                  <c:v>1716541594.1199999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1210,7 +1008,7 @@
                   <c:v>CO2 Cost</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>OM Costs</c:v>
+                  <c:v>CO2 Tax</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1222,16 +1020,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>277077142.11999989</c:v>
+                  <c:v>1639644093.5799999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64562824.119999886</c:v>
+                  <c:v>1075988715.1199999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>227573043.11999989</c:v>
+                  <c:v>484607417.11999989</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>146688504.73000002</c:v>
+                  <c:v>2127187000.4899998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1297,7 +1095,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1796024143"/>
-        <c:crossesAt val="280889892"/>
+        <c:crossesAt val="1305897263"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1307,7 +1105,6 @@
         <c:axId val="1796024143"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="50000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="t"/>
@@ -1359,6 +1156,7 @@
         <c:crossAx val="414221104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="200000000"/>
         <c:dispUnits>
           <c:builtInUnit val="millions"/>
           <c:dispUnitsLbl>
@@ -1523,7 +1321,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1727,22 +1525,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1847,8 +1646,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1980,19 +1779,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2534,23 +2334,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>755650</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>901700</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D9C13AF-5416-55C3-3682-46E9E1BCA5D9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B791DDA-9A7C-F0A4-11B7-20F0EC0741F3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2576,15 +2376,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>774700</xdr:colOff>
+      <xdr:colOff>406400</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2966,7 +2766,7 @@
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>low</a:t>
+            <a:t>x0.75</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200"/>
@@ -2978,7 +2778,7 @@
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>high</a:t>
+            <a:t>x1.25</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200"/>
@@ -3041,7 +2841,7 @@
                 <a:srgbClr val="C00000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> Ref. Δ(NPV) = $M 280.9</a:t>
+            <a:t> Ref. Δ(NPV) = $bn 1.306</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1400" b="1">
             <a:solidFill>
@@ -3054,19 +2854,19 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0</cdr:x>
-      <cdr:y>0.84024</cdr:y>
+      <cdr:x>0.02051</cdr:x>
+      <cdr:y>0.84537</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.11487</cdr:x>
+      <cdr:x>0.1047</cdr:x>
       <cdr:y>0.91953</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
-        <cdr:cNvPr id="8" name="TextBox 1">
+        <cdr:cNvPr id="7" name="TextBox 1">
           <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BB6F14E-B88B-D129-C5D6-6CC3C9D66D90}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D30689B-9DF2-BBC6-DA64-945EE317525F}"/>
             </a:ext>
           </a:extLst>
         </cdr:cNvPr>
@@ -3074,8 +2874,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="0" y="4508500"/>
-          <a:ext cx="1422378" cy="425450"/>
+          <a:off x="254000" y="4536026"/>
+          <a:ext cx="1042482" cy="397924"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -3160,7 +2960,7 @@
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>x0.75</a:t>
+            <a:t>30</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200"/>
@@ -3172,7 +2972,7 @@
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>x1.25</a:t>
+            <a:t>60</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200"/>
@@ -3180,7 +2980,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200" baseline="0"/>
-            <a:t> (FT+HTSE+H2 sto.)</a:t>
+            <a:t> $/ton</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200"/>
         </a:p>
@@ -3487,852 +3287,678 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FE355D-8072-1247-9790-841EBA440D66}">
-  <dimension ref="A1:AL8"/>
+  <dimension ref="A1:AN16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="R36" sqref="R36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="11.83203125" customWidth="1"/>
-    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.6640625" customWidth="1"/>
-    <col min="16" max="16" width="23.33203125" customWidth="1"/>
-    <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.83203125" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" customWidth="1"/>
+    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.6640625" customWidth="1"/>
+    <col min="18" max="18" width="23.33203125" customWidth="1"/>
+    <col min="19" max="19" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="18"/>
+    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="9"/>
     </row>
-    <row r="2" spans="1:38" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>72</v>
-      </c>
-      <c r="R2" t="s">
-        <v>61</v>
-      </c>
-      <c r="S2" t="s">
-        <v>73</v>
-      </c>
-      <c r="T2" t="s">
-        <v>74</v>
-      </c>
-      <c r="V2" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="W2" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="X2" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="Y2" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="AA2" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB2" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC2" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="AD2" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE2" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF2" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="AG2" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="AH2" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI2" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="AJ2" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="AK2" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="AL2" s="12" t="s">
-        <v>55</v>
-      </c>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
+      <c r="AA2" s="3"/>
+      <c r="AB2" s="3"/>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
+      <c r="AG2" s="3"/>
+      <c r="AH2" s="3"/>
+      <c r="AI2" s="3"/>
+      <c r="AJ2" s="3"/>
+      <c r="AK2" s="3"/>
+      <c r="AL2" s="3"/>
+      <c r="AM2" s="3"/>
+      <c r="AN2" s="3"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="str">
+        <f>UPPER(data!A2)</f>
+        <v>BRAIDWOOD</v>
+      </c>
+      <c r="B3" s="7">
+        <f>data!C2</f>
         <v>1193</v>
       </c>
-      <c r="C3">
-        <v>1175</v>
-      </c>
-      <c r="D3">
-        <v>2.5</v>
-      </c>
-      <c r="E3" s="3">
-        <v>12.7</v>
-      </c>
-      <c r="F3">
+      <c r="C3" s="7">
+        <f>data!D2</f>
+        <v>-1178</v>
+      </c>
+      <c r="D3" s="10">
+        <f>ABS(C3)*$B$16</f>
+        <v>29.597989949748744</v>
+      </c>
+      <c r="E3" s="10">
+        <f>ABS(data!E2/1000)</f>
+        <v>29.60314</v>
+      </c>
+      <c r="F3" s="12">
+        <f>data!K2/1000</f>
+        <v>0.01</v>
+      </c>
+      <c r="G3" s="6">
+        <f>F3/(24*D3)</f>
+        <v>1.4077532541029996E-5</v>
+      </c>
+      <c r="H3">
         <v>2102483898.8800001</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>10442175</v>
       </c>
-      <c r="H3">
-        <f>G3/F3</f>
+      <c r="J3">
+        <f>I3/H3</f>
         <v>4.9665897586956935E-3</v>
       </c>
-      <c r="I3">
-        <v>2383373790.52</v>
-      </c>
-      <c r="J3">
-        <v>2612665.1925300001</v>
-      </c>
       <c r="K3">
-        <f>J3/I3</f>
-        <v>1.0962045495851382E-3</v>
+        <f>data!P2</f>
+        <v>3408381162.0100002</v>
       </c>
       <c r="L3">
-        <f>I3-F3</f>
-        <v>280889891.63999987</v>
+        <f>data!Q2</f>
+        <v>1225.80578418</v>
       </c>
       <c r="M3">
-        <f>100*SQRT(POWER(K3,2)+POWER(H3,2))</f>
-        <v>0.50861260548389964</v>
+        <f>L3/K3</f>
+        <v>3.5964457198710559E-7</v>
       </c>
       <c r="N3">
-        <f>SQRT(POWER(J3,2)+POWER(G3,2))</f>
-        <v>10764062.343691755</v>
-      </c>
-      <c r="O3" s="1">
-        <f>L3</f>
-        <v>280889891.63999987</v>
-      </c>
-      <c r="P3" s="1">
+        <f>K3-H3</f>
+        <v>1305897263.1300001</v>
+      </c>
+      <c r="O3">
+        <f>100*SQRT(POWER(M3,2)+POWER(J3,2))</f>
+        <v>0.49665897717171253</v>
+      </c>
+      <c r="P3">
+        <f>SQRT(POWER(L3,2)+POWER(I3,2))</f>
+        <v>10442175.071948605</v>
+      </c>
+      <c r="Q3" s="1">
         <f>N3</f>
-        <v>10764062.343691755</v>
-      </c>
-      <c r="Q3" s="1">
-        <f>ABS(Z3+AE3+AD3)</f>
-        <v>839161044.90999997</v>
+        <v>1305897263.1300001</v>
       </c>
       <c r="R3" s="1">
-        <f>ABS(V3+AA3+AB3+AG3+AH3)</f>
-        <v>1318857619</v>
-      </c>
-      <c r="S3" s="15">
-        <f>(I3-Q3)/Q3</f>
-        <v>1.8401864040002203</v>
-      </c>
-      <c r="T3" s="15">
-        <f>(L3-Q3)/Q3</f>
-        <v>-0.66527296119885393</v>
-      </c>
-      <c r="V3" s="12">
-        <v>-159556675.40000001</v>
-      </c>
-      <c r="W3" s="12">
-        <v>67596719.530000001</v>
-      </c>
-      <c r="X3" s="12">
-        <v>2460801431</v>
-      </c>
-      <c r="Y3" s="12">
-        <v>-5860214.3420000002</v>
-      </c>
-      <c r="Z3" s="12">
-        <v>-64590994.810000002</v>
-      </c>
-      <c r="AA3" s="12">
-        <v>-305989671.60000002</v>
-      </c>
-      <c r="AB3" s="12">
-        <v>-107571299</v>
-      </c>
-      <c r="AC3" s="12">
-        <v>5320219258</v>
-      </c>
-      <c r="AD3" s="12">
-        <v>-6349175.0999999996</v>
-      </c>
-      <c r="AE3" s="12">
-        <v>-768220875</v>
-      </c>
-      <c r="AF3" s="12">
-        <v>-462130997</v>
-      </c>
-      <c r="AG3" s="12">
-        <v>-501614080</v>
-      </c>
-      <c r="AH3" s="12">
-        <v>-244125893</v>
-      </c>
-      <c r="AI3" s="12">
-        <v>149628733</v>
-      </c>
-      <c r="AJ3" s="12">
-        <v>58264473.700000003</v>
-      </c>
-      <c r="AK3" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="AL3" s="12">
-        <v>-3047000000</v>
-      </c>
+        <f>P3</f>
+        <v>10442175.071948605</v>
+      </c>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3"/>
+      <c r="AH3" s="3"/>
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="3"/>
+      <c r="AK3" s="3"/>
+      <c r="AL3" s="3"/>
+      <c r="AM3" s="3"/>
+      <c r="AN3" s="3"/>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>522</v>
-      </c>
-      <c r="C4">
-        <v>507</v>
-      </c>
-      <c r="D4">
-        <v>2.5</v>
-      </c>
-      <c r="E4" s="3">
-        <v>5.4</v>
-      </c>
-      <c r="F4">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="str">
+        <f>UPPER(data!A3)</f>
+        <v>COOPER</v>
+      </c>
+      <c r="B4" s="7">
+        <f>data!C3</f>
+        <v>769</v>
+      </c>
+      <c r="C4" s="7">
+        <f>data!D3</f>
+        <v>-754</v>
+      </c>
+      <c r="D4" s="10">
+        <f t="shared" ref="D4:D7" si="0">ABS(C4)*$B$16</f>
+        <v>18.944723618090453</v>
+      </c>
+      <c r="E4" s="10">
+        <f>ABS(data!E3/1000)</f>
+        <v>18.948</v>
+      </c>
+      <c r="F4" s="12">
+        <f>data!K3/1000</f>
+        <v>0.01</v>
+      </c>
+      <c r="G4" s="6">
+        <f t="shared" ref="G4:G7" si="1">F4/(24*D4)</f>
+        <v>2.1993810786914232E-5</v>
+      </c>
+      <c r="H4">
         <v>262560457.34999999</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>0</v>
       </c>
-      <c r="H4">
-        <f t="shared" ref="H4:H8" si="0">G4/F4</f>
+      <c r="J4">
+        <f t="shared" ref="J4:J7" si="2">I4/H4</f>
         <v>0</v>
       </c>
-      <c r="I4">
-        <v>710795533.796</v>
-      </c>
-      <c r="J4">
-        <v>47346.100903300001</v>
-      </c>
       <c r="K4">
-        <f t="shared" ref="K4:K8" si="1">J4/I4</f>
-        <v>6.6610014627481383E-5</v>
+        <f>data!P3</f>
+        <v>1941425295.5999999</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L8" si="2">I4-F4</f>
-        <v>448235076.44599998</v>
+        <f>data!Q3</f>
+        <v>6952.2878666099996</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M8" si="3">100*SQRT(POWER(K4,2)+POWER(H4,2))</f>
-        <v>6.6610014627481381E-3</v>
+        <f t="shared" ref="M4:M7" si="3">L4/K4</f>
+        <v>3.5810226035307666E-6</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N8" si="4">SQRT(POWER(J4,2)+POWER(G4,2))</f>
-        <v>47346.100903300001</v>
-      </c>
-      <c r="O4" s="1">
-        <f t="shared" ref="O4:O8" si="5">L4</f>
-        <v>448235076.44599998</v>
-      </c>
-      <c r="P4" s="1">
-        <f t="shared" ref="P4:P8" si="6">N4</f>
-        <v>47346.100903300001</v>
+        <f t="shared" ref="N4:N7" si="4">K4-H4</f>
+        <v>1678864838.25</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O7" si="5">100*SQRT(POWER(M4,2)+POWER(J4,2))</f>
+        <v>3.5810226035307667E-4</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P7" si="6">SQRT(POWER(L4,2)+POWER(I4,2))</f>
+        <v>6952.2878666099996</v>
       </c>
       <c r="Q4" s="1">
-        <f t="shared" ref="Q4:Q8" si="7">ABS(Z4+AE4+AD4)</f>
-        <v>572914401.57000005</v>
+        <f t="shared" ref="Q4:Q7" si="7">N4</f>
+        <v>1678864838.25</v>
       </c>
       <c r="R4" s="1">
-        <f t="shared" ref="R4:R8" si="8">ABS(V4+AA4+AB4+AG4+AH4)</f>
-        <v>1116501293.3</v>
-      </c>
-      <c r="S4" s="15">
-        <f t="shared" ref="S4:S8" si="9">(I4-Q4)/Q4</f>
-        <v>0.24066620047978199</v>
-      </c>
-      <c r="T4" s="15">
-        <f t="shared" ref="T4:T8" si="10">(L4-Q4)/Q4</f>
-        <v>-0.21762295516107122</v>
-      </c>
-      <c r="V4" s="12">
-        <v>-181941219.30000001</v>
-      </c>
-      <c r="W4" s="12">
-        <v>82505791.370000005</v>
-      </c>
-      <c r="X4" s="12">
-        <v>1317080775</v>
-      </c>
-      <c r="Y4" s="12">
-        <v>-6062491.6279999996</v>
-      </c>
-      <c r="Z4" s="12">
-        <v>-64117789.57</v>
-      </c>
-      <c r="AA4" s="12">
-        <v>-316551531</v>
-      </c>
-      <c r="AB4" s="12">
-        <v>-111284342</v>
-      </c>
-      <c r="AC4" s="12">
-        <v>3612255836</v>
-      </c>
-      <c r="AD4" s="12">
-        <v>-15827642</v>
-      </c>
-      <c r="AE4" s="12">
-        <v>-492968970</v>
-      </c>
-      <c r="AF4" s="12">
-        <v>-306786489</v>
-      </c>
-      <c r="AG4" s="12">
-        <v>-332997404</v>
-      </c>
-      <c r="AH4" s="12">
-        <v>-173726797</v>
-      </c>
-      <c r="AI4" s="12">
-        <v>158885300</v>
-      </c>
-      <c r="AJ4" s="12">
-        <v>54169944.700000003</v>
-      </c>
-      <c r="AK4" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="AL4" s="12">
-        <v>-1778000000</v>
-      </c>
+        <f t="shared" ref="R4:R7" si="8">P4</f>
+        <v>6952.2878666099996</v>
+      </c>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3"/>
+      <c r="AB4" s="3"/>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="3"/>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="3"/>
+      <c r="AJ4" s="3"/>
+      <c r="AK4" s="3"/>
+      <c r="AL4" s="3"/>
+      <c r="AM4" s="3"/>
+      <c r="AN4" s="3"/>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="str">
+        <f>UPPER(data!A4)</f>
+        <v>DAVIS-BESSE</v>
+      </c>
+      <c r="B5" s="7">
+        <f>data!C4</f>
         <v>894</v>
       </c>
-      <c r="C5">
-        <v>879</v>
-      </c>
-      <c r="D5">
-        <v>2.5</v>
-      </c>
-      <c r="E5" s="13">
-        <v>24.1</v>
-      </c>
-      <c r="F5">
+      <c r="C5" s="7">
+        <f>data!D4</f>
+        <v>-879</v>
+      </c>
+      <c r="D5" s="10">
+        <f t="shared" si="0"/>
+        <v>22.085427135678394</v>
+      </c>
+      <c r="E5" s="10">
+        <f>ABS(data!E4/1000)</f>
+        <v>22.088999999999999</v>
+      </c>
+      <c r="F5" s="12">
+        <f>data!K4/1000</f>
+        <v>0.01</v>
+      </c>
+      <c r="G5" s="6">
+        <f t="shared" si="1"/>
+        <v>1.8866135760333712E-5</v>
+      </c>
+      <c r="H5">
         <v>1765764570.5999999</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>0</v>
       </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
+      <c r="J5">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I5">
-        <v>2004280246.45</v>
-      </c>
-      <c r="J5">
-        <v>2778013.9205800002</v>
-      </c>
       <c r="K5">
-        <f t="shared" si="1"/>
-        <v>1.3860406624774378E-3</v>
+        <f>data!P4</f>
+        <v>2357253019.6300001</v>
       </c>
       <c r="L5">
-        <f t="shared" si="2"/>
-        <v>238515675.85000014</v>
+        <f>data!Q4</f>
+        <v>1077.46392866</v>
       </c>
       <c r="M5">
         <f t="shared" si="3"/>
-        <v>0.13860406624774377</v>
+        <v>4.5708454700765267E-7</v>
       </c>
       <c r="N5">
         <f t="shared" si="4"/>
-        <v>2778013.9205800002</v>
-      </c>
-      <c r="O5" s="1">
+        <v>591488449.03000021</v>
+      </c>
+      <c r="O5">
         <f t="shared" si="5"/>
-        <v>238515675.85000014</v>
-      </c>
-      <c r="P5" s="1">
+        <v>4.5708454700765264E-5</v>
+      </c>
+      <c r="P5">
         <f t="shared" si="6"/>
-        <v>2778013.9205800002</v>
+        <v>1077.46392866</v>
       </c>
       <c r="Q5" s="1">
         <f t="shared" si="7"/>
-        <v>398285924.56999999</v>
+        <v>591488449.03000021</v>
       </c>
       <c r="R5" s="1">
         <f t="shared" si="8"/>
-        <v>954964898.20000005</v>
-      </c>
-      <c r="S5" s="15">
-        <f t="shared" si="9"/>
-        <v>4.0322648198373416</v>
-      </c>
-      <c r="T5" s="15">
-        <f t="shared" si="10"/>
-        <v>-0.40114460206569447</v>
-      </c>
-      <c r="V5" s="12">
-        <v>-194078973.59999999</v>
-      </c>
-      <c r="W5" s="12">
-        <v>79052465.370000005</v>
-      </c>
-      <c r="X5" s="12">
-        <v>268199947.5</v>
-      </c>
-      <c r="Y5" s="12">
-        <v>-5931802.1880000001</v>
-      </c>
-      <c r="Z5" s="12">
-        <v>-64117789.57</v>
-      </c>
-      <c r="AA5" s="12">
-        <v>-309727613.60000002</v>
-      </c>
-      <c r="AB5" s="12">
-        <v>-108885380</v>
-      </c>
-      <c r="AC5" s="12">
-        <v>2381820594</v>
-      </c>
-      <c r="AD5" s="12">
-        <v>-2689000</v>
-      </c>
-      <c r="AE5" s="12">
-        <v>-331479135</v>
-      </c>
-      <c r="AF5" s="12">
-        <v>-201840517</v>
-      </c>
-      <c r="AG5" s="12">
-        <v>-219085164</v>
-      </c>
-      <c r="AH5" s="12">
-        <v>-123187767</v>
-      </c>
-      <c r="AI5" s="12">
-        <v>144176100</v>
-      </c>
-      <c r="AJ5" s="12">
-        <v>77493385.799999997</v>
-      </c>
-      <c r="AK5" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="AL5" s="12">
-        <v>-678923816</v>
-      </c>
+        <v>1077.46392866</v>
+      </c>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="3"/>
+      <c r="AJ5" s="3"/>
+      <c r="AK5" s="3"/>
+      <c r="AL5" s="3"/>
+      <c r="AM5" s="3"/>
+      <c r="AN5" s="3"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6">
-        <v>769</v>
-      </c>
-      <c r="C6">
-        <v>754</v>
-      </c>
-      <c r="D6">
-        <v>2.5</v>
-      </c>
-      <c r="E6" s="3">
-        <v>31.7</v>
-      </c>
-      <c r="F6">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="str">
+        <f>UPPER(data!A5)</f>
+        <v>PRAIRIE-ISLAND</v>
+      </c>
+      <c r="B6" s="7">
+        <f>data!C5</f>
+        <v>522</v>
+      </c>
+      <c r="C6" s="7">
+        <f>data!D5</f>
+        <v>-507</v>
+      </c>
+      <c r="D6" s="10">
+        <f t="shared" si="0"/>
+        <v>12.738693467336685</v>
+      </c>
+      <c r="E6" s="10">
+        <f>ABS(data!E5/1000)</f>
+        <v>12.741</v>
+      </c>
+      <c r="F6" s="12">
+        <f>data!K5/1000</f>
+        <v>35</v>
+      </c>
+      <c r="G6" s="6">
+        <f t="shared" si="1"/>
+        <v>0.11448060486522026</v>
+      </c>
+      <c r="H6">
         <v>1080996406.4100001</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>0</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
+      <c r="J6">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I6">
-        <v>1444589208.6700001</v>
-      </c>
-      <c r="J6">
-        <v>3125292.0733699999</v>
-      </c>
       <c r="K6">
-        <f t="shared" si="1"/>
-        <v>2.1634469194515057E-3</v>
+        <f>data!P5</f>
+        <v>1177078719.72</v>
       </c>
       <c r="L6">
-        <f t="shared" si="2"/>
-        <v>363592802.25999999</v>
+        <f>data!Q5</f>
+        <v>45333.174797</v>
       </c>
       <c r="M6">
         <f t="shared" si="3"/>
-        <v>0.21634469194515057</v>
+        <v>3.8513290604543185E-5</v>
       </c>
       <c r="N6">
         <f t="shared" si="4"/>
-        <v>3125292.0733699999</v>
-      </c>
-      <c r="O6" s="1">
+        <v>96082313.309999943</v>
+      </c>
+      <c r="O6">
         <f t="shared" si="5"/>
-        <v>363592802.25999999</v>
-      </c>
-      <c r="P6" s="1">
+        <v>3.8513290604543183E-3</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="6"/>
-        <v>3125292.0733699999</v>
+        <v>45333.174797</v>
       </c>
       <c r="Q6" s="1">
         <f t="shared" si="7"/>
-        <v>905276044.97000003</v>
+        <v>96082313.309999943</v>
       </c>
       <c r="R6" s="1">
         <f t="shared" si="8"/>
-        <v>1676410541</v>
-      </c>
-      <c r="S6" s="15">
-        <f t="shared" si="9"/>
-        <v>0.59574443253700848</v>
-      </c>
-      <c r="T6" s="15">
-        <f t="shared" si="10"/>
-        <v>-0.59836250580114592</v>
-      </c>
-      <c r="V6" s="12">
-        <v>-318375700.19999999</v>
-      </c>
-      <c r="W6" s="12">
-        <v>97058773.25</v>
-      </c>
-      <c r="X6" s="12">
-        <v>4822640884</v>
-      </c>
-      <c r="Y6" s="12">
-        <v>-6576092.7999999998</v>
-      </c>
-      <c r="Z6" s="12">
-        <v>-64174373.969999999</v>
-      </c>
-      <c r="AA6" s="12">
-        <v>-343369091.80000001</v>
-      </c>
-      <c r="AB6" s="12">
-        <v>-120712111</v>
-      </c>
-      <c r="AC6" s="12">
-        <v>6430992992</v>
-      </c>
-      <c r="AD6" s="12">
-        <v>-21915670</v>
-      </c>
-      <c r="AE6" s="12">
-        <v>-819186001</v>
-      </c>
-      <c r="AF6" s="12">
-        <v>-552988308</v>
-      </c>
-      <c r="AG6" s="12">
-        <v>-600233967</v>
-      </c>
-      <c r="AH6" s="12">
-        <v>-293719671</v>
-      </c>
-      <c r="AI6" s="12">
-        <v>178756070</v>
-      </c>
-      <c r="AJ6" s="12">
-        <v>55536235.799999997</v>
-      </c>
-      <c r="AK6" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="AL6" s="12">
-        <v>-5023000000</v>
-      </c>
+        <v>45333.174797</v>
+      </c>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="3"/>
     </row>
-    <row r="7" spans="1:38" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="4">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="str">
+        <f>UPPER(data!A6)</f>
+        <v>STP</v>
+      </c>
+      <c r="B7" s="7">
+        <f>data!C6</f>
         <v>1280</v>
       </c>
-      <c r="C7" s="4">
-        <v>1252</v>
-      </c>
-      <c r="D7" s="4">
-        <v>2.5</v>
-      </c>
-      <c r="E7" s="5">
-        <v>43.8</v>
-      </c>
-      <c r="F7">
+      <c r="C7" s="7">
+        <f>data!D6</f>
+        <v>-1265</v>
+      </c>
+      <c r="D7" s="10">
+        <f t="shared" si="0"/>
+        <v>31.78391959798995</v>
+      </c>
+      <c r="E7" s="10">
+        <f>ABS(data!E6/1000)</f>
+        <v>31.789000000000001</v>
+      </c>
+      <c r="F7" s="12">
+        <f>data!K6/1000</f>
+        <v>2000</v>
+      </c>
+      <c r="G7" s="6">
+        <f t="shared" si="1"/>
+        <v>2.6218708827404478</v>
+      </c>
+      <c r="H7">
         <v>2721027335.4499998</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>76104994.533299997</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
+      <c r="J7">
+        <f t="shared" si="2"/>
         <v>2.7969213517920744E-2</v>
       </c>
-      <c r="I7">
-        <v>3420909282.1900001</v>
-      </c>
-      <c r="J7">
-        <v>24784321.460499998</v>
-      </c>
       <c r="K7">
-        <f t="shared" si="1"/>
-        <v>7.2449513904190863E-3</v>
+        <f>data!P6</f>
+        <v>2880661882.02</v>
       </c>
       <c r="L7">
-        <f t="shared" si="2"/>
-        <v>699881946.74000025</v>
+        <f>data!Q6</f>
+        <v>18447721.6961</v>
       </c>
       <c r="M7">
         <f t="shared" si="3"/>
-        <v>2.8892321219669697</v>
+        <v>6.403987156994609E-3</v>
       </c>
       <c r="N7">
         <f t="shared" si="4"/>
-        <v>80038945.415160388</v>
-      </c>
-      <c r="O7" s="1">
+        <v>159634546.57000017</v>
+      </c>
+      <c r="O7">
         <f t="shared" si="5"/>
-        <v>699881946.74000025</v>
-      </c>
-      <c r="P7" s="1">
+        <v>2.8692994899765907</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="6"/>
-        <v>80038945.415160388</v>
+        <v>78308930.708383322</v>
       </c>
       <c r="Q7" s="1">
         <f t="shared" si="7"/>
-        <v>650849884.57000005</v>
+        <v>159634546.57000017</v>
       </c>
       <c r="R7" s="1">
         <f t="shared" si="8"/>
-        <v>1312805569.4000001</v>
-      </c>
-      <c r="S7" s="15">
-        <f t="shared" si="9"/>
-        <v>4.2560649748752857</v>
-      </c>
-      <c r="T7" s="15">
-        <f t="shared" si="10"/>
-        <v>7.5335439603549187E-2</v>
-      </c>
-      <c r="V7" s="12">
-        <v>-216764494.59999999</v>
-      </c>
-      <c r="W7" s="12">
-        <v>86936338.530000001</v>
-      </c>
-      <c r="X7" s="12">
-        <v>2025170723</v>
-      </c>
-      <c r="Y7" s="12">
-        <v>-6576092.7999999998</v>
-      </c>
-      <c r="Z7" s="12">
-        <v>-64117789.57</v>
-      </c>
-      <c r="AA7" s="12">
-        <v>-343369091.80000001</v>
-      </c>
-      <c r="AB7" s="12">
-        <v>-120712111</v>
-      </c>
-      <c r="AC7" s="12">
-        <v>4468067921</v>
-      </c>
-      <c r="AD7" s="12">
-        <v>-12037500</v>
-      </c>
-      <c r="AE7" s="12">
-        <v>-574694595</v>
-      </c>
-      <c r="AF7" s="12">
-        <v>-387945340</v>
-      </c>
-      <c r="AG7" s="12">
-        <v>-421090224</v>
-      </c>
-      <c r="AH7" s="12">
-        <v>-210869648</v>
-      </c>
-      <c r="AI7" s="12">
-        <v>168833369</v>
-      </c>
-      <c r="AJ7" s="12">
-        <v>91728575.099999994</v>
-      </c>
-      <c r="AK7" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL7" s="12">
-        <v>-2478000000</v>
-      </c>
+        <v>78308930.708383322</v>
+      </c>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="3"/>
+      <c r="AN7" s="3"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8">
-        <v>1280</v>
-      </c>
-      <c r="C8">
-        <v>1265</v>
-      </c>
-      <c r="D8">
-        <v>18.295738</v>
-      </c>
-      <c r="E8">
-        <v>68.556979999999996</v>
-      </c>
-      <c r="F8">
-        <v>2861165724.4899998</v>
-      </c>
-      <c r="G8">
-        <v>75472956.378800005</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>2.6378393859814952E-2</v>
-      </c>
-      <c r="I8">
-        <v>4600730995.6000004</v>
-      </c>
-      <c r="J8">
-        <v>2992301.6630600002</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="1"/>
-        <v>6.5039700558927409E-4</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="2"/>
-        <v>1739565271.1100006</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="3"/>
-        <v>2.6386410875456381</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="4"/>
-        <v>75532251.481066018</v>
-      </c>
-      <c r="O8" s="1">
-        <f t="shared" si="5"/>
-        <v>1739565271.1100006</v>
-      </c>
-      <c r="P8" s="1">
-        <f t="shared" si="6"/>
-        <v>75532251.481066018</v>
-      </c>
-      <c r="Q8" s="1">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="R8" s="1">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="S8" s="14" t="e">
-        <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T8" t="e">
-        <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="4"/>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="D12" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14">
+        <v>2.5125628140703519E-2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>25.125628140703519</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <f>B15/1000</f>
+        <v>2.5125628140703519E-2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4340,11 +3966,578 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35F0C96-D3AA-4F4B-9456-DE375A306C8A}">
+  <dimension ref="A1:AD6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P2" sqref="P2:Q2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O1" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" t="s">
+        <v>61</v>
+      </c>
+      <c r="S1" t="s">
+        <v>62</v>
+      </c>
+      <c r="T1" t="s">
+        <v>63</v>
+      </c>
+      <c r="U1" t="s">
+        <v>64</v>
+      </c>
+      <c r="V1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W1" t="s">
+        <v>66</v>
+      </c>
+      <c r="X1" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>1193</v>
+      </c>
+      <c r="D2">
+        <v>-1178</v>
+      </c>
+      <c r="E2">
+        <v>-29603.14</v>
+      </c>
+      <c r="F2">
+        <v>-14.9</v>
+      </c>
+      <c r="G2" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="H2" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="I2" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="J2" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="K2">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>75</v>
+      </c>
+      <c r="O2" t="s">
+        <v>76</v>
+      </c>
+      <c r="P2">
+        <v>3408381162.0100002</v>
+      </c>
+      <c r="Q2">
+        <v>1225.80578418</v>
+      </c>
+      <c r="R2">
+        <v>3408381275.7399998</v>
+      </c>
+      <c r="S2">
+        <v>3408382533.2399998</v>
+      </c>
+      <c r="T2">
+        <v>3408379563.3400002</v>
+      </c>
+      <c r="U2">
+        <v>3408379797.4699998</v>
+      </c>
+      <c r="V2">
+        <v>3408382367.3400002</v>
+      </c>
+      <c r="W2">
+        <v>4</v>
+      </c>
+      <c r="X2">
+        <v>1502599.82054</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>0.24493882102600001</v>
+      </c>
+      <c r="AA2">
+        <v>1.9309406027700001E-3</v>
+      </c>
+      <c r="AB2">
+        <v>2.4976248812400001E-2</v>
+      </c>
+      <c r="AC2">
+        <v>0.31563421828900001</v>
+      </c>
+      <c r="AD2" s="11">
+        <v>3.7621523992799998E-13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>769</v>
+      </c>
+      <c r="D3">
+        <v>-754</v>
+      </c>
+      <c r="E3">
+        <v>-18948</v>
+      </c>
+      <c r="F3">
+        <v>-14.9</v>
+      </c>
+      <c r="G3" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="H3" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="I3" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="J3" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="K3">
+        <v>10</v>
+      </c>
+      <c r="L3" t="s">
+        <v>74</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
+        <v>77</v>
+      </c>
+      <c r="O3" t="s">
+        <v>76</v>
+      </c>
+      <c r="P3">
+        <v>1941425295.5999999</v>
+      </c>
+      <c r="Q3">
+        <v>6952.2878666099996</v>
+      </c>
+      <c r="R3">
+        <v>1941428170.23</v>
+      </c>
+      <c r="S3">
+        <v>1941429832.72</v>
+      </c>
+      <c r="T3">
+        <v>1941415009.23</v>
+      </c>
+      <c r="U3">
+        <v>1941416830.3699999</v>
+      </c>
+      <c r="V3">
+        <v>1941429736.3599999</v>
+      </c>
+      <c r="W3">
+        <v>4</v>
+      </c>
+      <c r="X3">
+        <v>48334306.580200002</v>
+      </c>
+      <c r="Y3">
+        <v>0.263848935103</v>
+      </c>
+      <c r="Z3">
+        <v>2.1611600770599999E-2</v>
+      </c>
+      <c r="AA3">
+        <v>0.30264679038600001</v>
+      </c>
+      <c r="AB3" s="11">
+        <v>1.22768367385E-12</v>
+      </c>
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
+        <v>0.27064220183499998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>894</v>
+      </c>
+      <c r="D4">
+        <v>-879</v>
+      </c>
+      <c r="E4">
+        <v>-22089</v>
+      </c>
+      <c r="F4">
+        <v>-14.9</v>
+      </c>
+      <c r="G4" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="H4" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="I4" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="J4" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="K4">
+        <v>10</v>
+      </c>
+      <c r="L4" t="s">
+        <v>74</v>
+      </c>
+      <c r="M4" t="s">
+        <v>25</v>
+      </c>
+      <c r="N4" t="s">
+        <v>80</v>
+      </c>
+      <c r="O4" t="s">
+        <v>76</v>
+      </c>
+      <c r="P4">
+        <v>2357253019.6300001</v>
+      </c>
+      <c r="Q4">
+        <v>1077.46392866</v>
+      </c>
+      <c r="R4">
+        <v>2357252830.3800001</v>
+      </c>
+      <c r="S4">
+        <v>2357254371.6500001</v>
+      </c>
+      <c r="T4">
+        <v>2357252046.0900002</v>
+      </c>
+      <c r="U4">
+        <v>2357252079.1900001</v>
+      </c>
+      <c r="V4">
+        <v>2357254225.0100002</v>
+      </c>
+      <c r="W4">
+        <v>4</v>
+      </c>
+      <c r="X4">
+        <v>1160928.5175600001</v>
+      </c>
+      <c r="Y4">
+        <v>2.1252890767700001E-2</v>
+      </c>
+      <c r="Z4">
+        <v>0.30877094401299998</v>
+      </c>
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="11">
+        <v>7.2869255798000005E-13</v>
+      </c>
+      <c r="AC4">
+        <v>0.275353016688</v>
+      </c>
+      <c r="AD4">
+        <v>0.24997221913500001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>522</v>
+      </c>
+      <c r="D5">
+        <v>-507</v>
+      </c>
+      <c r="E5">
+        <v>-12741</v>
+      </c>
+      <c r="F5">
+        <v>-14.9</v>
+      </c>
+      <c r="G5" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="H5" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="I5" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="J5" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="K5">
+        <v>35000</v>
+      </c>
+      <c r="L5" t="s">
+        <v>74</v>
+      </c>
+      <c r="M5" t="s">
+        <v>23</v>
+      </c>
+      <c r="N5" t="s">
+        <v>82</v>
+      </c>
+      <c r="O5" t="s">
+        <v>76</v>
+      </c>
+      <c r="P5">
+        <v>1177078719.72</v>
+      </c>
+      <c r="Q5">
+        <v>45333.174797</v>
+      </c>
+      <c r="R5">
+        <v>1177087754.28</v>
+      </c>
+      <c r="S5">
+        <v>1177118966.7</v>
+      </c>
+      <c r="T5">
+        <v>1177020403.6300001</v>
+      </c>
+      <c r="U5">
+        <v>1177027183.3699999</v>
+      </c>
+      <c r="V5">
+        <v>1177117607.7</v>
+      </c>
+      <c r="W5">
+        <v>4</v>
+      </c>
+      <c r="X5">
+        <v>2055096737.1700001</v>
+      </c>
+      <c r="Y5">
+        <v>5.2021435833E-2</v>
+      </c>
+      <c r="Z5">
+        <v>0.5</v>
+      </c>
+      <c r="AA5">
+        <v>4</v>
+      </c>
+      <c r="AB5">
+        <v>0.315724815725</v>
+      </c>
+      <c r="AC5" s="11">
+        <v>3.4322497171699999E-12</v>
+      </c>
+      <c r="AD5">
+        <v>0.32953656628900002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1280</v>
+      </c>
+      <c r="D6">
+        <v>-1265</v>
+      </c>
+      <c r="E6">
+        <v>-31789</v>
+      </c>
+      <c r="F6">
+        <v>-14.9</v>
+      </c>
+      <c r="G6" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="H6" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="I6" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="J6" s="11">
+        <v>-9.9999999999999997E+199</v>
+      </c>
+      <c r="K6">
+        <v>2000000</v>
+      </c>
+      <c r="L6" t="s">
+        <v>74</v>
+      </c>
+      <c r="M6" t="s">
+        <v>83</v>
+      </c>
+      <c r="N6" t="s">
+        <v>84</v>
+      </c>
+      <c r="O6" t="s">
+        <v>76</v>
+      </c>
+      <c r="P6">
+        <v>2880661882.02</v>
+      </c>
+      <c r="Q6">
+        <v>18447721.6961</v>
+      </c>
+      <c r="R6">
+        <v>2882183403.02</v>
+      </c>
+      <c r="S6">
+        <v>2919873833.9099998</v>
+      </c>
+      <c r="T6">
+        <v>2851246232.9899998</v>
+      </c>
+      <c r="U6">
+        <v>2856011739.0500002</v>
+      </c>
+      <c r="V6">
+        <v>2905799143.7800002</v>
+      </c>
+      <c r="W6">
+        <v>10</v>
+      </c>
+      <c r="X6" s="11">
+        <v>340318435777000</v>
+      </c>
+      <c r="Y6">
+        <v>10</v>
+      </c>
+      <c r="Z6">
+        <v>0.28673657603500002</v>
+      </c>
+      <c r="AA6">
+        <v>0.26394849785399999</v>
+      </c>
+      <c r="AB6">
+        <v>1.8921016736099999E-2</v>
+      </c>
+      <c r="AC6" s="11">
+        <v>1.46600182842E-14</v>
+      </c>
+      <c r="AD6">
+        <v>0.25000125000599999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBA1661-1357-8E4D-8878-EEFCBAD9628D}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4357,30 +4550,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>2102483898.8800001</v>
@@ -4388,7 +4581,7 @@
       <c r="C2">
         <v>10442175.4814</v>
       </c>
-      <c r="D2" s="11">
+      <c r="D2" s="2">
         <f>C2/B2</f>
         <v>4.966589987662964E-3</v>
       </c>
@@ -4400,252 +4593,252 @@
         <f>SQRT(POWER($C$2,2)+POWER(C2,2))</f>
         <v>14767466.186475683</v>
       </c>
-      <c r="G2" s="11" t="e">
+      <c r="G2" s="2" t="e">
         <f>F2/E2</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B3">
-        <v>2383373790.52</v>
+        <v>3408381162.0100002</v>
       </c>
       <c r="C3">
-        <v>2612665.1925300001</v>
-      </c>
-      <c r="D3" s="11">
+        <v>1225.80578418</v>
+      </c>
+      <c r="D3" s="2">
         <f t="shared" ref="D3:D11" si="0">C3/B3</f>
-        <v>1.0962045495851382E-3</v>
+        <v>3.5964457198710559E-7</v>
       </c>
       <c r="E3">
         <f>B3-$B$2</f>
-        <v>280889891.63999987</v>
+        <v>1305897263.1300001</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F11" si="1">SQRT(POWER($C$2,2)+POWER(C3,2))</f>
-        <v>10764062.810696023</v>
-      </c>
-      <c r="G3" s="11">
+        <v>10442175.553348601</v>
+      </c>
+      <c r="G3" s="2">
         <f>F3/E3</f>
-        <v>3.8321289341702945E-2</v>
+        <v>7.9961692609115276E-3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="B4">
-        <v>2394924501.1399999</v>
+        <v>3074633986.1399999</v>
       </c>
       <c r="C4">
-        <v>10704791.368100001</v>
-      </c>
-      <c r="D4" s="11">
+        <v>512.38935146899996</v>
+      </c>
+      <c r="D4" s="2">
         <f t="shared" si="0"/>
-        <v>4.4697823931420175E-3</v>
+        <v>1.6665051963218262E-7</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E11" si="2">B4-$B$2</f>
-        <v>292440602.25999975</v>
+        <v>972150087.25999975</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>14954316.668403795</v>
-      </c>
-      <c r="G4" s="11">
+        <v>10442175.493971271</v>
+      </c>
+      <c r="G4" s="2">
         <f t="shared" ref="G4:G11" si="3">F4/E4</f>
-        <v>5.1136253149651159E-2</v>
+        <v>1.0741320327813261E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
       <c r="B5">
-        <v>2379561041</v>
+        <v>3742127992.46</v>
       </c>
       <c r="C5">
-        <v>946260.03899999999</v>
-      </c>
-      <c r="D5" s="11">
+        <v>327.84723676099998</v>
+      </c>
+      <c r="D5" s="2">
         <f t="shared" si="0"/>
-        <v>3.976615950151623E-4</v>
+        <v>8.7609840556383468E-8</v>
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
-        <v>277077142.11999989</v>
+        <v>1639644093.5799999</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>10484962.415085692</v>
-      </c>
-      <c r="G5" s="11">
+        <v>10442175.486546619</v>
+      </c>
+      <c r="G5" s="2">
         <f t="shared" si="3"/>
-        <v>3.7841311393867122E-2</v>
+        <v>6.3685622553289398E-3</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6">
-        <v>2599318853</v>
-      </c>
-      <c r="C6">
-        <v>3430459.52</v>
-      </c>
-      <c r="D6" s="11">
+        <v>88</v>
+      </c>
+      <c r="B6" s="3">
+        <v>3638289546</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1495.11133</v>
+      </c>
+      <c r="D6" s="2">
         <f t="shared" si="0"/>
-        <v>1.3197532561427545E-3</v>
+        <v>4.1093797266458682E-7</v>
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
-        <v>496834954.11999989</v>
+        <v>1535805647.1199999</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>10991227.470246894</v>
-      </c>
-      <c r="G6" s="11">
+        <v>10442175.588435065</v>
+      </c>
+      <c r="G6" s="2">
         <f t="shared" si="3"/>
-        <v>2.2122492347010265E-2</v>
+        <v>6.7991517077806186E-3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7">
-        <v>2167046723</v>
-      </c>
-      <c r="C7">
-        <v>4248457.0999999996</v>
-      </c>
-      <c r="D7" s="11">
+        <v>89</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3178472614</v>
+      </c>
+      <c r="C7" s="3">
+        <v>707.38896</v>
+      </c>
+      <c r="D7" s="2">
         <f t="shared" si="0"/>
-        <v>1.9604824644106206E-3</v>
+        <v>2.2255625449916178E-7</v>
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
-        <v>64562824.119999886</v>
+        <v>1075988715.1199999</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>11273349.835558716</v>
-      </c>
-      <c r="G7" s="11">
+        <v>10442175.505360482</v>
+      </c>
+      <c r="G7" s="2">
         <f t="shared" si="3"/>
-        <v>0.17461054390380246</v>
+        <v>9.7047258569026122E-3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="B8">
-        <v>2361787989.04</v>
+        <v>2997736770.0300002</v>
       </c>
       <c r="C8">
-        <v>3573229.9468999999</v>
-      </c>
-      <c r="D8" s="11">
+        <v>667.62040469600004</v>
+      </c>
+      <c r="D8" s="2">
         <f t="shared" si="0"/>
-        <v>1.5129342529819608E-3</v>
+        <v>2.227081481504858E-7</v>
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
-        <v>259304090.15999985</v>
+        <v>895252871.1500001</v>
       </c>
       <c r="F8">
         <f t="shared" si="1"/>
-        <v>11036620.906680372</v>
-      </c>
-      <c r="G8" s="11">
+        <v>10442175.502742153</v>
+      </c>
+      <c r="G8" s="2">
         <f t="shared" si="3"/>
-        <v>4.2562463630521151E-2</v>
+        <v>1.1663939697092087E-2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9">
-        <v>2330056942</v>
-      </c>
-      <c r="C9">
-        <v>3963896.24</v>
-      </c>
-      <c r="D9" s="11">
+        <v>91</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2587091316</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1407.3527200000001</v>
+      </c>
+      <c r="D9" s="2">
         <f t="shared" si="0"/>
-        <v>1.7012014464322907E-3</v>
+        <v>5.4399035368259108E-7</v>
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
-        <v>227573043.11999989</v>
+        <v>484607417.11999989</v>
       </c>
       <c r="F9">
         <f t="shared" si="1"/>
-        <v>11169221.198715579</v>
-      </c>
-      <c r="G9" s="11">
+        <v>10442175.576238554</v>
+      </c>
+      <c r="G9" s="2">
         <f t="shared" si="3"/>
-        <v>4.9079719836703235E-2</v>
+        <v>2.1547700689964536E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>69</v>
-      </c>
-      <c r="B10">
-        <v>2516165805.98</v>
-      </c>
-      <c r="C10">
-        <v>4113660.2426399998</v>
-      </c>
-      <c r="D10" s="11">
+        <v>92</v>
+      </c>
+      <c r="B10" s="3">
+        <v>3819025493</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1204.90344</v>
+      </c>
+      <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>1.6348923560058496E-3</v>
+        <v>3.1550023486580589E-7</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>413681907.0999999</v>
+        <v>1716541594.1199999</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>11223245.04660877</v>
-      </c>
-      <c r="G10" s="11">
+        <v>10442175.550915796</v>
+      </c>
+      <c r="G10" s="2">
         <f t="shared" si="3"/>
-        <v>2.7130132727549428E-2</v>
+        <v>6.0832639224621112E-3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="B11">
-        <v>2249172403.6100001</v>
+        <v>4229670899.3699999</v>
       </c>
       <c r="C11">
-        <v>1997773.4791000001</v>
-      </c>
-      <c r="D11" s="11">
+        <v>1029.5019684700001</v>
+      </c>
+      <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>8.8822603189222138E-4</v>
+        <v>2.4340001691936414E-7</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>146688504.73000002</v>
+        <v>2127187000.4899998</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>10631562.804129345</v>
-      </c>
-      <c r="G11" s="11">
+        <v>10442175.532149687</v>
+      </c>
+      <c r="G11" s="2">
         <f t="shared" si="3"/>
-        <v>7.2477136662468342E-2</v>
+        <v>4.9089128176057492E-3</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -4653,255 +4846,104 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>63</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="B14">
         <f>E4</f>
-        <v>292440602.25999975</v>
+        <v>972150087.25999975</v>
       </c>
       <c r="C14">
         <f>E5</f>
-        <v>277077142.11999989</v>
+        <v>1639644093.5799999</v>
       </c>
       <c r="D14">
         <f>F4</f>
-        <v>14954316.668403795</v>
+        <v>10442175.493971271</v>
       </c>
       <c r="E14">
         <f>F5</f>
-        <v>10484962.415085692</v>
+        <v>10442175.486546619</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>31</v>
       </c>
       <c r="B15">
         <f>E6</f>
-        <v>496834954.11999989</v>
+        <v>1535805647.1199999</v>
       </c>
       <c r="C15">
         <f>E7</f>
-        <v>64562824.119999886</v>
+        <v>1075988715.1199999</v>
       </c>
       <c r="D15">
         <f>F6</f>
-        <v>10991227.470246894</v>
+        <v>10442175.588435065</v>
       </c>
       <c r="E15">
         <f>F7</f>
-        <v>11273349.835558716</v>
+        <v>10442175.505360482</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B16">
         <f>E8</f>
-        <v>259304090.15999985</v>
+        <v>895252871.1500001</v>
       </c>
       <c r="C16">
         <f>E9</f>
-        <v>227573043.11999989</v>
+        <v>484607417.11999989</v>
       </c>
       <c r="D16">
         <f>F8</f>
-        <v>11036620.906680372</v>
+        <v>10442175.502742153</v>
       </c>
       <c r="E16">
         <f>F9</f>
-        <v>11169221.198715579</v>
+        <v>10442175.576238554</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>71</v>
+        <v>94</v>
       </c>
       <c r="B17">
         <f>E10</f>
-        <v>413681907.0999999</v>
+        <v>1716541594.1199999</v>
       </c>
       <c r="C17">
         <f>E11</f>
-        <v>146688504.73000002</v>
+        <v>2127187000.4899998</v>
       </c>
       <c r="D17">
         <f>F10</f>
-        <v>11223245.04660877</v>
+        <v>10442175.550915796</v>
       </c>
       <c r="E17">
         <f>F11</f>
-        <v>10631562.804129345</v>
+        <v>10442175.532149687</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BBBBF4E-63B1-3B49-81EC-48E68EDAAD9B}">
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2">
-        <v>2102483898.8800001</v>
-      </c>
-      <c r="C2">
-        <v>10442175.4814</v>
-      </c>
-      <c r="D2" s="11">
-        <f>C2/B2</f>
-        <v>4.966589987662964E-3</v>
-      </c>
-      <c r="E2">
-        <f>B2-$B$2</f>
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <f>SQRT(POWER(C2,2)+POWER($C$2,2))</f>
-        <v>14767466.186475683</v>
-      </c>
-      <c r="G2" s="11" t="e">
-        <f>F2/E2</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3">
-        <v>3589667022.7199998</v>
-      </c>
-      <c r="C3">
-        <v>20927.310484099999</v>
-      </c>
-      <c r="D3" s="11">
-        <f t="shared" ref="D3:D5" si="0">C3/B3</f>
-        <v>5.8298751253654551E-6</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E5" si="1">B3-$B$2</f>
-        <v>1487183123.8399997</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F5" si="2">SQRT(POWER(C3,2)+POWER($C$2,2))</f>
-        <v>10442196.451737316</v>
-      </c>
-      <c r="G3" s="11">
-        <f t="shared" ref="G3:G5" si="3">F3/E3</f>
-        <v>7.0214597545828206E-3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4">
-        <v>2162947058</v>
-      </c>
-      <c r="C4">
-        <v>15334997.619999999</v>
-      </c>
-      <c r="D4" s="11">
-        <f t="shared" si="0"/>
-        <v>7.0898626775357711E-3</v>
-      </c>
-      <c r="E4">
-        <f>B4-$B$2</f>
-        <v>60463159.119999886</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="2"/>
-        <v>18552659.668892678</v>
-      </c>
-      <c r="G4" s="11">
-        <f t="shared" si="3"/>
-        <v>0.30684238036705341</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5">
-        <v>3311505178.27</v>
-      </c>
-      <c r="C5">
-        <v>4118428.9192300001</v>
-      </c>
-      <c r="D5" s="11">
-        <f t="shared" si="0"/>
-        <v>1.2436728005908039E-3</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="1"/>
-        <v>1209021279.3899999</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="2"/>
-        <v>11224993.788287871</v>
-      </c>
-      <c r="G5" s="11">
-        <f t="shared" si="3"/>
-        <v>9.2843641213257496E-3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
add o&m to braidwood sa
</commit_message>
<xml_diff>
--- a/use_cases/IES_Feb23/run/results.xlsx
+++ b/use_cases/IES_Feb23/run/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/IES_Feb23/run/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB11A45-FBFA-F249-B550-04FD1B0849CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5037D8-AB86-5B46-84A4-515CBC38AA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36140" yWindow="2000" windowWidth="35840" windowHeight="20200" activeTab="2" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
   </bookViews>
@@ -316,13 +316,13 @@
     <t>co2 cost high</t>
   </si>
   <si>
-    <t>co2 tax med</t>
-  </si>
-  <si>
-    <t>co2 tax high</t>
-  </si>
-  <si>
-    <t>CO2 Tax</t>
+    <t>o&amp;m 0.75</t>
+  </si>
+  <si>
+    <t>o&amp;m1.25</t>
+  </si>
+  <si>
+    <t>O&amp;M</t>
   </si>
 </sst>
 </file>
@@ -379,7 +379,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -387,16 +387,15 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -937,7 +936,7 @@
                   <c:v>CO2 Cost</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CO2 Tax</c:v>
+                  <c:v>O&amp;M</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -958,7 +957,7 @@
                   <c:v>895252871.1500001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1716541594.1199999</c:v>
+                  <c:v>1488603302.1199999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1008,7 +1007,7 @@
                   <c:v>CO2 Cost</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>CO2 Tax</c:v>
+                  <c:v>O&amp;M</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1029,7 +1028,7 @@
                   <c:v>484607417.11999989</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2127187000.4899998</c:v>
+                  <c:v>1123190020.5299997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3319,36 +3318,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A1" s="7"/>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="9"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="7"/>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" t="s">
         <v>85</v>
       </c>
       <c r="H2" t="s">
@@ -3403,27 +3401,27 @@
       <c r="AN2" s="3"/>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="str">
+      <c r="A3" t="str">
         <f>UPPER(data!A2)</f>
         <v>BRAIDWOOD</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3">
         <f>data!C2</f>
         <v>1193</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3">
         <f>data!D2</f>
         <v>-1178</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="8">
         <f>ABS(C3)*$B$16</f>
         <v>29.597989949748744</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="8">
         <f>ABS(data!E2/1000)</f>
         <v>29.60314</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="10">
         <f>data!K2/1000</f>
         <v>0.01</v>
       </c>
@@ -3496,27 +3494,27 @@
       <c r="AN3" s="3"/>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="str">
+      <c r="A4" t="str">
         <f>UPPER(data!A3)</f>
         <v>COOPER</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4">
         <f>data!C3</f>
         <v>769</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4">
         <f>data!D3</f>
         <v>-754</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="8">
         <f t="shared" ref="D4:D7" si="0">ABS(C4)*$B$16</f>
         <v>18.944723618090453</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="8">
         <f>ABS(data!E3/1000)</f>
         <v>18.948</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="10">
         <f>data!K3/1000</f>
         <v>0.01</v>
       </c>
@@ -3589,27 +3587,27 @@
       <c r="AN4" s="3"/>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A5" s="7" t="str">
+      <c r="A5" t="str">
         <f>UPPER(data!A4)</f>
         <v>DAVIS-BESSE</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5">
         <f>data!C4</f>
         <v>894</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5">
         <f>data!D4</f>
         <v>-879</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="8">
         <f t="shared" si="0"/>
         <v>22.085427135678394</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="8">
         <f>ABS(data!E4/1000)</f>
         <v>22.088999999999999</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="10">
         <f>data!K4/1000</f>
         <v>0.01</v>
       </c>
@@ -3682,27 +3680,27 @@
       <c r="AN5" s="3"/>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A6" s="7" t="str">
+      <c r="A6" t="str">
         <f>UPPER(data!A5)</f>
         <v>PRAIRIE-ISLAND</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6">
         <f>data!C5</f>
         <v>522</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6">
         <f>data!D5</f>
         <v>-507</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="8">
         <f t="shared" si="0"/>
         <v>12.738693467336685</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="8">
         <f>ABS(data!E5/1000)</f>
         <v>12.741</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="10">
         <f>data!K5/1000</f>
         <v>35</v>
       </c>
@@ -3775,27 +3773,27 @@
       <c r="AN6" s="3"/>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="str">
+      <c r="A7" t="str">
         <f>UPPER(data!A6)</f>
         <v>STP</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7">
         <f>data!C6</f>
         <v>1280</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7">
         <f>data!D6</f>
         <v>-1265</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="8">
         <f t="shared" si="0"/>
         <v>31.78391959798995</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="8">
         <f>ABS(data!E6/1000)</f>
         <v>31.789000000000001</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="10">
         <f>data!K6/1000</f>
         <v>2000</v>
       </c>
@@ -3868,49 +3866,21 @@
       <c r="AN7" s="3"/>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
       <c r="U8" s="4"/>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="A10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="A11" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
@@ -4086,16 +4056,16 @@
       <c r="F2">
         <v>-14.9</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="J2" s="11">
+      <c r="J2" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
       <c r="K2">
@@ -4155,7 +4125,7 @@
       <c r="AC2">
         <v>0.31563421828900001</v>
       </c>
-      <c r="AD2" s="11">
+      <c r="AD2" s="9">
         <v>3.7621523992799998E-13</v>
       </c>
     </row>
@@ -4178,16 +4148,16 @@
       <c r="F3">
         <v>-14.9</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="I3" s="11">
+      <c r="I3" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="J3" s="11">
+      <c r="J3" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
       <c r="K3">
@@ -4241,7 +4211,7 @@
       <c r="AA3">
         <v>0.30264679038600001</v>
       </c>
-      <c r="AB3" s="11">
+      <c r="AB3" s="9">
         <v>1.22768367385E-12</v>
       </c>
       <c r="AC3">
@@ -4270,16 +4240,16 @@
       <c r="F4">
         <v>-14.9</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
       <c r="K4">
@@ -4333,7 +4303,7 @@
       <c r="AA4">
         <v>1</v>
       </c>
-      <c r="AB4" s="11">
+      <c r="AB4" s="9">
         <v>7.2869255798000005E-13</v>
       </c>
       <c r="AC4">
@@ -4362,16 +4332,16 @@
       <c r="F5">
         <v>-14.9</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="H5" s="11">
+      <c r="H5" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="J5" s="11">
+      <c r="J5" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
       <c r="K5">
@@ -4428,7 +4398,7 @@
       <c r="AB5">
         <v>0.315724815725</v>
       </c>
-      <c r="AC5" s="11">
+      <c r="AC5" s="9">
         <v>3.4322497171699999E-12</v>
       </c>
       <c r="AD5">
@@ -4454,16 +4424,16 @@
       <c r="F6">
         <v>-14.9</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="9">
         <v>-9.9999999999999997E+199</v>
       </c>
       <c r="K6">
@@ -4505,7 +4475,7 @@
       <c r="W6">
         <v>10</v>
       </c>
-      <c r="X6" s="11">
+      <c r="X6" s="9">
         <v>340318435777000</v>
       </c>
       <c r="Y6">
@@ -4520,7 +4490,7 @@
       <c r="AB6">
         <v>1.8921016736099999E-2</v>
       </c>
-      <c r="AC6" s="11">
+      <c r="AC6" s="9">
         <v>1.46600182842E-14</v>
       </c>
       <c r="AD6">
@@ -4537,7 +4507,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4791,27 +4761,27 @@
       <c r="A10" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="3">
-        <v>3819025493</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1204.90344</v>
+      <c r="B10">
+        <v>3591087201</v>
+      </c>
+      <c r="C10">
+        <v>476.18838690899997</v>
       </c>
       <c r="D10" s="2">
         <f t="shared" si="0"/>
-        <v>3.1550023486580589E-7</v>
+        <v>1.3260284706436457E-7</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>1716541594.1199999</v>
+        <v>1488603302.1199999</v>
       </c>
       <c r="F10">
         <f t="shared" si="1"/>
-        <v>10442175.550915796</v>
+        <v>10442175.49225767</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="3"/>
-        <v>6.0832639224621112E-3</v>
+        <v>7.0147469627310421E-3</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -4819,26 +4789,26 @@
         <v>93</v>
       </c>
       <c r="B11">
-        <v>4229670899.3699999</v>
+        <v>3225673919.4099998</v>
       </c>
       <c r="C11">
-        <v>1029.5019684700001</v>
+        <v>1255.44823124</v>
       </c>
       <c r="D11" s="2">
         <f t="shared" si="0"/>
-        <v>2.4340001691936414E-7</v>
+        <v>3.8920494216279338E-7</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>2127187000.4899998</v>
+        <v>1123190020.5299997</v>
       </c>
       <c r="F11">
         <f t="shared" si="1"/>
-        <v>10442175.532149687</v>
+        <v>10442175.556870397</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="3"/>
-        <v>4.9089128176057492E-3</v>
+        <v>9.2968913238234141E-3</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -4927,19 +4897,19 @@
       </c>
       <c r="B17">
         <f>E10</f>
-        <v>1716541594.1199999</v>
+        <v>1488603302.1199999</v>
       </c>
       <c r="C17">
         <f>E11</f>
-        <v>2127187000.4899998</v>
+        <v>1123190020.5299997</v>
       </c>
       <c r="D17">
         <f>F10</f>
-        <v>10442175.550915796</v>
+        <v>10442175.49225767</v>
       </c>
       <c r="E17">
         <f>F11</f>
-        <v>10442175.532149687</v>
+        <v>10442175.556870397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update results and add sweep png files
</commit_message>
<xml_diff>
--- a/use_cases/IES_Feb23/run/results.xlsx
+++ b/use_cases/IES_Feb23/run/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/IES_Feb23/run/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5037D8-AB86-5B46-84A4-515CBC38AA6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B255BB-2633-1C4D-A5D0-2B6CC1E7E06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36140" yWindow="2000" windowWidth="35840" windowHeight="20200" activeTab="2" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
+    <workbookView xWindow="5120" yWindow="7640" windowWidth="30720" windowHeight="17000" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="96">
   <si>
     <t>Location</t>
   </si>
@@ -323,6 +323,9 @@
   </si>
   <si>
     <t>O&amp;M</t>
+  </si>
+  <si>
+    <t>Standardized added value (M$/MWh)</t>
   </si>
 </sst>
 </file>
@@ -429,37 +432,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -491,7 +464,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
-            <c:numFmt formatCode="&quot;$&quot;#,##0" sourceLinked="0"/>
+            <c:numFmt formatCode="&quot;$&quot;#,##0.00" sourceLinked="0"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -569,10 +542,10 @@
                     <c:v>1077.46392866</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>45333.174797</c:v>
+                    <c:v>555817.3250380737</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>78308930.708383322</c:v>
+                    <c:v>85899046.268169791</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -593,10 +566,10 @@
                     <c:v>1077.46392866</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>45333.174797</c:v>
+                    <c:v>555817.3250380737</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>78308930.708383322</c:v>
+                    <c:v>85899046.268169791</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -654,10 +627,10 @@
                   <c:v>591488449.03000021</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>96082313.309999943</c:v>
+                  <c:v>914678100.61800003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>159634546.57000017</c:v>
+                  <c:v>138177069.53999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -790,7 +763,7 @@
         <c:crossBetween val="between"/>
         <c:majorUnit val="250000000"/>
         <c:dispUnits>
-          <c:builtInUnit val="millions"/>
+          <c:builtInUnit val="billions"/>
           <c:dispUnitsLbl>
             <c:spPr>
               <a:noFill/>
@@ -2339,9 +2312,9 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>901700</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3288,8 +3261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FE355D-8072-1247-9790-841EBA440D66}">
   <dimension ref="A1:AN16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O35" sqref="O35"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3304,9 +3277,9 @@
     <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="14.6640625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="11.1640625" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20.6640625" customWidth="1"/>
@@ -3381,6 +3354,9 @@
       </c>
       <c r="R2" t="s">
         <v>13</v>
+      </c>
+      <c r="S2" t="s">
+        <v>95</v>
       </c>
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
@@ -3471,7 +3447,10 @@
         <f>P3</f>
         <v>10442175.071948605</v>
       </c>
-      <c r="S3" s="1"/>
+      <c r="S3" s="1">
+        <f>Q3/B3</f>
+        <v>1094633.0789019279</v>
+      </c>
       <c r="T3" s="1"/>
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
@@ -3564,7 +3543,10 @@
         <f t="shared" ref="R4:R7" si="8">P4</f>
         <v>6952.2878666099996</v>
       </c>
-      <c r="S4" s="1"/>
+      <c r="S4" s="1">
+        <f>Q4/B4</f>
+        <v>2183179.2434980492</v>
+      </c>
       <c r="T4" s="1"/>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
@@ -3657,7 +3639,10 @@
         <f t="shared" si="8"/>
         <v>1077.46392866</v>
       </c>
-      <c r="S5" s="1"/>
+      <c r="S5" s="1">
+        <f t="shared" ref="S5:S7" si="9">Q5/B5</f>
+        <v>661620.18907158857</v>
+      </c>
       <c r="T5" s="1"/>
       <c r="U5" s="5"/>
       <c r="V5" s="5"/>
@@ -3709,14 +3694,14 @@
         <v>0.11448060486522026</v>
       </c>
       <c r="H6">
-        <v>1080996406.4100001</v>
+        <v>262400619.102</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>553965.52426600002</v>
       </c>
       <c r="J6">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2.1111441206267249E-3</v>
       </c>
       <c r="K6">
         <f>data!P5</f>
@@ -3732,25 +3717,28 @@
       </c>
       <c r="N6">
         <f t="shared" si="4"/>
-        <v>96082313.309999943</v>
+        <v>914678100.61800003</v>
       </c>
       <c r="O6">
         <f t="shared" si="5"/>
-        <v>3.8513290604543183E-3</v>
+        <v>0.21114953875417244</v>
       </c>
       <c r="P6">
         <f t="shared" si="6"/>
-        <v>45333.174797</v>
+        <v>555817.3250380737</v>
       </c>
       <c r="Q6" s="1">
         <f t="shared" si="7"/>
-        <v>96082313.309999943</v>
+        <v>914678100.61800003</v>
       </c>
       <c r="R6" s="1">
         <f t="shared" si="8"/>
-        <v>45333.174797</v>
-      </c>
-      <c r="S6" s="1"/>
+        <v>555817.3250380737</v>
+      </c>
+      <c r="S6" s="1">
+        <f t="shared" si="9"/>
+        <v>1752256.8977356323</v>
+      </c>
       <c r="T6" s="1"/>
       <c r="U6" s="5"/>
       <c r="V6" s="5"/>
@@ -3802,14 +3790,14 @@
         <v>2.6218708827404478</v>
       </c>
       <c r="H7">
-        <v>2721027335.4499998</v>
+        <v>2742484812.48</v>
       </c>
       <c r="I7">
-        <v>76104994.533299997</v>
+        <v>83894741.873400003</v>
       </c>
       <c r="J7">
         <f t="shared" si="2"/>
-        <v>2.7969213517920744E-2</v>
+        <v>3.0590777200160638E-2</v>
       </c>
       <c r="K7">
         <f>data!P6</f>
@@ -3825,25 +3813,28 @@
       </c>
       <c r="N7">
         <f t="shared" si="4"/>
-        <v>159634546.57000017</v>
+        <v>138177069.53999996</v>
       </c>
       <c r="O7">
         <f t="shared" si="5"/>
-        <v>2.8692994899765907</v>
+        <v>3.1253906975237826</v>
       </c>
       <c r="P7">
         <f t="shared" si="6"/>
-        <v>78308930.708383322</v>
+        <v>85899046.268169791</v>
       </c>
       <c r="Q7" s="1">
         <f t="shared" si="7"/>
-        <v>159634546.57000017</v>
+        <v>138177069.53999996</v>
       </c>
       <c r="R7" s="1">
         <f t="shared" si="8"/>
-        <v>78308930.708383322</v>
-      </c>
-      <c r="S7" s="1"/>
+        <v>85899046.268169791</v>
+      </c>
+      <c r="S7" s="1">
+        <f t="shared" si="9"/>
+        <v>107950.83557812497</v>
+      </c>
       <c r="T7" s="1"/>
       <c r="U7" s="5"/>
       <c r="V7" s="5"/>
@@ -4506,7 +4497,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBA1661-1357-8E4D-8878-EEFCBAD9628D}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update cooper, wrong baseline npv
</commit_message>
<xml_diff>
--- a/use_cases/IES_Feb23/run/results.xlsx
+++ b/use_cases/IES_Feb23/run/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/IES_Feb23/run/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B255BB-2633-1C4D-A5D0-2B6CC1E7E06F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5F8997-FCBC-7B45-8DBF-8E278A27C18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5120" yWindow="7640" windowWidth="30720" windowHeight="17000" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
+    <workbookView xWindow="5120" yWindow="3700" windowWidth="30720" windowHeight="17000" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
@@ -337,7 +337,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -358,6 +358,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFF8F8F2"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -382,7 +388,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -399,6 +405,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -536,7 +543,7 @@
                     <c:v>10442175.071948605</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>6952.2878666099996</c:v>
+                    <c:v>29664094.113293801</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>1077.46392866</c:v>
@@ -560,7 +567,7 @@
                     <c:v>10442175.071948605</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>6952.2878666099996</c:v>
+                    <c:v>29664094.113293801</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>1077.46392866</c:v>
@@ -621,7 +628,7 @@
                   <c:v>1305897263.1300001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1678864838.25</c:v>
+                  <c:v>882854724.43999994</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>591488449.03000021</c:v>
@@ -709,7 +716,7 @@
         <c:axId val="2124379024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="2000000000"/>
+          <c:max val="1500000000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -3261,8 +3268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FE355D-8072-1247-9790-841EBA440D66}">
   <dimension ref="A1:AN16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="R24" sqref="R24"/>
+    <sheetView tabSelected="1" topLeftCell="C11" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3273,7 +3280,7 @@
     <col min="5" max="5" width="11.83203125" customWidth="1"/>
     <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
@@ -3501,15 +3508,15 @@
         <f t="shared" ref="G4:G7" si="1">F4/(24*D4)</f>
         <v>2.1993810786914232E-5</v>
       </c>
-      <c r="H4">
-        <v>262560457.34999999</v>
+      <c r="H4" s="12">
+        <v>1058570571.16</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>29664093.298599999</v>
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J7" si="2">I4/H4</f>
-        <v>0</v>
+        <v>2.8022782898728775E-2</v>
       </c>
       <c r="K4">
         <f>data!P3</f>
@@ -3525,27 +3532,27 @@
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N7" si="4">K4-H4</f>
-        <v>1678864838.25</v>
+        <v>882854724.43999994</v>
       </c>
       <c r="O4">
         <f t="shared" ref="O4:O7" si="5">100*SQRT(POWER(M4,2)+POWER(J4,2))</f>
-        <v>3.5810226035307667E-4</v>
+        <v>2.8022783127537649</v>
       </c>
       <c r="P4">
         <f t="shared" ref="P4:P7" si="6">SQRT(POWER(L4,2)+POWER(I4,2))</f>
-        <v>6952.2878666099996</v>
+        <v>29664094.113293801</v>
       </c>
       <c r="Q4" s="1">
         <f t="shared" ref="Q4:Q7" si="7">N4</f>
-        <v>1678864838.25</v>
+        <v>882854724.43999994</v>
       </c>
       <c r="R4" s="1">
         <f t="shared" ref="R4:R7" si="8">P4</f>
-        <v>6952.2878666099996</v>
+        <v>29664094.113293801</v>
       </c>
       <c r="S4" s="1">
         <f>Q4/B4</f>
-        <v>2183179.2434980492</v>
+        <v>1148055.5584395318</v>
       </c>
       <c r="T4" s="1"/>
       <c r="U4" s="5"/>

</xml_diff>

<commit_message>
error bar = 2x STD
</commit_message>
<xml_diff>
--- a/use_cases/IES_Feb23/run/results.xlsx
+++ b/use_cases/IES_Feb23/run/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/IES_Feb23/run/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5F8997-FCBC-7B45-8DBF-8E278A27C18A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECACCE0-5729-FF4E-AA78-6E04F4F6B1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5120" yWindow="3700" windowWidth="30720" windowHeight="17000" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="94">
   <si>
     <t>Location</t>
   </si>
@@ -58,12 +58,6 @@
     <t>Std opt NPV</t>
   </si>
   <si>
-    <t>Std baseline NPV frac</t>
-  </si>
-  <si>
-    <t>Std opt NPV frac</t>
-  </si>
-  <si>
     <t>Std delta NPV (%)</t>
   </si>
   <si>
@@ -79,9 +73,6 @@
     <t>Delta NPV (M$)</t>
   </si>
   <si>
-    <t>Std Delta NPV (M$)</t>
-  </si>
-  <si>
     <t>Std Delta NPV</t>
   </si>
   <si>
@@ -326,6 +317,9 @@
   </si>
   <si>
     <t>Standardized added value (M$/MWh)</t>
+  </si>
+  <si>
+    <t>2Std Delta NPV (M$)</t>
   </si>
 </sst>
 </file>
@@ -337,7 +331,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -358,12 +352,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFF8F8F2"/>
-      <name val="Menlo"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -405,7 +393,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -451,7 +439,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>cases!$Q$2</c:f>
+              <c:f>cases!$N$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -486,7 +474,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="75000"/>
@@ -535,48 +523,48 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>cases!$R$3:$R$8</c:f>
+                <c:f>cases!$O$3:$O$7</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="6"/>
+                  <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>10442175.071948605</c:v>
+                    <c:v>20884350.143897209</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>29664094.113293801</c:v>
+                    <c:v>59328188.226587601</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1077.46392866</c:v>
+                    <c:v>2154.9278573199999</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>555817.3250380737</c:v>
+                    <c:v>1111634.6500761474</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>85899046.268169791</c:v>
+                    <c:v>171798092.53633958</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>cases!$R$3:$R$8</c:f>
+                <c:f>cases!$O$3:$O$7</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="6"/>
+                  <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>10442175.071948605</c:v>
+                    <c:v>20884350.143897209</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>29664094.113293801</c:v>
+                    <c:v>59328188.226587601</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1077.46392866</c:v>
+                    <c:v>2154.9278573199999</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>555817.3250380737</c:v>
+                    <c:v>1111634.6500761474</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>85899046.268169791</c:v>
+                    <c:v>171798092.53633958</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -620,7 +608,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>cases!$Q$3:$Q$7</c:f>
+              <c:f>cases!$N$3:$N$7</c:f>
               <c:numCache>
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="5"/>
@@ -671,7 +659,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -690,7 +678,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -750,7 +738,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -784,7 +772,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -2313,16 +2301,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>977900</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3266,40 +3254,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FE355D-8072-1247-9790-841EBA440D66}">
-  <dimension ref="A1:AN16"/>
+  <dimension ref="A1:AK32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C11" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.5" customWidth="1"/>
-    <col min="5" max="5" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.1640625" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="11.1640625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.6640625" customWidth="1"/>
-    <col min="18" max="18" width="23.33203125" customWidth="1"/>
-    <col min="19" max="19" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="16" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.6640625" customWidth="1"/>
+    <col min="15" max="15" width="23.33203125" customWidth="1"/>
+    <col min="16" max="16" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B1" s="11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -3307,27 +3292,27 @@
       <c r="F1" s="11"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
       <c r="G2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H2" t="s">
         <v>1</v>
@@ -3336,35 +3321,29 @@
         <v>4</v>
       </c>
       <c r="J2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="K2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="N2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="O2" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
       <c r="P2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>12</v>
-      </c>
-      <c r="R2" t="s">
-        <v>13</v>
-      </c>
-      <c r="S2" t="s">
-        <v>95</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
       <c r="X2" s="3"/>
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
@@ -3379,11 +3358,8 @@
       <c r="AI2" s="3"/>
       <c r="AJ2" s="3"/>
       <c r="AK2" s="3"/>
-      <c r="AL2" s="3"/>
-      <c r="AM2" s="3"/>
-      <c r="AN2" s="3"/>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>UPPER(data!A2)</f>
         <v>BRAIDWOOD</v>
@@ -3419,48 +3395,39 @@
         <v>10442175</v>
       </c>
       <c r="J3">
-        <f>I3/H3</f>
-        <v>4.9665897586956935E-3</v>
-      </c>
-      <c r="K3">
         <f>data!P2</f>
         <v>3408381162.0100002</v>
       </c>
-      <c r="L3">
+      <c r="K3">
         <f>data!Q2</f>
         <v>1225.80578418</v>
       </c>
+      <c r="L3">
+        <f>J3-H3</f>
+        <v>1305897263.1300001</v>
+      </c>
       <c r="M3">
-        <f>L3/K3</f>
-        <v>3.5964457198710559E-7</v>
-      </c>
-      <c r="N3">
-        <f>K3-H3</f>
+        <f>SQRT(POWER(K3,2)+POWER(I3,2))</f>
+        <v>10442175.071948605</v>
+      </c>
+      <c r="N3" s="1">
+        <f>L3</f>
         <v>1305897263.1300001</v>
       </c>
-      <c r="O3">
-        <f>100*SQRT(POWER(M3,2)+POWER(J3,2))</f>
-        <v>0.49665897717171253</v>
-      </c>
-      <c r="P3">
-        <f>SQRT(POWER(L3,2)+POWER(I3,2))</f>
-        <v>10442175.071948605</v>
-      </c>
-      <c r="Q3" s="1">
-        <f>N3</f>
-        <v>1305897263.1300001</v>
-      </c>
-      <c r="R3" s="1">
-        <f>P3</f>
-        <v>10442175.071948605</v>
-      </c>
-      <c r="S3" s="1">
-        <f>Q3/B3</f>
+      <c r="O3" s="1">
+        <f>2*M3</f>
+        <v>20884350.143897209</v>
+      </c>
+      <c r="P3" s="1">
+        <f>N3/B3</f>
         <v>1094633.0789019279</v>
       </c>
-      <c r="T3" s="1"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="5"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
       <c r="X3" s="3"/>
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
@@ -3475,11 +3442,8 @@
       <c r="AI3" s="3"/>
       <c r="AJ3" s="3"/>
       <c r="AK3" s="3"/>
-      <c r="AL3" s="3"/>
-      <c r="AM3" s="3"/>
-      <c r="AN3" s="3"/>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
         <f>UPPER(data!A3)</f>
         <v>COOPER</v>
@@ -3508,55 +3472,46 @@
         <f t="shared" ref="G4:G7" si="1">F4/(24*D4)</f>
         <v>2.1993810786914232E-5</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4">
         <v>1058570571.16</v>
       </c>
       <c r="I4">
         <v>29664093.298599999</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J7" si="2">I4/H4</f>
-        <v>2.8022782898728775E-2</v>
-      </c>
-      <c r="K4">
         <f>data!P3</f>
         <v>1941425295.5999999</v>
       </c>
-      <c r="L4">
+      <c r="K4">
         <f>data!Q3</f>
         <v>6952.2878666099996</v>
       </c>
+      <c r="L4">
+        <f>J4-H4</f>
+        <v>882854724.43999994</v>
+      </c>
       <c r="M4">
-        <f t="shared" ref="M4:M7" si="3">L4/K4</f>
-        <v>3.5810226035307666E-6</v>
-      </c>
-      <c r="N4">
-        <f t="shared" ref="N4:N7" si="4">K4-H4</f>
+        <f t="shared" ref="M4:M7" si="2">SQRT(POWER(K4,2)+POWER(I4,2))</f>
+        <v>29664094.113293801</v>
+      </c>
+      <c r="N4" s="1">
+        <f>L4</f>
         <v>882854724.43999994</v>
       </c>
-      <c r="O4">
-        <f t="shared" ref="O4:O7" si="5">100*SQRT(POWER(M4,2)+POWER(J4,2))</f>
-        <v>2.8022783127537649</v>
-      </c>
-      <c r="P4">
-        <f t="shared" ref="P4:P7" si="6">SQRT(POWER(L4,2)+POWER(I4,2))</f>
-        <v>29664094.113293801</v>
-      </c>
-      <c r="Q4" s="1">
-        <f t="shared" ref="Q4:Q7" si="7">N4</f>
-        <v>882854724.43999994</v>
-      </c>
-      <c r="R4" s="1">
-        <f t="shared" ref="R4:R7" si="8">P4</f>
-        <v>29664094.113293801</v>
-      </c>
-      <c r="S4" s="1">
-        <f>Q4/B4</f>
+      <c r="O4" s="1">
+        <f t="shared" ref="O4:O7" si="3">2*M4</f>
+        <v>59328188.226587601</v>
+      </c>
+      <c r="P4" s="1">
+        <f>N4/B4</f>
         <v>1148055.5584395318</v>
       </c>
-      <c r="T4" s="1"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="5"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
@@ -3571,11 +3526,8 @@
       <c r="AI4" s="3"/>
       <c r="AJ4" s="3"/>
       <c r="AK4" s="3"/>
-      <c r="AL4" s="3"/>
-      <c r="AM4" s="3"/>
-      <c r="AN4" s="3"/>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A5" t="str">
         <f>UPPER(data!A4)</f>
         <v>DAVIS-BESSE</v>
@@ -3611,48 +3563,39 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="K5">
         <f>data!P4</f>
         <v>2357253019.6300001</v>
       </c>
-      <c r="L5">
+      <c r="K5">
         <f>data!Q4</f>
         <v>1077.46392866</v>
       </c>
+      <c r="L5">
+        <f>J5-H5</f>
+        <v>591488449.03000021</v>
+      </c>
       <c r="M5">
+        <f t="shared" si="2"/>
+        <v>1077.46392866</v>
+      </c>
+      <c r="N5" s="1">
+        <f>L5</f>
+        <v>591488449.03000021</v>
+      </c>
+      <c r="O5" s="1">
         <f t="shared" si="3"/>
-        <v>4.5708454700765267E-7</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="4"/>
-        <v>591488449.03000021</v>
-      </c>
-      <c r="O5">
-        <f t="shared" si="5"/>
-        <v>4.5708454700765264E-5</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="6"/>
-        <v>1077.46392866</v>
-      </c>
-      <c r="Q5" s="1">
-        <f t="shared" si="7"/>
-        <v>591488449.03000021</v>
-      </c>
-      <c r="R5" s="1">
-        <f t="shared" si="8"/>
-        <v>1077.46392866</v>
-      </c>
-      <c r="S5" s="1">
-        <f t="shared" ref="S5:S7" si="9">Q5/B5</f>
+        <v>2154.9278573199999</v>
+      </c>
+      <c r="P5" s="1">
+        <f>N5/B5</f>
         <v>661620.18907158857</v>
       </c>
-      <c r="T5" s="1"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="5"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
       <c r="X5" s="3"/>
       <c r="Y5" s="3"/>
       <c r="Z5" s="3"/>
@@ -3667,11 +3610,8 @@
       <c r="AI5" s="3"/>
       <c r="AJ5" s="3"/>
       <c r="AK5" s="3"/>
-      <c r="AL5" s="3"/>
-      <c r="AM5" s="3"/>
-      <c r="AN5" s="3"/>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>UPPER(data!A5)</f>
         <v>PRAIRIE-ISLAND</v>
@@ -3707,48 +3647,39 @@
         <v>553965.52426600002</v>
       </c>
       <c r="J6">
-        <f t="shared" si="2"/>
-        <v>2.1111441206267249E-3</v>
-      </c>
-      <c r="K6">
         <f>data!P5</f>
         <v>1177078719.72</v>
       </c>
-      <c r="L6">
+      <c r="K6">
         <f>data!Q5</f>
         <v>45333.174797</v>
       </c>
+      <c r="L6">
+        <f>J6-H6</f>
+        <v>914678100.61800003</v>
+      </c>
       <c r="M6">
+        <f t="shared" si="2"/>
+        <v>555817.3250380737</v>
+      </c>
+      <c r="N6" s="1">
+        <f>L6</f>
+        <v>914678100.61800003</v>
+      </c>
+      <c r="O6" s="1">
         <f t="shared" si="3"/>
-        <v>3.8513290604543185E-5</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="4"/>
-        <v>914678100.61800003</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="5"/>
-        <v>0.21114953875417244</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="6"/>
-        <v>555817.3250380737</v>
-      </c>
-      <c r="Q6" s="1">
-        <f t="shared" si="7"/>
-        <v>914678100.61800003</v>
-      </c>
-      <c r="R6" s="1">
-        <f t="shared" si="8"/>
-        <v>555817.3250380737</v>
-      </c>
-      <c r="S6" s="1">
-        <f t="shared" si="9"/>
+        <v>1111634.6500761474</v>
+      </c>
+      <c r="P6" s="1">
+        <f>N6/B6</f>
         <v>1752256.8977356323</v>
       </c>
-      <c r="T6" s="1"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="5"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
       <c r="X6" s="3"/>
       <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
@@ -3763,11 +3694,8 @@
       <c r="AI6" s="3"/>
       <c r="AJ6" s="3"/>
       <c r="AK6" s="3"/>
-      <c r="AL6" s="3"/>
-      <c r="AM6" s="3"/>
-      <c r="AN6" s="3"/>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
         <f>UPPER(data!A6)</f>
         <v>STP</v>
@@ -3803,48 +3731,39 @@
         <v>83894741.873400003</v>
       </c>
       <c r="J7">
-        <f t="shared" si="2"/>
-        <v>3.0590777200160638E-2</v>
-      </c>
-      <c r="K7">
         <f>data!P6</f>
         <v>2880661882.02</v>
       </c>
-      <c r="L7">
+      <c r="K7">
         <f>data!Q6</f>
         <v>18447721.6961</v>
       </c>
+      <c r="L7">
+        <f>J7-H7</f>
+        <v>138177069.53999996</v>
+      </c>
       <c r="M7">
+        <f t="shared" si="2"/>
+        <v>85899046.268169791</v>
+      </c>
+      <c r="N7" s="1">
+        <f>L7</f>
+        <v>138177069.53999996</v>
+      </c>
+      <c r="O7" s="1">
         <f t="shared" si="3"/>
-        <v>6.403987156994609E-3</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="4"/>
-        <v>138177069.53999996</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="5"/>
-        <v>3.1253906975237826</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="6"/>
-        <v>85899046.268169791</v>
-      </c>
-      <c r="Q7" s="1">
-        <f t="shared" si="7"/>
-        <v>138177069.53999996</v>
-      </c>
-      <c r="R7" s="1">
-        <f t="shared" si="8"/>
-        <v>85899046.268169791</v>
-      </c>
-      <c r="S7" s="1">
-        <f t="shared" si="9"/>
+        <v>171798092.53633958</v>
+      </c>
+      <c r="P7" s="1">
+        <f>N7/B7</f>
         <v>107950.83557812497</v>
       </c>
-      <c r="T7" s="1"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="5"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
       <c r="X7" s="3"/>
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
@@ -3859,70 +3778,138 @@
       <c r="AI7" s="3"/>
       <c r="AJ7" s="3"/>
       <c r="AK7" s="3"/>
-      <c r="AL7" s="3"/>
-      <c r="AM7" s="3"/>
-      <c r="AN7" s="3"/>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="4"/>
+      <c r="R8" s="4"/>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B12">
         <v>39.799999999999997</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B14">
         <v>2.5125628140703519E-2</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B15">
         <v>25.125628140703519</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B16">
         <f>B15/1000</f>
         <v>2.5125628140703519E-2</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
-      </c>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="12"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="12"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="10"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="12"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="10"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="12"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="10"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J25" s="8"/>
+      <c r="K25" s="10"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="10"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C30" s="8"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="10"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C31" s="8"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="10"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3937,107 +3924,107 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E35F0C96-D3AA-4F4B-9456-DE375A306C8A}">
   <dimension ref="A1:AD6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:Q2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>51</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>52</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>53</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>54</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>55</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>56</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>57</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>58</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>59</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>60</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>61</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>62</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>63</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>64</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>65</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>66</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>67</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>68</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>69</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>70</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>71</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>72</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -4070,16 +4057,16 @@
         <v>10</v>
       </c>
       <c r="L2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="N2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P2">
         <v>3408381162.0100002</v>
@@ -4129,7 +4116,7 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4162,16 +4149,16 @@
         <v>10</v>
       </c>
       <c r="L3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" t="s">
         <v>74</v>
       </c>
-      <c r="M3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" t="s">
-        <v>77</v>
-      </c>
       <c r="O3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P3">
         <v>1941425295.5999999</v>
@@ -4221,7 +4208,7 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -4254,16 +4241,16 @@
         <v>10</v>
       </c>
       <c r="L4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="N4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="O4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P4">
         <v>2357253019.6300001</v>
@@ -4313,7 +4300,7 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4346,16 +4333,16 @@
         <v>35000</v>
       </c>
       <c r="L5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="N5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="O5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P5">
         <v>1177078719.72</v>
@@ -4405,7 +4392,7 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -4438,16 +4425,16 @@
         <v>2000000</v>
       </c>
       <c r="L6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M6" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="N6" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="O6" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P6">
         <v>2880661882.02</v>
@@ -4518,30 +4505,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>2102483898.8800001</v>
@@ -4568,7 +4555,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>3408381162.0100002</v>
@@ -4595,7 +4582,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B4">
         <v>3074633986.1399999</v>
@@ -4622,7 +4609,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B5">
         <v>3742127992.46</v>
@@ -4649,7 +4636,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B6" s="3">
         <v>3638289546</v>
@@ -4676,7 +4663,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B7" s="3">
         <v>3178472614</v>
@@ -4703,7 +4690,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B8">
         <v>2997736770.0300002</v>
@@ -4730,7 +4717,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B9" s="3">
         <v>2587091316</v>
@@ -4757,7 +4744,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B10">
         <v>3591087201</v>
@@ -4784,7 +4771,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B11">
         <v>3225673919.4099998</v>
@@ -4814,21 +4801,21 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
         <v>26</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B14">
         <f>E4</f>
@@ -4849,7 +4836,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B15">
         <f>E6</f>
@@ -4870,7 +4857,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B16">
         <f>E8</f>
@@ -4891,7 +4878,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B17">
         <f>E10</f>

</xml_diff>

<commit_message>
Add results h2 ptc sa for braidwood
</commit_message>
<xml_diff>
--- a/use_cases/IES_Feb23/run/results.xlsx
+++ b/use_cases/IES_Feb23/run/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/FORCE/use_cases/IES_Feb23/run/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ECACCE0-5729-FF4E-AA78-6E04F4F6B1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70831F6D-C55C-9B4F-A390-63D177012F68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5120" yWindow="3700" windowWidth="30720" windowHeight="17000" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
+    <workbookView xWindow="2480" yWindow="1000" windowWidth="33360" windowHeight="19680" activeTab="2" xr2:uid="{0E0AD5E1-F50E-5F4E-9139-BDA2035603EC}"/>
   </bookViews>
   <sheets>
     <sheet name="cases" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
   <si>
     <t>Location</t>
   </si>
@@ -320,6 +320,15 @@
   </si>
   <si>
     <t>2Std Delta NPV (M$)</t>
+  </si>
+  <si>
+    <t>ptc100</t>
+  </si>
+  <si>
+    <t>ptc270</t>
+  </si>
+  <si>
+    <t>H2 PTC</t>
   </si>
 </sst>
 </file>
@@ -376,7 +385,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
@@ -393,7 +402,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -891,9 +899,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>braidwood_SA!$A$14:$A$17</c:f>
+              <c:f>braidwood_SA!$A$16:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Synfuel Price</c:v>
                 </c:pt>
@@ -906,15 +914,18 @@
                 <c:pt idx="3">
                   <c:v>O&amp;M</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>H2 PTC</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>braidwood_SA!$B$14:$B$17</c:f>
+              <c:f>braidwood_SA!$B$16:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>972150087.25999975</c:v>
                 </c:pt>
@@ -926,6 +937,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1488603302.1199999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1849336819.7800002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -941,7 +955,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>braidwood_SA!$C$13</c:f>
+              <c:f>braidwood_SA!$C$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -962,9 +976,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>braidwood_SA!$A$14:$A$17</c:f>
+              <c:f>braidwood_SA!$A$16:$A$20</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>Synfuel Price</c:v>
                 </c:pt>
@@ -977,15 +991,18 @@
                 <c:pt idx="3">
                   <c:v>O&amp;M</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>H2 PTC</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>braidwood_SA!$C$14:$C$17</c:f>
+              <c:f>braidwood_SA!$C$16:$C$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>1639644093.5799999</c:v>
                 </c:pt>
@@ -997,6 +1014,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1123190020.5299997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-946118919.88000011</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1125,7 +1145,7 @@
         <c:crossBetween val="between"/>
         <c:majorUnit val="200000000"/>
         <c:dispUnits>
-          <c:builtInUnit val="millions"/>
+          <c:builtInUnit val="billions"/>
           <c:dispUnitsLbl>
             <c:spPr>
               <a:noFill/>
@@ -2343,15 +2363,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2421,12 +2441,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.02785</cdr:x>
-      <cdr:y>0.64512</cdr:y>
+      <cdr:x>0.02887</cdr:x>
+      <cdr:y>0.54571</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.11204</cdr:x>
-      <cdr:y>0.71928</cdr:y>
+      <cdr:x>0.11306</cdr:x>
+      <cdr:y>0.61987</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -2441,8 +2461,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="344853" y="3461564"/>
-          <a:ext cx="1042482" cy="397924"/>
+          <a:off x="358967" y="2928153"/>
+          <a:ext cx="1046760" cy="397924"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2493,11 +2513,11 @@
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
       <cdr:x>0</cdr:x>
-      <cdr:y>0.44497</cdr:y>
+      <cdr:y>0.38343</cdr:y>
     </cdr:from>
     <cdr:to>
       <cdr:x>0.11487</cdr:x>
-      <cdr:y>0.52426</cdr:y>
+      <cdr:y>0.46272</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -2512,8 +2532,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="0" y="2387624"/>
-          <a:ext cx="1422378" cy="425450"/>
+          <a:off x="0" y="2057398"/>
+          <a:ext cx="1428213" cy="425450"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2627,12 +2647,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.02769</cdr:x>
-      <cdr:y>0.24616</cdr:y>
+      <cdr:x>0.02871</cdr:x>
+      <cdr:y>0.22012</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.11188</cdr:x>
-      <cdr:y>0.32032</cdr:y>
+      <cdr:x>0.1129</cdr:x>
+      <cdr:y>0.29428</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -2647,8 +2667,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="342925" y="1320817"/>
-          <a:ext cx="1042483" cy="397924"/>
+          <a:off x="356978" y="1181133"/>
+          <a:ext cx="1046760" cy="397924"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2821,12 +2841,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.02051</cdr:x>
-      <cdr:y>0.84537</cdr:y>
+      <cdr:x>0.01532</cdr:x>
+      <cdr:y>0.8643</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.1047</cdr:x>
-      <cdr:y>0.91953</cdr:y>
+      <cdr:x>0.12002</cdr:x>
+      <cdr:y>0.93846</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -2841,8 +2861,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="254000" y="4536026"/>
-          <a:ext cx="1042482" cy="397924"/>
+          <a:off x="190500" y="4637644"/>
+          <a:ext cx="1301767" cy="397924"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2927,7 +2947,7 @@
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>30</a:t>
+            <a:t>1.0</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200"/>
@@ -2939,7 +2959,7 @@
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>60</a:t>
+            <a:t>2.7</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200"/>
@@ -2947,7 +2967,142 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1200" baseline="0"/>
-            <a:t> $/ton</a:t>
+            <a:t> $/kg-H2</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1200"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.03575</cdr:x>
+      <cdr:y>0.70059</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.11994</cdr:x>
+      <cdr:y>0.77475</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="8" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDC46EDB-3304-493A-113E-4B832002B71E}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="444500" y="3759200"/>
+          <a:ext cx="1046760" cy="397924"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:pPr algn="r"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>[</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" b="1">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>x0.75</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>,</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>x1.25</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200"/>
+            <a:t>]</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" baseline="0"/>
+            <a:t> </a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1200"/>
         </a:p>
@@ -3256,7 +3411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00FE355D-8072-1247-9790-841EBA440D66}">
   <dimension ref="A1:AK32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
@@ -3840,18 +3995,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="12"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="12"/>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
@@ -3860,8 +4004,7 @@
       <c r="J22" s="8"/>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
@@ -3870,8 +4013,7 @@
       <c r="J23" s="8"/>
       <c r="K23" s="10"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="12"/>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="10"/>
@@ -3880,33 +4022,26 @@
       <c r="J24" s="8"/>
       <c r="K24" s="10"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:11" x14ac:dyDescent="0.2">
       <c r="J25" s="8"/>
       <c r="K25" s="10"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
       <c r="E29" s="10"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
       <c r="E30" s="10"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
       <c r="E31" s="10"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:11" x14ac:dyDescent="0.2">
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="10"/>
@@ -4489,16 +4624,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADBA1661-1357-8E4D-8878-EEFCBAD9628D}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -4564,7 +4700,7 @@
         <v>1225.80578418</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D11" si="0">C3/B3</f>
+        <f t="shared" ref="D3:D13" si="0">C3/B3</f>
         <v>3.5964457198710559E-7</v>
       </c>
       <c r="E3">
@@ -4572,7 +4708,7 @@
         <v>1305897263.1300001</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F11" si="1">SQRT(POWER($C$2,2)+POWER(C3,2))</f>
+        <f t="shared" ref="F3:F13" si="1">SQRT(POWER($C$2,2)+POWER(C3,2))</f>
         <v>10442175.553348601</v>
       </c>
       <c r="G3" s="2">
@@ -4595,7 +4731,7 @@
         <v>1.6665051963218262E-7</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E11" si="2">B4-$B$2</f>
+        <f t="shared" ref="E4:E13" si="2">B4-$B$2</f>
         <v>972150087.25999975</v>
       </c>
       <c r="F4">
@@ -4603,7 +4739,7 @@
         <v>10442175.493971271</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G11" si="3">F4/E4</f>
+        <f t="shared" ref="G4:G13" si="3">F4/E4</f>
         <v>1.0741320327813261E-2</v>
       </c>
     </row>
@@ -4796,105 +4932,180 @@
         <v>9.2968913238234141E-3</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12">
+        <v>253147079.09999999</v>
+      </c>
+      <c r="C12">
+        <v>7678473.3109999998</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" si="0"/>
+        <v>3.0332063629961117E-2</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>-1849336819.7800002</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>12961403.518604403</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="3"/>
+        <v>-7.00867650498967E-3</v>
+      </c>
+    </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14">
-        <f>E4</f>
-        <v>972150087.25999975</v>
-      </c>
-      <c r="C14">
-        <f>E5</f>
-        <v>1639644093.5799999</v>
-      </c>
-      <c r="D14">
-        <f>F4</f>
-        <v>10442175.493971271</v>
-      </c>
-      <c r="E14">
-        <f>F5</f>
-        <v>10442175.486546619</v>
+        <v>95</v>
+      </c>
+      <c r="B13">
+        <v>1156364979</v>
+      </c>
+      <c r="C13">
+        <v>11451206.1</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="0"/>
+        <v>9.902761072808311E-3</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>-946118919.88000011</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>15497391.713737784</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="3"/>
+        <v>-1.6379961744875979E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15">
-        <f>E6</f>
-        <v>1535805647.1199999</v>
-      </c>
-      <c r="C15">
-        <f>E7</f>
-        <v>1075988715.1199999</v>
-      </c>
-      <c r="D15">
-        <f>F6</f>
-        <v>10442175.588435065</v>
-      </c>
-      <c r="E15">
-        <f>F7</f>
-        <v>10442175.505360482</v>
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16">
-        <f>E8</f>
-        <v>895252871.1500001</v>
+        <f>E4</f>
+        <v>972150087.25999975</v>
       </c>
       <c r="C16">
-        <f>E9</f>
-        <v>484607417.11999989</v>
+        <f>E5</f>
+        <v>1639644093.5799999</v>
       </c>
       <c r="D16">
-        <f>F8</f>
-        <v>10442175.502742153</v>
+        <f>F4</f>
+        <v>10442175.493971271</v>
       </c>
       <c r="E16">
-        <f>F9</f>
-        <v>10442175.576238554</v>
+        <f>F5</f>
+        <v>10442175.486546619</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <f>E6</f>
+        <v>1535805647.1199999</v>
+      </c>
+      <c r="C17">
+        <f>E7</f>
+        <v>1075988715.1199999</v>
+      </c>
+      <c r="D17">
+        <f>F6</f>
+        <v>10442175.588435065</v>
+      </c>
+      <c r="E17">
+        <f>F7</f>
+        <v>10442175.505360482</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18">
+        <f>E8</f>
+        <v>895252871.1500001</v>
+      </c>
+      <c r="C18">
+        <f>E9</f>
+        <v>484607417.11999989</v>
+      </c>
+      <c r="D18">
+        <f>F8</f>
+        <v>10442175.502742153</v>
+      </c>
+      <c r="E18">
+        <f>F9</f>
+        <v>10442175.576238554</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>91</v>
       </c>
-      <c r="B17">
+      <c r="B19">
         <f>E10</f>
         <v>1488603302.1199999</v>
       </c>
-      <c r="C17">
+      <c r="C19">
         <f>E11</f>
         <v>1123190020.5299997</v>
       </c>
-      <c r="D17">
+      <c r="D19">
         <f>F10</f>
         <v>10442175.49225767</v>
       </c>
-      <c r="E17">
+      <c r="E19">
         <f>F11</f>
         <v>10442175.556870397</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20">
+        <f>E12</f>
+        <v>-1849336819.7800002</v>
+      </c>
+      <c r="C20">
+        <f>E13</f>
+        <v>-946118919.88000011</v>
+      </c>
+      <c r="D20">
+        <f>F12</f>
+        <v>12961403.518604403</v>
+      </c>
+      <c r="E20">
+        <f>F13</f>
+        <v>15497391.713737784</v>
       </c>
     </row>
   </sheetData>

</xml_diff>